<commit_message>
Updated with Engineering Committee's recommended FPs. New question: AA from GenBank -> DNA seq to order?
</commit_message>
<xml_diff>
--- a/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
+++ b/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Fluorescent Reporter Proteins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6F8D9E-9292-2C46-9FF9-17FEB5ACFB2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570B4EA2-BB64-2447-B85F-59ADE136FA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48520" yWindow="4540" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39200" yWindow="1700" windowWidth="39640" windowHeight="20780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Parts" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7605" uniqueCount="7542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7663" uniqueCount="7568">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22701,34 +22701,112 @@
     <t>IP-Free TannenRFP</t>
   </si>
   <si>
-    <t>Excitation 550nm, Emission 565nm</t>
-  </si>
-  <si>
-    <t>Excitation 515nm, Emission 534nm</t>
-  </si>
-  <si>
-    <t>Excitation 508nm, Emission 521nm</t>
-  </si>
-  <si>
-    <t>Excitation 398nm, Emission 498nm</t>
-  </si>
-  <si>
-    <t>Excitation 584nm, Emission 607nm</t>
-  </si>
-  <si>
-    <t>Excitation 501nm, Emission 511nm</t>
-  </si>
-  <si>
-    <t>Excitation 514nm, Emission 527nm</t>
-  </si>
-  <si>
-    <t>Excitation 439nm, Emission 476nm</t>
-  </si>
-  <si>
-    <t>Fluorescent Proteins in vector (BioBrick)</t>
-  </si>
-  <si>
-    <t>E0040, E1010, E0030, E0020, J97000, J97001, J97002, J97003</t>
+    <t>K864100</t>
+  </si>
+  <si>
+    <t>Excit. 501 / Emiss. 511</t>
+  </si>
+  <si>
+    <t>Excit. 584 / Emiss. 607</t>
+  </si>
+  <si>
+    <t>Excit. 514 / Emiss. 527</t>
+  </si>
+  <si>
+    <t>Excit. 439 / Emiss. 476</t>
+  </si>
+  <si>
+    <t>Excit. 398 / Emiss. 498</t>
+  </si>
+  <si>
+    <t>Excit. 508 / Emiss. 521</t>
+  </si>
+  <si>
+    <t>Excit. 515 / Emiss. 534</t>
+  </si>
+  <si>
+    <t>Excit. 550 / Emiss. 565</t>
+  </si>
+  <si>
+    <t>sYFP2</t>
+  </si>
+  <si>
+    <t>GFPmut3b*</t>
+  </si>
+  <si>
+    <t>AAB18957.1</t>
+  </si>
+  <si>
+    <t>mCherry</t>
+  </si>
+  <si>
+    <t>J06504</t>
+  </si>
+  <si>
+    <t>mKate2</t>
+  </si>
+  <si>
+    <t>mRFP1*</t>
+  </si>
+  <si>
+    <t>CAH64892</t>
+  </si>
+  <si>
+    <t>mScarlet</t>
+  </si>
+  <si>
+    <t>K592100</t>
+  </si>
+  <si>
+    <t>TagBFP</t>
+  </si>
+  <si>
+    <t>mCerulean3</t>
+  </si>
+  <si>
+    <t>Excit. 515 / Emiss. 527, brightness 68, maturation time 4.1 min (from FPBase)</t>
+  </si>
+  <si>
+    <t>Excit. 587 / Emiss. 610, brightness 16, maturation time 15 min, pKa 4.5 (from FPBase)</t>
+  </si>
+  <si>
+    <t>Excit. 500 / Emiss. 513, brightness 35, maturation time 4.1 min, weak dimer (from FPBase)</t>
+  </si>
+  <si>
+    <t>Excit. 588 / Emiss. 633, brightness 25, maturation time 20 min, pKa 5.4 (from FPBase)</t>
+  </si>
+  <si>
+    <t>Excit. 584 / Emiss. 607, brightness 12.5, maturation time 60 min, pKa 4.5 (from FPBase)</t>
+  </si>
+  <si>
+    <t>Excit. 569 / Emiss. 594, brightness 70, maturation time 174 min, pKa 5.3 (from FPBase)</t>
+  </si>
+  <si>
+    <t>Excit. 402 / Emiss. 457, brightness 33, maturation time 13 min, pKa 2.7 (from FPBase)</t>
+  </si>
+  <si>
+    <t>Excit. 433 / Emiss. 475, brightness 35, maturation time 70 min, pKa 3.2 (from FPBase)</t>
+  </si>
+  <si>
+    <t>S2R mutation</t>
+  </si>
+  <si>
+    <t>Includes barcode after double stop</t>
+  </si>
+  <si>
+    <t>ATP07149.1</t>
+  </si>
+  <si>
+    <t>AEX25288.1</t>
+  </si>
+  <si>
+    <t>APD76535.1</t>
+  </si>
+  <si>
+    <t>E0040, E1010, E0030, E0020, J97000, J97001, J97002, J97003, K592100, J06504, K864100</t>
+  </si>
+  <si>
+    <t>Fluorescent Proteins in vector</t>
   </si>
 </sst>
 </file>
@@ -23573,8 +23651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15:G22"/>
+    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23583,7 +23661,7 @@
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="42.28515625" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
@@ -23895,15 +23973,17 @@
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
       <c r="A15" s="18" t="s">
-        <v>7520</v>
+        <v>7542</v>
       </c>
       <c r="B15" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="C15" s="18" t="s">
+        <v>7561</v>
+      </c>
       <c r="D15" s="18"/>
       <c r="E15" s="18" t="s">
-        <v>7537</v>
+        <v>7533</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>43</v>
@@ -23930,24 +24010,26 @@
       <c r="M15" s="19"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A16" s="21" t="s">
-        <v>7521</v>
-      </c>
-      <c r="B16" s="41" t="s">
+      <c r="A16" s="18" t="s">
+        <v>7520</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="21"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="18" t="s">
-        <v>7536</v>
+        <v>7555</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>43</v>
+        <v>7470</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>7519</v>
-      </c>
-      <c r="H16" s="18"/>
+        <v>7543</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>10</v>
+      </c>
       <c r="I16" s="18" t="s">
         <v>7420</v>
       </c>
@@ -23965,13 +24047,13 @@
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
       <c r="A17" s="18" t="s">
-        <v>7522</v>
+        <v>7529</v>
       </c>
       <c r="B17" s="41" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="18" t="s">
         <v>7538</v>
       </c>
@@ -23979,10 +24061,10 @@
         <v>43</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>7517</v>
+        <v>7525</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>10</v>
+        <v>7418</v>
       </c>
       <c r="I17" s="18" t="s">
         <v>7420</v>
@@ -24001,21 +24083,21 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
       <c r="A18" s="18" t="s">
-        <v>7523</v>
+        <v>7522</v>
       </c>
       <c r="B18" s="41" t="s">
         <v>48</v>
       </c>
       <c r="C18" s="18"/>
-      <c r="D18" s="20"/>
+      <c r="D18" s="18"/>
       <c r="E18" s="18" t="s">
-        <v>7539</v>
+        <v>7535</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>43</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>7518</v>
+        <v>7517</v>
       </c>
       <c r="H18" s="18" t="s">
         <v>10</v>
@@ -24037,23 +24119,25 @@
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
       <c r="A19" s="18" t="s">
-        <v>7528</v>
-      </c>
-      <c r="B19" s="41" t="s">
+        <v>7541</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="20"/>
       <c r="E19" s="18" t="s">
-        <v>7535</v>
+        <v>7553</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="18" t="s">
-        <v>7524</v>
-      </c>
-      <c r="H19" s="18"/>
+      <c r="G19" s="20" t="s">
+        <v>7532</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>10</v>
+      </c>
       <c r="I19" s="18" t="s">
         <v>7420</v>
       </c>
@@ -24071,7 +24155,7 @@
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
       <c r="A20" s="18" t="s">
-        <v>7529</v>
+        <v>7530</v>
       </c>
       <c r="B20" s="41" t="s">
         <v>48</v>
@@ -24079,15 +24163,17 @@
       <c r="C20" s="18"/>
       <c r="D20" s="20"/>
       <c r="E20" s="18" t="s">
-        <v>7534</v>
+        <v>7539</v>
       </c>
       <c r="F20" s="18" t="s">
         <v>43</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>7525</v>
-      </c>
-      <c r="H20" s="18"/>
+        <v>7526</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>7418</v>
+      </c>
       <c r="I20" s="18" t="s">
         <v>7420</v>
       </c>
@@ -24104,22 +24190,24 @@
       <c r="M20" s="21"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A21" s="18" t="s">
-        <v>7530</v>
+      <c r="A21" s="21" t="s">
+        <v>7547</v>
       </c>
       <c r="B21" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="20"/>
+      <c r="C21" s="21" t="s">
+        <v>7562</v>
+      </c>
+      <c r="D21" s="18"/>
       <c r="E21" s="18" t="s">
-        <v>7533</v>
+        <v>7534</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>43</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>7526</v>
+        <v>7519</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="18" t="s">
@@ -24138,22 +24226,22 @@
       <c r="M21" s="18"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A22" s="18" t="s">
-        <v>7531</v>
-      </c>
-      <c r="B22" s="41" t="s">
+      <c r="A22" s="41" t="s">
+        <v>7521</v>
+      </c>
+      <c r="B22" s="18" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="D22" s="20"/>
       <c r="E22" s="18" t="s">
-        <v>7532</v>
+        <v>7557</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>43</v>
+        <v>7470</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>7527</v>
+        <v>7548</v>
       </c>
       <c r="H22" s="18"/>
       <c r="I22" s="18" t="s">
@@ -24172,30 +24260,34 @@
       <c r="M22" s="18"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A23" s="18" t="s">
-        <v>7502</v>
+      <c r="A23" s="41" t="s">
+        <v>7549</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="18" t="s">
+        <v>7558</v>
+      </c>
       <c r="F23" s="18" t="s">
-        <v>43</v>
+        <v>7470</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>7502</v>
-      </c>
-      <c r="H23" s="18"/>
+        <v>7565</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>7418</v>
+      </c>
       <c r="I23" s="18" t="s">
         <v>7420</v>
       </c>
       <c r="J23" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" s="18" t="b">
         <v>0</v>
-      </c>
-      <c r="K23" s="18" t="b">
-        <v>1</v>
       </c>
       <c r="L23" s="15">
         <f t="shared" si="0"/>
@@ -24204,17 +24296,29 @@
       <c r="M23" s="18"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
+      <c r="A24" s="18" t="s">
+        <v>7544</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>48</v>
+      </c>
       <c r="C24" s="18"/>
       <c r="D24" s="20"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="20"/>
+      <c r="E24" s="18" t="s">
+        <v>7554</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>7545</v>
+      </c>
       <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
+      <c r="I24" t="s">
+        <v>7420</v>
+      </c>
       <c r="J24" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="18" t="b">
         <v>0</v>
@@ -24226,17 +24330,29 @@
       <c r="M24" s="18"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
+      <c r="A25" s="18" t="s">
+        <v>7546</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>48</v>
+      </c>
       <c r="C25" s="18"/>
       <c r="D25" s="20"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="20"/>
+      <c r="E25" s="18" t="s">
+        <v>7556</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>7470</v>
+      </c>
+      <c r="G25" t="s">
+        <v>7564</v>
+      </c>
       <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
+      <c r="I25" s="18" t="s">
+        <v>7420</v>
+      </c>
       <c r="J25" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" s="18" t="b">
         <v>0</v>
@@ -24248,17 +24364,31 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
+      <c r="A26" s="18" t="s">
+        <v>7531</v>
+      </c>
+      <c r="B26" s="41" t="s">
+        <v>48</v>
+      </c>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
+      <c r="E26" s="18" t="s">
+        <v>7540</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>7527</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>7418</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>7420</v>
+      </c>
       <c r="J26" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="18" t="b">
         <v>0</v>
@@ -24270,17 +24400,31 @@
       <c r="M26" s="18"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
+      <c r="A27" s="18" t="s">
+        <v>7523</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>48</v>
+      </c>
       <c r="C27" s="18"/>
       <c r="D27" s="20"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
+      <c r="E27" s="18" t="s">
+        <v>7536</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>7518</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>7420</v>
+      </c>
       <c r="J27" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="18" t="b">
         <v>0</v>
@@ -24292,17 +24436,29 @@
       <c r="M27" s="18"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="41"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
+      <c r="A28" s="41" t="s">
+        <v>7551</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="21"/>
       <c r="D28" s="20"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="E28" s="18" t="s">
+        <v>7559</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>7550</v>
+      </c>
       <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
+      <c r="I28" s="18" t="s">
+        <v>7420</v>
+      </c>
       <c r="J28" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" s="18" t="b">
         <v>0</v>
@@ -24314,17 +24470,31 @@
       <c r="M28" s="18"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A29" s="41"/>
-      <c r="B29" s="18"/>
+      <c r="A29" s="41" t="s">
+        <v>7552</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>48</v>
+      </c>
       <c r="C29" s="18"/>
       <c r="D29" s="20"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
+      <c r="E29" s="18" t="s">
+        <v>7560</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>7470</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>7563</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>7420</v>
+      </c>
       <c r="J29" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" s="18" t="b">
         <v>0</v>
@@ -24336,17 +24506,31 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A30" s="41"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="21"/>
+      <c r="A30" s="18" t="s">
+        <v>7528</v>
+      </c>
+      <c r="B30" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="18"/>
       <c r="D30" s="20"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
+      <c r="E30" s="18" t="s">
+        <v>7537</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>7524</v>
+      </c>
+      <c r="H30" t="s">
+        <v>7418</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>7420</v>
+      </c>
       <c r="J30" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" s="18" t="b">
         <v>0</v>
@@ -24358,20 +24542,30 @@
       <c r="M30" s="23"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A31" s="41"/>
-      <c r="B31" s="18"/>
+      <c r="A31" s="18" t="s">
+        <v>7502</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>54</v>
+      </c>
       <c r="C31" s="18"/>
       <c r="D31" s="20"/>
       <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="20"/>
+      <c r="F31" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>7502</v>
+      </c>
       <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
+      <c r="I31" s="18" t="s">
+        <v>7420</v>
+      </c>
       <c r="J31" s="18" t="b">
         <v>0</v>
       </c>
       <c r="K31" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L31" s="15">
         <f t="shared" si="0"/>
@@ -24380,15 +24574,6 @@
       <c r="M31" s="23"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A32" s="41"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
       <c r="J32" s="18" t="b">
         <v>0</v>
       </c>
@@ -24402,13 +24587,6 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A33" s="41"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="20"/>
       <c r="H33" s="18"/>
       <c r="I33" s="18"/>
       <c r="J33" s="18" t="b">
@@ -24424,14 +24602,6 @@
       <c r="M33" s="24"/>
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A34" s="41"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="18"/>
       <c r="I34" s="18"/>
       <c r="J34" s="18" t="b">
         <v>0</v>
@@ -24446,14 +24616,6 @@
       <c r="M34" s="21"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A35" s="41"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="18"/>
       <c r="I35" s="18"/>
       <c r="J35" s="18" t="b">
         <v>0</v>
@@ -24468,13 +24630,13 @@
       <c r="M35" s="21"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A36" s="41"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
       <c r="D36" s="20"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
-      <c r="G36" s="20"/>
+      <c r="G36" s="18"/>
       <c r="H36" s="18"/>
       <c r="I36" s="18"/>
       <c r="J36" s="18" t="b">
@@ -25490,35 +25652,35 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
+          <x14:formula1>
+            <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>J15:K38</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>data_source!$B$2:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F15:F38</xm:sqref>
+          <xm:sqref>F15:F31 F36:F38</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'Organism Terms'!$A$2:$A$34</xm:f>
           </x14:formula1>
-          <xm:sqref>H15:I38</xm:sqref>
+          <xm:sqref>I34:I35 I21:I23 H22:I22 H31:I31 H27:I27 I25:I30 H33:I33 H36:I38 H15:I20 H21 H23:H29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>'Ontology Terms'!$B$2:$B$2518</xm:f>
           </x14:formula1>
-          <xm:sqref>B15:B38</xm:sqref>
+          <xm:sqref>B15:B31 B36:B38</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>Sequence_alteration_terms!$A$2:$A$19</xm:f>
           </x14:formula1>
-          <xm:sqref>D15:D38</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
-          <x14:formula1>
-            <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>J15:K38</xm:sqref>
+          <xm:sqref>D15:D31 D36:D38</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -25530,8 +25692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -26025,7 +26187,7 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" s="21" t="s">
-        <v>7540</v>
+        <v>7567</v>
       </c>
       <c r="B14" s="21"/>
       <c r="D14" s="21" t="b">
@@ -26036,7 +26198,7 @@
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="21" t="s">
-        <v>7541</v>
+        <v>7566</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="32"/>

</xml_diff>

<commit_message>
Found DNA sequences for non-iGEM FPs and modified as necessary. Corrected target organisms for those as well. Also testing how sequence files should be stored.
</commit_message>
<xml_diff>
--- a/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
+++ b/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/Fluorescent Reporter Proteins/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Fluorescent Reporter Proteins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BDE7C8-466F-3F41-B202-15EF1D67D776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473C8122-6198-2241-A1BE-ABEEE54D629E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10120" yWindow="2140" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1420" yWindow="500" windowWidth="35840" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,15 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataSignature="AMtx7miW6g6zRmueViZFkusAasilJg/+wQ=="/>
     </ext>
@@ -34,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7663" uniqueCount="7568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7668" uniqueCount="7570">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22716,12 +22725,6 @@
     <t>sYFP2</t>
   </si>
   <si>
-    <t>GFPmut3b*</t>
-  </si>
-  <si>
-    <t>AAB18957.1</t>
-  </si>
-  <si>
     <t>mCherry</t>
   </si>
   <si>
@@ -22731,12 +22734,6 @@
     <t>mKate2</t>
   </si>
   <si>
-    <t>mRFP1*</t>
-  </si>
-  <si>
-    <t>CAH64892</t>
-  </si>
-  <si>
     <t>mScarlet</t>
   </si>
   <si>
@@ -22776,18 +22773,6 @@
     <t>S2R mutation</t>
   </si>
   <si>
-    <t>Includes barcode after double stop</t>
-  </si>
-  <si>
-    <t>ATP07149.1</t>
-  </si>
-  <si>
-    <t>AEX25288.1</t>
-  </si>
-  <si>
-    <t>APD76535.1</t>
-  </si>
-  <si>
     <t>E0040, E1010, E0030, E0020, J97000, J97001, J97002, J97003, K592100, J06504, K864100</t>
   </si>
   <si>
@@ -22798,6 +22783,36 @@
   </si>
   <si>
     <t>DNA Parts and Devices</t>
+  </si>
+  <si>
+    <t>GFPmut3</t>
+  </si>
+  <si>
+    <t>includes barcode after double stop, 4 BbsI cut sites</t>
+  </si>
+  <si>
+    <t>Type IIS compatible version from Murray Lab</t>
+  </si>
+  <si>
+    <t>Mammalia</t>
+  </si>
+  <si>
+    <t>Sequence was missing bases, but matched to repressilator</t>
+  </si>
+  <si>
+    <t>stop codons added</t>
+  </si>
+  <si>
+    <t>Chlamydomonas reinhardtii</t>
+  </si>
+  <si>
+    <t>KY484012</t>
+  </si>
+  <si>
+    <t>KY021423</t>
+  </si>
+  <si>
+    <t>Xenopus laevis</t>
   </si>
 </sst>
 </file>
@@ -23131,7 +23146,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23186,6 +23201,8 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23642,8 +23659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23863,7 +23880,7 @@
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>7567</v>
+        <v>7559</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>13</v>
@@ -23908,7 +23925,7 @@
       <c r="I13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="41" t="s">
         <v>22</v>
       </c>
       <c r="K13" s="3" t="s">
@@ -23964,13 +23981,13 @@
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
       <c r="A15" s="18" t="s">
-        <v>7540</v>
+        <v>7518</v>
       </c>
       <c r="B15" s="41" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>7559</v>
+        <v>7555</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="18" t="s">
@@ -24002,21 +24019,25 @@
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
       <c r="A16" s="18" t="s">
-        <v>7518</v>
+        <v>7560</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="C16" s="41" t="s">
+        <v>7564</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E16" s="18" t="s">
-        <v>7553</v>
+        <v>7549</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>7469</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>7541</v>
+        <v>7485</v>
+      </c>
+      <c r="G16" s="41">
+        <v>26495</v>
       </c>
       <c r="H16" s="18" t="s">
         <v>10</v>
@@ -24118,7 +24139,7 @@
       <c r="C19" s="18"/>
       <c r="D19" s="20"/>
       <c r="E19" s="18" t="s">
-        <v>7551</v>
+        <v>7547</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>42</v>
@@ -24181,14 +24202,14 @@
       <c r="M20" s="21"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A21" s="21" t="s">
-        <v>7545</v>
+      <c r="A21" s="49" t="s">
+        <v>7519</v>
       </c>
       <c r="B21" s="41" t="s">
         <v>47</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>7560</v>
+        <v>7561</v>
       </c>
       <c r="D21" s="18"/>
       <c r="E21" s="18" t="s">
@@ -24223,16 +24244,18 @@
       <c r="B22" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="18"/>
+      <c r="C22" s="18" t="s">
+        <v>7562</v>
+      </c>
       <c r="D22" s="20"/>
       <c r="E22" s="18" t="s">
-        <v>7555</v>
+        <v>7551</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>7469</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>7546</v>
+        <v>7485</v>
+      </c>
+      <c r="G22" s="41">
+        <v>120957</v>
       </c>
       <c r="H22" s="18"/>
       <c r="I22" s="18" t="s">
@@ -24252,27 +24275,31 @@
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
       <c r="A23" s="41" t="s">
-        <v>7547</v>
+        <v>7543</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="20"/>
+      <c r="C23" s="41" t="s">
+        <v>7565</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>7445</v>
+      </c>
       <c r="E23" s="18" t="s">
-        <v>7556</v>
+        <v>7552</v>
       </c>
       <c r="F23" s="18" t="s">
         <v>7469</v>
       </c>
-      <c r="G23" s="18" t="s">
-        <v>7563</v>
+      <c r="G23" s="41" t="s">
+        <v>7568</v>
       </c>
       <c r="H23" s="18" t="s">
         <v>7417</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>7419</v>
+        <v>7563</v>
       </c>
       <c r="J23" s="18" t="b">
         <v>1</v>
@@ -24288,7 +24315,7 @@
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
       <c r="A24" s="18" t="s">
-        <v>7542</v>
+        <v>7540</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>47</v>
@@ -24296,13 +24323,13 @@
       <c r="C24" s="18"/>
       <c r="D24" s="20"/>
       <c r="E24" s="18" t="s">
-        <v>7552</v>
+        <v>7548</v>
       </c>
       <c r="F24" s="18" t="s">
         <v>42</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>7543</v>
+        <v>7541</v>
       </c>
       <c r="H24" s="18"/>
       <c r="I24" t="s">
@@ -24322,7 +24349,7 @@
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>7544</v>
+        <v>7542</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>47</v>
@@ -24330,17 +24357,17 @@
       <c r="C25" s="18"/>
       <c r="D25" s="20"/>
       <c r="E25" s="18" t="s">
-        <v>7554</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>7469</v>
-      </c>
-      <c r="G25" t="s">
-        <v>7562</v>
+        <v>7550</v>
+      </c>
+      <c r="F25" s="41" t="s">
+        <v>7485</v>
+      </c>
+      <c r="G25" s="49">
+        <v>54827</v>
       </c>
       <c r="H25" s="18"/>
       <c r="I25" s="18" t="s">
-        <v>7419</v>
+        <v>7569</v>
       </c>
       <c r="J25" s="18" t="b">
         <v>1</v>
@@ -24428,7 +24455,7 @@
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
       <c r="A28" s="41" t="s">
-        <v>7549</v>
+        <v>7545</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>47</v>
@@ -24436,13 +24463,13 @@
       <c r="C28" s="21"/>
       <c r="D28" s="20"/>
       <c r="E28" s="18" t="s">
-        <v>7557</v>
+        <v>7553</v>
       </c>
       <c r="F28" s="18" t="s">
         <v>42</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>7548</v>
+        <v>7544</v>
       </c>
       <c r="H28" s="18"/>
       <c r="I28" s="18" t="s">
@@ -24462,7 +24489,7 @@
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
       <c r="A29" s="41" t="s">
-        <v>7550</v>
+        <v>7546</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>47</v>
@@ -24470,19 +24497,19 @@
       <c r="C29" s="18"/>
       <c r="D29" s="20"/>
       <c r="E29" s="18" t="s">
-        <v>7558</v>
+        <v>7554</v>
       </c>
       <c r="F29" s="18" t="s">
         <v>7469</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>7561</v>
+        <v>7567</v>
       </c>
       <c r="H29" s="18" t="s">
         <v>10</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>7419</v>
+        <v>7566</v>
       </c>
       <c r="J29" s="18" t="b">
         <v>1</v>
@@ -26178,7 +26205,7 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" s="21" t="s">
-        <v>7565</v>
+        <v>7557</v>
       </c>
       <c r="B14" s="21"/>
       <c r="D14" s="21" t="b">
@@ -26189,7 +26216,7 @@
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="21" t="s">
-        <v>7564</v>
+        <v>7556</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="32"/>
@@ -68957,7 +68984,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -69366,15 +69393,30 @@
       <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B30" s="3"/>
+      <c r="A30" s="48" t="s">
+        <v>7563</v>
+      </c>
+      <c r="B30" s="18">
+        <v>40674</v>
+      </c>
       <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1">
-      <c r="B31" s="3"/>
+      <c r="A31" s="48" t="s">
+        <v>7566</v>
+      </c>
+      <c r="B31" s="18">
+        <v>3055</v>
+      </c>
       <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1">
-      <c r="B32" s="3"/>
+      <c r="A32" s="48" t="s">
+        <v>7569</v>
+      </c>
+      <c r="B32" s="18">
+        <v>8355</v>
+      </c>
       <c r="C32" s="3"/>
     </row>
     <row r="33" spans="2:3" ht="15.75" customHeight="1">
@@ -73282,7 +73324,7 @@
         <v>7514</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>7566</v>
+        <v>7558</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="33"/>

</xml_diff>

<commit_message>
update contributed excel to current template
(cherry picked from commit 1cf50d032562e6e8d8a6a267133e0c9cf55d2e44)
</commit_message>
<xml_diff>
--- a/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
+++ b/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Fluorescent Reporter Proteins/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/Fluorescent Reporter Proteins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473C8122-6198-2241-A1BE-ABEEE54D629E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED12EE5-8A8C-1E4D-B629-5E469F1EA25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="500" windowWidth="35840" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7668" uniqueCount="7570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7669" uniqueCount="7571">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22814,12 +22814,15 @@
   <si>
     <t>Xenopus laevis</t>
   </si>
+  <si>
+    <t>Literal Part</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -22998,6 +23001,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -23146,7 +23155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23196,13 +23205,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23659,7 +23669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -23730,12 +23740,12 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="47"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="49"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -24202,7 +24212,7 @@
       <c r="M20" s="21"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="46" t="s">
         <v>7519</v>
       </c>
       <c r="B21" s="41" t="s">
@@ -24362,7 +24372,7 @@
       <c r="F25" s="41" t="s">
         <v>7485</v>
       </c>
-      <c r="G25" s="49">
+      <c r="G25" s="46">
         <v>54827</v>
       </c>
       <c r="H25" s="18"/>
@@ -69393,7 +69403,7 @@
       <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A30" s="48" t="s">
+      <c r="A30" s="45" t="s">
         <v>7563</v>
       </c>
       <c r="B30" s="18">
@@ -69402,7 +69412,7 @@
       <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="45" t="s">
         <v>7566</v>
       </c>
       <c r="B31" s="18">
@@ -69411,7 +69421,7 @@
       <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1">
-      <c r="A32" s="48" t="s">
+      <c r="A32" s="45" t="s">
         <v>7569</v>
       </c>
       <c r="B32" s="18">
@@ -72085,10 +72095,10 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -72098,10 +72108,12 @@
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="26" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="40" customWidth="1"/>
+    <col min="8" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="37" t="s">
         <v>7462</v>
       </c>
@@ -72120,8 +72132,11 @@
       <c r="F1" s="37" t="s">
         <v>7467</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G1" s="33" t="s">
+        <v>7570</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>7468</v>
       </c>
@@ -72140,8 +72155,11 @@
       <c r="F2" s="38" t="s">
         <v>7473</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G2" s="50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>7474</v>
       </c>
@@ -72160,8 +72178,11 @@
       <c r="F3" s="38" t="s">
         <v>7478</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G3" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="11" t="s">
         <v>7479</v>
       </c>
@@ -72180,8 +72201,11 @@
       <c r="F4" s="38" t="s">
         <v>7483</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G4" s="50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="11" t="s">
         <v>7484</v>
       </c>
@@ -72200,8 +72224,11 @@
       <c r="F5" s="38" t="s">
         <v>7489</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G5" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="11" t="s">
         <v>8</v>
       </c>
@@ -72220,8 +72247,11 @@
       <c r="F6" s="38" t="s">
         <v>7494</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G6" s="50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>7416</v>
       </c>
@@ -72240,1042 +72270,3024 @@
       <c r="F7" s="38" t="s">
         <v>7499</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G7" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="35"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G8" s="50"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G9" s="50"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G10" s="50"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G11" s="50"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G12" s="50"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G13" s="50"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1"/>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
-    <row r="97" ht="15.75" customHeight="1"/>
-    <row r="98" ht="15.75" customHeight="1"/>
-    <row r="99" ht="15.75" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1"/>
-    <row r="114" ht="15.75" customHeight="1"/>
-    <row r="115" ht="15.75" customHeight="1"/>
-    <row r="116" ht="15.75" customHeight="1"/>
-    <row r="117" ht="15.75" customHeight="1"/>
-    <row r="118" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="120" ht="15.75" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
-    <row r="126" ht="15.75" customHeight="1"/>
-    <row r="127" ht="15.75" customHeight="1"/>
-    <row r="128" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
-    <row r="134" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="136" ht="15.75" customHeight="1"/>
-    <row r="137" ht="15.75" customHeight="1"/>
-    <row r="138" ht="15.75" customHeight="1"/>
-    <row r="139" ht="15.75" customHeight="1"/>
-    <row r="140" ht="15.75" customHeight="1"/>
-    <row r="141" ht="15.75" customHeight="1"/>
-    <row r="142" ht="15.75" customHeight="1"/>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
-    <row r="147" ht="15.75" customHeight="1"/>
-    <row r="148" ht="15.75" customHeight="1"/>
-    <row r="149" ht="15.75" customHeight="1"/>
-    <row r="150" ht="15.75" customHeight="1"/>
-    <row r="151" ht="15.75" customHeight="1"/>
-    <row r="152" ht="15.75" customHeight="1"/>
-    <row r="153" ht="15.75" customHeight="1"/>
-    <row r="154" ht="15.75" customHeight="1"/>
-    <row r="155" ht="15.75" customHeight="1"/>
-    <row r="156" ht="15.75" customHeight="1"/>
-    <row r="157" ht="15.75" customHeight="1"/>
-    <row r="158" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
-    <row r="161" ht="15.75" customHeight="1"/>
-    <row r="162" ht="15.75" customHeight="1"/>
-    <row r="163" ht="15.75" customHeight="1"/>
-    <row r="164" ht="15.75" customHeight="1"/>
-    <row r="165" ht="15.75" customHeight="1"/>
-    <row r="166" ht="15.75" customHeight="1"/>
-    <row r="167" ht="15.75" customHeight="1"/>
-    <row r="168" ht="15.75" customHeight="1"/>
-    <row r="169" ht="15.75" customHeight="1"/>
-    <row r="170" ht="15.75" customHeight="1"/>
-    <row r="171" ht="15.75" customHeight="1"/>
-    <row r="172" ht="15.75" customHeight="1"/>
-    <row r="173" ht="15.75" customHeight="1"/>
-    <row r="174" ht="15.75" customHeight="1"/>
-    <row r="175" ht="15.75" customHeight="1"/>
-    <row r="176" ht="15.75" customHeight="1"/>
-    <row r="177" ht="15.75" customHeight="1"/>
-    <row r="178" ht="15.75" customHeight="1"/>
-    <row r="179" ht="15.75" customHeight="1"/>
-    <row r="180" ht="15.75" customHeight="1"/>
-    <row r="181" ht="15.75" customHeight="1"/>
-    <row r="182" ht="15.75" customHeight="1"/>
-    <row r="183" ht="15.75" customHeight="1"/>
-    <row r="184" ht="15.75" customHeight="1"/>
-    <row r="185" ht="15.75" customHeight="1"/>
-    <row r="186" ht="15.75" customHeight="1"/>
-    <row r="187" ht="15.75" customHeight="1"/>
-    <row r="188" ht="15.75" customHeight="1"/>
-    <row r="189" ht="15.75" customHeight="1"/>
-    <row r="190" ht="15.75" customHeight="1"/>
-    <row r="191" ht="15.75" customHeight="1"/>
-    <row r="192" ht="15.75" customHeight="1"/>
-    <row r="193" ht="15.75" customHeight="1"/>
-    <row r="194" ht="15.75" customHeight="1"/>
-    <row r="195" ht="15.75" customHeight="1"/>
-    <row r="196" ht="15.75" customHeight="1"/>
-    <row r="197" ht="15.75" customHeight="1"/>
-    <row r="198" ht="15.75" customHeight="1"/>
-    <row r="199" ht="15.75" customHeight="1"/>
-    <row r="200" ht="15.75" customHeight="1"/>
-    <row r="201" ht="15.75" customHeight="1"/>
-    <row r="202" ht="15.75" customHeight="1"/>
-    <row r="203" ht="15.75" customHeight="1"/>
-    <row r="204" ht="15.75" customHeight="1"/>
-    <row r="205" ht="15.75" customHeight="1"/>
-    <row r="206" ht="15.75" customHeight="1"/>
-    <row r="207" ht="15.75" customHeight="1"/>
-    <row r="208" ht="15.75" customHeight="1"/>
-    <row r="209" ht="15.75" customHeight="1"/>
-    <row r="210" ht="15.75" customHeight="1"/>
-    <row r="211" ht="15.75" customHeight="1"/>
-    <row r="212" ht="15.75" customHeight="1"/>
-    <row r="213" ht="15.75" customHeight="1"/>
-    <row r="214" ht="15.75" customHeight="1"/>
-    <row r="215" ht="15.75" customHeight="1"/>
-    <row r="216" ht="15.75" customHeight="1"/>
-    <row r="217" ht="15.75" customHeight="1"/>
-    <row r="218" ht="15.75" customHeight="1"/>
-    <row r="219" ht="15.75" customHeight="1"/>
-    <row r="220" ht="15.75" customHeight="1"/>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
-    <row r="225" ht="15.75" customHeight="1"/>
-    <row r="226" ht="15.75" customHeight="1"/>
-    <row r="227" ht="15.75" customHeight="1"/>
-    <row r="228" ht="15.75" customHeight="1"/>
-    <row r="229" ht="15.75" customHeight="1"/>
-    <row r="230" ht="15.75" customHeight="1"/>
-    <row r="231" ht="15.75" customHeight="1"/>
-    <row r="232" ht="15.75" customHeight="1"/>
-    <row r="233" ht="15.75" customHeight="1"/>
-    <row r="234" ht="15.75" customHeight="1"/>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
-    <row r="237" ht="15.75" customHeight="1"/>
-    <row r="238" ht="15.75" customHeight="1"/>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="240" ht="15.75" customHeight="1"/>
-    <row r="241" ht="15.75" customHeight="1"/>
-    <row r="242" ht="15.75" customHeight="1"/>
-    <row r="243" ht="15.75" customHeight="1"/>
-    <row r="244" ht="15.75" customHeight="1"/>
-    <row r="245" ht="15.75" customHeight="1"/>
-    <row r="246" ht="15.75" customHeight="1"/>
-    <row r="247" ht="15.75" customHeight="1"/>
-    <row r="248" ht="15.75" customHeight="1"/>
-    <row r="249" ht="15.75" customHeight="1"/>
-    <row r="250" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
-    <row r="252" ht="15.75" customHeight="1"/>
-    <row r="253" ht="15.75" customHeight="1"/>
-    <row r="254" ht="15.75" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="256" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
+      <c r="G14" s="50"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+      <c r="G15" s="50"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+      <c r="G16" s="50"/>
+    </row>
+    <row r="17" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G17" s="50"/>
+    </row>
+    <row r="18" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G18" s="50"/>
+    </row>
+    <row r="19" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G19" s="50"/>
+    </row>
+    <row r="20" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G20" s="50"/>
+    </row>
+    <row r="21" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G21" s="50"/>
+    </row>
+    <row r="22" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G22" s="50"/>
+    </row>
+    <row r="23" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G23" s="50"/>
+    </row>
+    <row r="24" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G24" s="50"/>
+    </row>
+    <row r="25" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G25" s="50"/>
+    </row>
+    <row r="26" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G26" s="50"/>
+    </row>
+    <row r="27" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G27" s="50"/>
+    </row>
+    <row r="28" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G28" s="50"/>
+    </row>
+    <row r="29" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G29" s="50"/>
+    </row>
+    <row r="30" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G30" s="50"/>
+    </row>
+    <row r="31" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G31" s="50"/>
+    </row>
+    <row r="32" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G32" s="50"/>
+    </row>
+    <row r="33" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G33" s="50"/>
+    </row>
+    <row r="34" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G34" s="50"/>
+    </row>
+    <row r="35" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G35" s="50"/>
+    </row>
+    <row r="36" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G36" s="50"/>
+    </row>
+    <row r="37" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G37" s="50"/>
+    </row>
+    <row r="38" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G38" s="50"/>
+    </row>
+    <row r="39" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G39" s="50"/>
+    </row>
+    <row r="40" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G40" s="50"/>
+    </row>
+    <row r="41" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G41" s="50"/>
+    </row>
+    <row r="42" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G42" s="50"/>
+    </row>
+    <row r="43" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G43" s="50"/>
+    </row>
+    <row r="44" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G44" s="50"/>
+    </row>
+    <row r="45" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G45" s="50"/>
+    </row>
+    <row r="46" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G46" s="50"/>
+    </row>
+    <row r="47" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G47" s="50"/>
+    </row>
+    <row r="48" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G48" s="50"/>
+    </row>
+    <row r="49" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G49" s="50"/>
+    </row>
+    <row r="50" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G50" s="50"/>
+    </row>
+    <row r="51" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G51" s="50"/>
+    </row>
+    <row r="52" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G52" s="50"/>
+    </row>
+    <row r="53" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G53" s="50"/>
+    </row>
+    <row r="54" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G54" s="50"/>
+    </row>
+    <row r="55" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G55" s="50"/>
+    </row>
+    <row r="56" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G56" s="50"/>
+    </row>
+    <row r="57" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G57" s="50"/>
+    </row>
+    <row r="58" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G58" s="50"/>
+    </row>
+    <row r="59" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G59" s="50"/>
+    </row>
+    <row r="60" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G60" s="50"/>
+    </row>
+    <row r="61" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G61" s="50"/>
+    </row>
+    <row r="62" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G62" s="50"/>
+    </row>
+    <row r="63" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G63" s="50"/>
+    </row>
+    <row r="64" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G64" s="50"/>
+    </row>
+    <row r="65" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G65" s="50"/>
+    </row>
+    <row r="66" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G66" s="50"/>
+    </row>
+    <row r="67" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G67" s="50"/>
+    </row>
+    <row r="68" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G68" s="50"/>
+    </row>
+    <row r="69" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G69" s="50"/>
+    </row>
+    <row r="70" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G70" s="50"/>
+    </row>
+    <row r="71" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G71" s="50"/>
+    </row>
+    <row r="72" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G72" s="50"/>
+    </row>
+    <row r="73" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G73" s="50"/>
+    </row>
+    <row r="74" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G74" s="50"/>
+    </row>
+    <row r="75" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G75" s="50"/>
+    </row>
+    <row r="76" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G76" s="50"/>
+    </row>
+    <row r="77" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G77" s="50"/>
+    </row>
+    <row r="78" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G78" s="50"/>
+    </row>
+    <row r="79" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G79" s="50"/>
+    </row>
+    <row r="80" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G80" s="50"/>
+    </row>
+    <row r="81" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G81" s="50"/>
+    </row>
+    <row r="82" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G82" s="50"/>
+    </row>
+    <row r="83" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G83" s="50"/>
+    </row>
+    <row r="84" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G84" s="50"/>
+    </row>
+    <row r="85" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G85" s="50"/>
+    </row>
+    <row r="86" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G86" s="50"/>
+    </row>
+    <row r="87" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G87" s="50"/>
+    </row>
+    <row r="88" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G88" s="50"/>
+    </row>
+    <row r="89" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G89" s="50"/>
+    </row>
+    <row r="90" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G90" s="50"/>
+    </row>
+    <row r="91" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G91" s="50"/>
+    </row>
+    <row r="92" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G92" s="50"/>
+    </row>
+    <row r="93" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G93" s="50"/>
+    </row>
+    <row r="94" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G94" s="50"/>
+    </row>
+    <row r="95" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G95" s="50"/>
+    </row>
+    <row r="96" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G96" s="50"/>
+    </row>
+    <row r="97" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G97" s="50"/>
+    </row>
+    <row r="98" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G98" s="50"/>
+    </row>
+    <row r="99" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G99" s="50"/>
+    </row>
+    <row r="100" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G100" s="50"/>
+    </row>
+    <row r="101" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G101" s="50"/>
+    </row>
+    <row r="102" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G102" s="50"/>
+    </row>
+    <row r="103" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G103" s="50"/>
+    </row>
+    <row r="104" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G104" s="50"/>
+    </row>
+    <row r="105" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G105" s="50"/>
+    </row>
+    <row r="106" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G106" s="50"/>
+    </row>
+    <row r="107" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G107" s="50"/>
+    </row>
+    <row r="108" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G108" s="50"/>
+    </row>
+    <row r="109" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G109" s="50"/>
+    </row>
+    <row r="110" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G110" s="50"/>
+    </row>
+    <row r="111" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G111" s="50"/>
+    </row>
+    <row r="112" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G112" s="50"/>
+    </row>
+    <row r="113" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G113" s="50"/>
+    </row>
+    <row r="114" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G114" s="50"/>
+    </row>
+    <row r="115" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G115" s="50"/>
+    </row>
+    <row r="116" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G116" s="50"/>
+    </row>
+    <row r="117" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G117" s="50"/>
+    </row>
+    <row r="118" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G118" s="50"/>
+    </row>
+    <row r="119" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G119" s="50"/>
+    </row>
+    <row r="120" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G120" s="50"/>
+    </row>
+    <row r="121" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G121" s="50"/>
+    </row>
+    <row r="122" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G122" s="50"/>
+    </row>
+    <row r="123" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G123" s="50"/>
+    </row>
+    <row r="124" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G124" s="50"/>
+    </row>
+    <row r="125" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G125" s="50"/>
+    </row>
+    <row r="126" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G126" s="50"/>
+    </row>
+    <row r="127" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G127" s="50"/>
+    </row>
+    <row r="128" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G128" s="50"/>
+    </row>
+    <row r="129" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G129" s="50"/>
+    </row>
+    <row r="130" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G130" s="50"/>
+    </row>
+    <row r="131" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G131" s="50"/>
+    </row>
+    <row r="132" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G132" s="50"/>
+    </row>
+    <row r="133" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G133" s="50"/>
+    </row>
+    <row r="134" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G134" s="50"/>
+    </row>
+    <row r="135" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G135" s="50"/>
+    </row>
+    <row r="136" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G136" s="50"/>
+    </row>
+    <row r="137" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G137" s="50"/>
+    </row>
+    <row r="138" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G138" s="50"/>
+    </row>
+    <row r="139" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G139" s="50"/>
+    </row>
+    <row r="140" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G140" s="50"/>
+    </row>
+    <row r="141" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G141" s="50"/>
+    </row>
+    <row r="142" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G142" s="50"/>
+    </row>
+    <row r="143" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G143" s="50"/>
+    </row>
+    <row r="144" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G144" s="50"/>
+    </row>
+    <row r="145" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G145" s="50"/>
+    </row>
+    <row r="146" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G146" s="50"/>
+    </row>
+    <row r="147" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G147" s="50"/>
+    </row>
+    <row r="148" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G148" s="50"/>
+    </row>
+    <row r="149" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G149" s="50"/>
+    </row>
+    <row r="150" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G150" s="50"/>
+    </row>
+    <row r="151" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G151" s="50"/>
+    </row>
+    <row r="152" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G152" s="50"/>
+    </row>
+    <row r="153" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G153" s="50"/>
+    </row>
+    <row r="154" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G154" s="50"/>
+    </row>
+    <row r="155" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G155" s="50"/>
+    </row>
+    <row r="156" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G156" s="50"/>
+    </row>
+    <row r="157" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G157" s="50"/>
+    </row>
+    <row r="158" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G158" s="50"/>
+    </row>
+    <row r="159" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G159" s="50"/>
+    </row>
+    <row r="160" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G160" s="50"/>
+    </row>
+    <row r="161" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G161" s="50"/>
+    </row>
+    <row r="162" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G162" s="50"/>
+    </row>
+    <row r="163" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G163" s="50"/>
+    </row>
+    <row r="164" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G164" s="50"/>
+    </row>
+    <row r="165" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G165" s="50"/>
+    </row>
+    <row r="166" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G166" s="50"/>
+    </row>
+    <row r="167" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G167" s="50"/>
+    </row>
+    <row r="168" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G168" s="50"/>
+    </row>
+    <row r="169" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G169" s="50"/>
+    </row>
+    <row r="170" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G170" s="50"/>
+    </row>
+    <row r="171" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G171" s="50"/>
+    </row>
+    <row r="172" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G172" s="50"/>
+    </row>
+    <row r="173" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G173" s="50"/>
+    </row>
+    <row r="174" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G174" s="50"/>
+    </row>
+    <row r="175" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G175" s="50"/>
+    </row>
+    <row r="176" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G176" s="50"/>
+    </row>
+    <row r="177" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G177" s="50"/>
+    </row>
+    <row r="178" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G178" s="50"/>
+    </row>
+    <row r="179" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G179" s="50"/>
+    </row>
+    <row r="180" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G180" s="50"/>
+    </row>
+    <row r="181" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G181" s="50"/>
+    </row>
+    <row r="182" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G182" s="50"/>
+    </row>
+    <row r="183" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G183" s="50"/>
+    </row>
+    <row r="184" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G184" s="50"/>
+    </row>
+    <row r="185" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G185" s="50"/>
+    </row>
+    <row r="186" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G186" s="50"/>
+    </row>
+    <row r="187" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G187" s="50"/>
+    </row>
+    <row r="188" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G188" s="50"/>
+    </row>
+    <row r="189" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G189" s="50"/>
+    </row>
+    <row r="190" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G190" s="50"/>
+    </row>
+    <row r="191" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G191" s="50"/>
+    </row>
+    <row r="192" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G192" s="50"/>
+    </row>
+    <row r="193" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G193" s="50"/>
+    </row>
+    <row r="194" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G194" s="50"/>
+    </row>
+    <row r="195" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G195" s="50"/>
+    </row>
+    <row r="196" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G196" s="50"/>
+    </row>
+    <row r="197" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G197" s="50"/>
+    </row>
+    <row r="198" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G198" s="50"/>
+    </row>
+    <row r="199" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G199" s="50"/>
+    </row>
+    <row r="200" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G200" s="50"/>
+    </row>
+    <row r="201" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G201" s="50"/>
+    </row>
+    <row r="202" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G202" s="50"/>
+    </row>
+    <row r="203" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G203" s="50"/>
+    </row>
+    <row r="204" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G204" s="50"/>
+    </row>
+    <row r="205" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G205" s="50"/>
+    </row>
+    <row r="206" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G206" s="50"/>
+    </row>
+    <row r="207" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G207" s="50"/>
+    </row>
+    <row r="208" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G208" s="50"/>
+    </row>
+    <row r="209" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G209" s="50"/>
+    </row>
+    <row r="210" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G210" s="50"/>
+    </row>
+    <row r="211" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G211" s="50"/>
+    </row>
+    <row r="212" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G212" s="50"/>
+    </row>
+    <row r="213" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G213" s="50"/>
+    </row>
+    <row r="214" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G214" s="50"/>
+    </row>
+    <row r="215" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G215" s="50"/>
+    </row>
+    <row r="216" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G216" s="50"/>
+    </row>
+    <row r="217" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G217" s="50"/>
+    </row>
+    <row r="218" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G218" s="50"/>
+    </row>
+    <row r="219" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G219" s="50"/>
+    </row>
+    <row r="220" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G220" s="50"/>
+    </row>
+    <row r="221" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G221" s="50"/>
+    </row>
+    <row r="222" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G222" s="50"/>
+    </row>
+    <row r="223" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G223" s="50"/>
+    </row>
+    <row r="224" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G224" s="50"/>
+    </row>
+    <row r="225" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G225" s="50"/>
+    </row>
+    <row r="226" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G226" s="50"/>
+    </row>
+    <row r="227" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G227" s="50"/>
+    </row>
+    <row r="228" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G228" s="50"/>
+    </row>
+    <row r="229" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G229" s="50"/>
+    </row>
+    <row r="230" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G230" s="50"/>
+    </row>
+    <row r="231" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G231" s="50"/>
+    </row>
+    <row r="232" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G232" s="50"/>
+    </row>
+    <row r="233" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G233" s="50"/>
+    </row>
+    <row r="234" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G234" s="50"/>
+    </row>
+    <row r="235" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G235" s="50"/>
+    </row>
+    <row r="236" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G236" s="50"/>
+    </row>
+    <row r="237" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G237" s="50"/>
+    </row>
+    <row r="238" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G238" s="50"/>
+    </row>
+    <row r="239" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G239" s="50"/>
+    </row>
+    <row r="240" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G240" s="50"/>
+    </row>
+    <row r="241" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G241" s="50"/>
+    </row>
+    <row r="242" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G242" s="50"/>
+    </row>
+    <row r="243" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G243" s="50"/>
+    </row>
+    <row r="244" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G244" s="50"/>
+    </row>
+    <row r="245" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G245" s="50"/>
+    </row>
+    <row r="246" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G246" s="50"/>
+    </row>
+    <row r="247" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G247" s="50"/>
+    </row>
+    <row r="248" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G248" s="50"/>
+    </row>
+    <row r="249" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G249" s="50"/>
+    </row>
+    <row r="250" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G250" s="50"/>
+    </row>
+    <row r="251" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G251" s="50"/>
+    </row>
+    <row r="252" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G252" s="50"/>
+    </row>
+    <row r="253" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G253" s="50"/>
+    </row>
+    <row r="254" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G254" s="50"/>
+    </row>
+    <row r="255" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G255" s="50"/>
+    </row>
+    <row r="256" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G256" s="50"/>
+    </row>
+    <row r="257" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G257" s="50"/>
+    </row>
+    <row r="258" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G258" s="50"/>
+    </row>
+    <row r="259" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G259" s="50"/>
+    </row>
+    <row r="260" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G260" s="50"/>
+    </row>
+    <row r="261" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G261" s="50"/>
+    </row>
+    <row r="262" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G262" s="50"/>
+    </row>
+    <row r="263" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G263" s="50"/>
+    </row>
+    <row r="264" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G264" s="50"/>
+    </row>
+    <row r="265" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G265" s="50"/>
+    </row>
+    <row r="266" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G266" s="50"/>
+    </row>
+    <row r="267" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G267" s="50"/>
+    </row>
+    <row r="268" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G268" s="50"/>
+    </row>
+    <row r="269" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G269" s="50"/>
+    </row>
+    <row r="270" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G270" s="50"/>
+    </row>
+    <row r="271" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G271" s="50"/>
+    </row>
+    <row r="272" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G272" s="50"/>
+    </row>
+    <row r="273" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G273" s="50"/>
+    </row>
+    <row r="274" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G274" s="50"/>
+    </row>
+    <row r="275" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G275" s="50"/>
+    </row>
+    <row r="276" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G276" s="50"/>
+    </row>
+    <row r="277" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G277" s="50"/>
+    </row>
+    <row r="278" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G278" s="50"/>
+    </row>
+    <row r="279" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G279" s="50"/>
+    </row>
+    <row r="280" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G280" s="50"/>
+    </row>
+    <row r="281" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G281" s="50"/>
+    </row>
+    <row r="282" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G282" s="50"/>
+    </row>
+    <row r="283" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G283" s="50"/>
+    </row>
+    <row r="284" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G284" s="50"/>
+    </row>
+    <row r="285" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G285" s="50"/>
+    </row>
+    <row r="286" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G286" s="50"/>
+    </row>
+    <row r="287" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G287" s="50"/>
+    </row>
+    <row r="288" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G288" s="50"/>
+    </row>
+    <row r="289" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G289" s="50"/>
+    </row>
+    <row r="290" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G290" s="50"/>
+    </row>
+    <row r="291" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G291" s="50"/>
+    </row>
+    <row r="292" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G292" s="50"/>
+    </row>
+    <row r="293" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G293" s="50"/>
+    </row>
+    <row r="294" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G294" s="50"/>
+    </row>
+    <row r="295" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G295" s="50"/>
+    </row>
+    <row r="296" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G296" s="50"/>
+    </row>
+    <row r="297" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G297" s="50"/>
+    </row>
+    <row r="298" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G298" s="50"/>
+    </row>
+    <row r="299" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G299" s="50"/>
+    </row>
+    <row r="300" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G300" s="50"/>
+    </row>
+    <row r="301" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G301" s="50"/>
+    </row>
+    <row r="302" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G302" s="50"/>
+    </row>
+    <row r="303" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G303" s="50"/>
+    </row>
+    <row r="304" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G304" s="50"/>
+    </row>
+    <row r="305" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G305" s="50"/>
+    </row>
+    <row r="306" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G306" s="50"/>
+    </row>
+    <row r="307" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G307" s="50"/>
+    </row>
+    <row r="308" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G308" s="50"/>
+    </row>
+    <row r="309" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G309" s="50"/>
+    </row>
+    <row r="310" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G310" s="50"/>
+    </row>
+    <row r="311" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G311" s="50"/>
+    </row>
+    <row r="312" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G312" s="50"/>
+    </row>
+    <row r="313" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G313" s="50"/>
+    </row>
+    <row r="314" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G314" s="50"/>
+    </row>
+    <row r="315" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G315" s="50"/>
+    </row>
+    <row r="316" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G316" s="50"/>
+    </row>
+    <row r="317" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G317" s="50"/>
+    </row>
+    <row r="318" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G318" s="50"/>
+    </row>
+    <row r="319" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G319" s="50"/>
+    </row>
+    <row r="320" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G320" s="50"/>
+    </row>
+    <row r="321" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G321" s="50"/>
+    </row>
+    <row r="322" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G322" s="50"/>
+    </row>
+    <row r="323" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G323" s="50"/>
+    </row>
+    <row r="324" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G324" s="50"/>
+    </row>
+    <row r="325" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G325" s="50"/>
+    </row>
+    <row r="326" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G326" s="50"/>
+    </row>
+    <row r="327" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G327" s="50"/>
+    </row>
+    <row r="328" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G328" s="50"/>
+    </row>
+    <row r="329" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G329" s="50"/>
+    </row>
+    <row r="330" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G330" s="50"/>
+    </row>
+    <row r="331" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G331" s="50"/>
+    </row>
+    <row r="332" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G332" s="50"/>
+    </row>
+    <row r="333" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G333" s="50"/>
+    </row>
+    <row r="334" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G334" s="50"/>
+    </row>
+    <row r="335" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G335" s="50"/>
+    </row>
+    <row r="336" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G336" s="50"/>
+    </row>
+    <row r="337" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G337" s="50"/>
+    </row>
+    <row r="338" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G338" s="50"/>
+    </row>
+    <row r="339" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G339" s="50"/>
+    </row>
+    <row r="340" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G340" s="50"/>
+    </row>
+    <row r="341" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G341" s="50"/>
+    </row>
+    <row r="342" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G342" s="50"/>
+    </row>
+    <row r="343" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G343" s="50"/>
+    </row>
+    <row r="344" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G344" s="50"/>
+    </row>
+    <row r="345" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G345" s="50"/>
+    </row>
+    <row r="346" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G346" s="50"/>
+    </row>
+    <row r="347" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G347" s="50"/>
+    </row>
+    <row r="348" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G348" s="50"/>
+    </row>
+    <row r="349" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G349" s="50"/>
+    </row>
+    <row r="350" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G350" s="50"/>
+    </row>
+    <row r="351" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G351" s="50"/>
+    </row>
+    <row r="352" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G352" s="50"/>
+    </row>
+    <row r="353" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G353" s="50"/>
+    </row>
+    <row r="354" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G354" s="50"/>
+    </row>
+    <row r="355" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G355" s="50"/>
+    </row>
+    <row r="356" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G356" s="50"/>
+    </row>
+    <row r="357" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G357" s="50"/>
+    </row>
+    <row r="358" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G358" s="50"/>
+    </row>
+    <row r="359" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G359" s="50"/>
+    </row>
+    <row r="360" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G360" s="50"/>
+    </row>
+    <row r="361" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G361" s="50"/>
+    </row>
+    <row r="362" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G362" s="50"/>
+    </row>
+    <row r="363" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G363" s="50"/>
+    </row>
+    <row r="364" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G364" s="50"/>
+    </row>
+    <row r="365" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G365" s="50"/>
+    </row>
+    <row r="366" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G366" s="50"/>
+    </row>
+    <row r="367" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G367" s="50"/>
+    </row>
+    <row r="368" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G368" s="50"/>
+    </row>
+    <row r="369" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G369" s="50"/>
+    </row>
+    <row r="370" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G370" s="50"/>
+    </row>
+    <row r="371" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G371" s="50"/>
+    </row>
+    <row r="372" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G372" s="50"/>
+    </row>
+    <row r="373" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G373" s="50"/>
+    </row>
+    <row r="374" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G374" s="50"/>
+    </row>
+    <row r="375" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G375" s="50"/>
+    </row>
+    <row r="376" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G376" s="50"/>
+    </row>
+    <row r="377" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G377" s="50"/>
+    </row>
+    <row r="378" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G378" s="50"/>
+    </row>
+    <row r="379" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G379" s="50"/>
+    </row>
+    <row r="380" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G380" s="50"/>
+    </row>
+    <row r="381" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G381" s="50"/>
+    </row>
+    <row r="382" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G382" s="50"/>
+    </row>
+    <row r="383" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G383" s="50"/>
+    </row>
+    <row r="384" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G384" s="50"/>
+    </row>
+    <row r="385" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G385" s="50"/>
+    </row>
+    <row r="386" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G386" s="50"/>
+    </row>
+    <row r="387" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G387" s="50"/>
+    </row>
+    <row r="388" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G388" s="50"/>
+    </row>
+    <row r="389" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G389" s="50"/>
+    </row>
+    <row r="390" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G390" s="50"/>
+    </row>
+    <row r="391" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G391" s="50"/>
+    </row>
+    <row r="392" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G392" s="50"/>
+    </row>
+    <row r="393" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G393" s="50"/>
+    </row>
+    <row r="394" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G394" s="50"/>
+    </row>
+    <row r="395" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G395" s="50"/>
+    </row>
+    <row r="396" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G396" s="50"/>
+    </row>
+    <row r="397" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G397" s="50"/>
+    </row>
+    <row r="398" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G398" s="50"/>
+    </row>
+    <row r="399" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G399" s="50"/>
+    </row>
+    <row r="400" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G400" s="50"/>
+    </row>
+    <row r="401" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G401" s="50"/>
+    </row>
+    <row r="402" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G402" s="50"/>
+    </row>
+    <row r="403" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G403" s="50"/>
+    </row>
+    <row r="404" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G404" s="50"/>
+    </row>
+    <row r="405" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G405" s="50"/>
+    </row>
+    <row r="406" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G406" s="50"/>
+    </row>
+    <row r="407" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G407" s="50"/>
+    </row>
+    <row r="408" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G408" s="50"/>
+    </row>
+    <row r="409" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G409" s="50"/>
+    </row>
+    <row r="410" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G410" s="50"/>
+    </row>
+    <row r="411" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G411" s="50"/>
+    </row>
+    <row r="412" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G412" s="50"/>
+    </row>
+    <row r="413" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G413" s="50"/>
+    </row>
+    <row r="414" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G414" s="50"/>
+    </row>
+    <row r="415" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G415" s="50"/>
+    </row>
+    <row r="416" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G416" s="50"/>
+    </row>
+    <row r="417" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G417" s="50"/>
+    </row>
+    <row r="418" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G418" s="50"/>
+    </row>
+    <row r="419" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G419" s="50"/>
+    </row>
+    <row r="420" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G420" s="50"/>
+    </row>
+    <row r="421" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G421" s="50"/>
+    </row>
+    <row r="422" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G422" s="50"/>
+    </row>
+    <row r="423" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G423" s="50"/>
+    </row>
+    <row r="424" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G424" s="50"/>
+    </row>
+    <row r="425" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G425" s="50"/>
+    </row>
+    <row r="426" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G426" s="50"/>
+    </row>
+    <row r="427" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G427" s="50"/>
+    </row>
+    <row r="428" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G428" s="50"/>
+    </row>
+    <row r="429" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G429" s="50"/>
+    </row>
+    <row r="430" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G430" s="50"/>
+    </row>
+    <row r="431" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G431" s="50"/>
+    </row>
+    <row r="432" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G432" s="50"/>
+    </row>
+    <row r="433" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G433" s="50"/>
+    </row>
+    <row r="434" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G434" s="50"/>
+    </row>
+    <row r="435" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G435" s="50"/>
+    </row>
+    <row r="436" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G436" s="50"/>
+    </row>
+    <row r="437" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G437" s="50"/>
+    </row>
+    <row r="438" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G438" s="50"/>
+    </row>
+    <row r="439" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G439" s="50"/>
+    </row>
+    <row r="440" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G440" s="50"/>
+    </row>
+    <row r="441" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G441" s="50"/>
+    </row>
+    <row r="442" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G442" s="50"/>
+    </row>
+    <row r="443" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G443" s="50"/>
+    </row>
+    <row r="444" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G444" s="50"/>
+    </row>
+    <row r="445" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G445" s="50"/>
+    </row>
+    <row r="446" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G446" s="50"/>
+    </row>
+    <row r="447" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G447" s="50"/>
+    </row>
+    <row r="448" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G448" s="50"/>
+    </row>
+    <row r="449" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G449" s="50"/>
+    </row>
+    <row r="450" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G450" s="50"/>
+    </row>
+    <row r="451" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G451" s="50"/>
+    </row>
+    <row r="452" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G452" s="50"/>
+    </row>
+    <row r="453" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G453" s="50"/>
+    </row>
+    <row r="454" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G454" s="50"/>
+    </row>
+    <row r="455" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G455" s="50"/>
+    </row>
+    <row r="456" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G456" s="50"/>
+    </row>
+    <row r="457" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G457" s="50"/>
+    </row>
+    <row r="458" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G458" s="50"/>
+    </row>
+    <row r="459" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G459" s="50"/>
+    </row>
+    <row r="460" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G460" s="50"/>
+    </row>
+    <row r="461" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G461" s="50"/>
+    </row>
+    <row r="462" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G462" s="50"/>
+    </row>
+    <row r="463" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G463" s="50"/>
+    </row>
+    <row r="464" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G464" s="50"/>
+    </row>
+    <row r="465" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G465" s="50"/>
+    </row>
+    <row r="466" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G466" s="50"/>
+    </row>
+    <row r="467" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G467" s="50"/>
+    </row>
+    <row r="468" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G468" s="50"/>
+    </row>
+    <row r="469" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G469" s="50"/>
+    </row>
+    <row r="470" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G470" s="50"/>
+    </row>
+    <row r="471" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G471" s="50"/>
+    </row>
+    <row r="472" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G472" s="50"/>
+    </row>
+    <row r="473" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G473" s="50"/>
+    </row>
+    <row r="474" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G474" s="50"/>
+    </row>
+    <row r="475" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G475" s="50"/>
+    </row>
+    <row r="476" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G476" s="50"/>
+    </row>
+    <row r="477" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G477" s="50"/>
+    </row>
+    <row r="478" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G478" s="50"/>
+    </row>
+    <row r="479" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G479" s="50"/>
+    </row>
+    <row r="480" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G480" s="50"/>
+    </row>
+    <row r="481" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G481" s="50"/>
+    </row>
+    <row r="482" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G482" s="50"/>
+    </row>
+    <row r="483" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G483" s="50"/>
+    </row>
+    <row r="484" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G484" s="50"/>
+    </row>
+    <row r="485" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G485" s="50"/>
+    </row>
+    <row r="486" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G486" s="50"/>
+    </row>
+    <row r="487" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G487" s="50"/>
+    </row>
+    <row r="488" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G488" s="50"/>
+    </row>
+    <row r="489" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G489" s="50"/>
+    </row>
+    <row r="490" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G490" s="50"/>
+    </row>
+    <row r="491" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G491" s="50"/>
+    </row>
+    <row r="492" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G492" s="50"/>
+    </row>
+    <row r="493" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G493" s="50"/>
+    </row>
+    <row r="494" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G494" s="50"/>
+    </row>
+    <row r="495" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G495" s="50"/>
+    </row>
+    <row r="496" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G496" s="50"/>
+    </row>
+    <row r="497" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G497" s="50"/>
+    </row>
+    <row r="498" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G498" s="50"/>
+    </row>
+    <row r="499" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G499" s="50"/>
+    </row>
+    <row r="500" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G500" s="50"/>
+    </row>
+    <row r="501" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G501" s="50"/>
+    </row>
+    <row r="502" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G502" s="50"/>
+    </row>
+    <row r="503" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G503" s="50"/>
+    </row>
+    <row r="504" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G504" s="50"/>
+    </row>
+    <row r="505" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G505" s="50"/>
+    </row>
+    <row r="506" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G506" s="50"/>
+    </row>
+    <row r="507" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G507" s="50"/>
+    </row>
+    <row r="508" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G508" s="50"/>
+    </row>
+    <row r="509" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G509" s="50"/>
+    </row>
+    <row r="510" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G510" s="50"/>
+    </row>
+    <row r="511" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G511" s="50"/>
+    </row>
+    <row r="512" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G512" s="50"/>
+    </row>
+    <row r="513" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G513" s="50"/>
+    </row>
+    <row r="514" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G514" s="50"/>
+    </row>
+    <row r="515" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G515" s="50"/>
+    </row>
+    <row r="516" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G516" s="50"/>
+    </row>
+    <row r="517" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G517" s="50"/>
+    </row>
+    <row r="518" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G518" s="50"/>
+    </row>
+    <row r="519" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G519" s="50"/>
+    </row>
+    <row r="520" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G520" s="50"/>
+    </row>
+    <row r="521" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G521" s="50"/>
+    </row>
+    <row r="522" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G522" s="50"/>
+    </row>
+    <row r="523" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G523" s="50"/>
+    </row>
+    <row r="524" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G524" s="50"/>
+    </row>
+    <row r="525" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G525" s="50"/>
+    </row>
+    <row r="526" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G526" s="50"/>
+    </row>
+    <row r="527" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G527" s="50"/>
+    </row>
+    <row r="528" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G528" s="50"/>
+    </row>
+    <row r="529" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G529" s="50"/>
+    </row>
+    <row r="530" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G530" s="50"/>
+    </row>
+    <row r="531" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G531" s="50"/>
+    </row>
+    <row r="532" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G532" s="50"/>
+    </row>
+    <row r="533" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G533" s="50"/>
+    </row>
+    <row r="534" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G534" s="50"/>
+    </row>
+    <row r="535" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G535" s="50"/>
+    </row>
+    <row r="536" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G536" s="50"/>
+    </row>
+    <row r="537" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G537" s="50"/>
+    </row>
+    <row r="538" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G538" s="50"/>
+    </row>
+    <row r="539" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G539" s="50"/>
+    </row>
+    <row r="540" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G540" s="50"/>
+    </row>
+    <row r="541" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G541" s="50"/>
+    </row>
+    <row r="542" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G542" s="50"/>
+    </row>
+    <row r="543" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G543" s="50"/>
+    </row>
+    <row r="544" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G544" s="50"/>
+    </row>
+    <row r="545" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G545" s="50"/>
+    </row>
+    <row r="546" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G546" s="50"/>
+    </row>
+    <row r="547" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G547" s="50"/>
+    </row>
+    <row r="548" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G548" s="50"/>
+    </row>
+    <row r="549" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G549" s="50"/>
+    </row>
+    <row r="550" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G550" s="50"/>
+    </row>
+    <row r="551" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G551" s="50"/>
+    </row>
+    <row r="552" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G552" s="50"/>
+    </row>
+    <row r="553" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G553" s="50"/>
+    </row>
+    <row r="554" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G554" s="50"/>
+    </row>
+    <row r="555" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G555" s="50"/>
+    </row>
+    <row r="556" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G556" s="50"/>
+    </row>
+    <row r="557" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G557" s="50"/>
+    </row>
+    <row r="558" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G558" s="50"/>
+    </row>
+    <row r="559" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G559" s="50"/>
+    </row>
+    <row r="560" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G560" s="50"/>
+    </row>
+    <row r="561" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G561" s="50"/>
+    </row>
+    <row r="562" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G562" s="50"/>
+    </row>
+    <row r="563" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G563" s="50"/>
+    </row>
+    <row r="564" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G564" s="50"/>
+    </row>
+    <row r="565" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G565" s="50"/>
+    </row>
+    <row r="566" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G566" s="50"/>
+    </row>
+    <row r="567" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G567" s="50"/>
+    </row>
+    <row r="568" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G568" s="50"/>
+    </row>
+    <row r="569" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G569" s="50"/>
+    </row>
+    <row r="570" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G570" s="50"/>
+    </row>
+    <row r="571" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G571" s="50"/>
+    </row>
+    <row r="572" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G572" s="50"/>
+    </row>
+    <row r="573" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G573" s="50"/>
+    </row>
+    <row r="574" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G574" s="50"/>
+    </row>
+    <row r="575" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G575" s="50"/>
+    </row>
+    <row r="576" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G576" s="50"/>
+    </row>
+    <row r="577" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G577" s="50"/>
+    </row>
+    <row r="578" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G578" s="50"/>
+    </row>
+    <row r="579" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G579" s="50"/>
+    </row>
+    <row r="580" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G580" s="50"/>
+    </row>
+    <row r="581" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G581" s="50"/>
+    </row>
+    <row r="582" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G582" s="50"/>
+    </row>
+    <row r="583" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G583" s="50"/>
+    </row>
+    <row r="584" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G584" s="50"/>
+    </row>
+    <row r="585" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G585" s="50"/>
+    </row>
+    <row r="586" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G586" s="50"/>
+    </row>
+    <row r="587" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G587" s="50"/>
+    </row>
+    <row r="588" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G588" s="50"/>
+    </row>
+    <row r="589" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G589" s="50"/>
+    </row>
+    <row r="590" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G590" s="50"/>
+    </row>
+    <row r="591" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G591" s="50"/>
+    </row>
+    <row r="592" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G592" s="50"/>
+    </row>
+    <row r="593" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G593" s="50"/>
+    </row>
+    <row r="594" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G594" s="50"/>
+    </row>
+    <row r="595" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G595" s="50"/>
+    </row>
+    <row r="596" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G596" s="50"/>
+    </row>
+    <row r="597" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G597" s="50"/>
+    </row>
+    <row r="598" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G598" s="50"/>
+    </row>
+    <row r="599" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G599" s="50"/>
+    </row>
+    <row r="600" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G600" s="50"/>
+    </row>
+    <row r="601" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G601" s="50"/>
+    </row>
+    <row r="602" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G602" s="50"/>
+    </row>
+    <row r="603" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G603" s="50"/>
+    </row>
+    <row r="604" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G604" s="50"/>
+    </row>
+    <row r="605" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G605" s="50"/>
+    </row>
+    <row r="606" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G606" s="50"/>
+    </row>
+    <row r="607" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G607" s="50"/>
+    </row>
+    <row r="608" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G608" s="50"/>
+    </row>
+    <row r="609" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G609" s="50"/>
+    </row>
+    <row r="610" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G610" s="50"/>
+    </row>
+    <row r="611" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G611" s="50"/>
+    </row>
+    <row r="612" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G612" s="50"/>
+    </row>
+    <row r="613" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G613" s="50"/>
+    </row>
+    <row r="614" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G614" s="50"/>
+    </row>
+    <row r="615" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G615" s="50"/>
+    </row>
+    <row r="616" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G616" s="50"/>
+    </row>
+    <row r="617" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G617" s="50"/>
+    </row>
+    <row r="618" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G618" s="50"/>
+    </row>
+    <row r="619" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G619" s="50"/>
+    </row>
+    <row r="620" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G620" s="50"/>
+    </row>
+    <row r="621" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G621" s="50"/>
+    </row>
+    <row r="622" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G622" s="50"/>
+    </row>
+    <row r="623" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G623" s="50"/>
+    </row>
+    <row r="624" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G624" s="50"/>
+    </row>
+    <row r="625" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G625" s="50"/>
+    </row>
+    <row r="626" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G626" s="50"/>
+    </row>
+    <row r="627" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G627" s="50"/>
+    </row>
+    <row r="628" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G628" s="50"/>
+    </row>
+    <row r="629" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G629" s="50"/>
+    </row>
+    <row r="630" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G630" s="50"/>
+    </row>
+    <row r="631" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G631" s="50"/>
+    </row>
+    <row r="632" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G632" s="50"/>
+    </row>
+    <row r="633" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G633" s="50"/>
+    </row>
+    <row r="634" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G634" s="50"/>
+    </row>
+    <row r="635" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G635" s="50"/>
+    </row>
+    <row r="636" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G636" s="50"/>
+    </row>
+    <row r="637" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G637" s="50"/>
+    </row>
+    <row r="638" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G638" s="50"/>
+    </row>
+    <row r="639" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G639" s="50"/>
+    </row>
+    <row r="640" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G640" s="50"/>
+    </row>
+    <row r="641" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G641" s="50"/>
+    </row>
+    <row r="642" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G642" s="50"/>
+    </row>
+    <row r="643" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G643" s="50"/>
+    </row>
+    <row r="644" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G644" s="50"/>
+    </row>
+    <row r="645" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G645" s="50"/>
+    </row>
+    <row r="646" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G646" s="50"/>
+    </row>
+    <row r="647" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G647" s="50"/>
+    </row>
+    <row r="648" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G648" s="50"/>
+    </row>
+    <row r="649" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G649" s="50"/>
+    </row>
+    <row r="650" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G650" s="50"/>
+    </row>
+    <row r="651" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G651" s="50"/>
+    </row>
+    <row r="652" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G652" s="50"/>
+    </row>
+    <row r="653" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G653" s="50"/>
+    </row>
+    <row r="654" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G654" s="50"/>
+    </row>
+    <row r="655" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G655" s="50"/>
+    </row>
+    <row r="656" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G656" s="50"/>
+    </row>
+    <row r="657" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G657" s="50"/>
+    </row>
+    <row r="658" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G658" s="50"/>
+    </row>
+    <row r="659" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G659" s="50"/>
+    </row>
+    <row r="660" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G660" s="50"/>
+    </row>
+    <row r="661" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G661" s="50"/>
+    </row>
+    <row r="662" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G662" s="50"/>
+    </row>
+    <row r="663" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G663" s="50"/>
+    </row>
+    <row r="664" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G664" s="50"/>
+    </row>
+    <row r="665" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G665" s="50"/>
+    </row>
+    <row r="666" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G666" s="50"/>
+    </row>
+    <row r="667" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G667" s="50"/>
+    </row>
+    <row r="668" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G668" s="50"/>
+    </row>
+    <row r="669" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G669" s="50"/>
+    </row>
+    <row r="670" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G670" s="50"/>
+    </row>
+    <row r="671" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G671" s="50"/>
+    </row>
+    <row r="672" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G672" s="50"/>
+    </row>
+    <row r="673" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G673" s="50"/>
+    </row>
+    <row r="674" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G674" s="50"/>
+    </row>
+    <row r="675" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G675" s="50"/>
+    </row>
+    <row r="676" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G676" s="50"/>
+    </row>
+    <row r="677" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G677" s="50"/>
+    </row>
+    <row r="678" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G678" s="50"/>
+    </row>
+    <row r="679" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G679" s="50"/>
+    </row>
+    <row r="680" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G680" s="50"/>
+    </row>
+    <row r="681" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G681" s="50"/>
+    </row>
+    <row r="682" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G682" s="50"/>
+    </row>
+    <row r="683" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G683" s="50"/>
+    </row>
+    <row r="684" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G684" s="50"/>
+    </row>
+    <row r="685" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G685" s="50"/>
+    </row>
+    <row r="686" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G686" s="50"/>
+    </row>
+    <row r="687" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G687" s="50"/>
+    </row>
+    <row r="688" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G688" s="50"/>
+    </row>
+    <row r="689" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G689" s="50"/>
+    </row>
+    <row r="690" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G690" s="50"/>
+    </row>
+    <row r="691" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G691" s="50"/>
+    </row>
+    <row r="692" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G692" s="50"/>
+    </row>
+    <row r="693" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G693" s="50"/>
+    </row>
+    <row r="694" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G694" s="50"/>
+    </row>
+    <row r="695" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G695" s="50"/>
+    </row>
+    <row r="696" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G696" s="50"/>
+    </row>
+    <row r="697" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G697" s="50"/>
+    </row>
+    <row r="698" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G698" s="50"/>
+    </row>
+    <row r="699" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G699" s="50"/>
+    </row>
+    <row r="700" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G700" s="50"/>
+    </row>
+    <row r="701" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G701" s="50"/>
+    </row>
+    <row r="702" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G702" s="50"/>
+    </row>
+    <row r="703" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G703" s="50"/>
+    </row>
+    <row r="704" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G704" s="50"/>
+    </row>
+    <row r="705" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G705" s="50"/>
+    </row>
+    <row r="706" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G706" s="50"/>
+    </row>
+    <row r="707" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G707" s="50"/>
+    </row>
+    <row r="708" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G708" s="50"/>
+    </row>
+    <row r="709" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G709" s="50"/>
+    </row>
+    <row r="710" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G710" s="50"/>
+    </row>
+    <row r="711" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G711" s="50"/>
+    </row>
+    <row r="712" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G712" s="50"/>
+    </row>
+    <row r="713" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G713" s="50"/>
+    </row>
+    <row r="714" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G714" s="50"/>
+    </row>
+    <row r="715" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G715" s="50"/>
+    </row>
+    <row r="716" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G716" s="50"/>
+    </row>
+    <row r="717" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G717" s="50"/>
+    </row>
+    <row r="718" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G718" s="50"/>
+    </row>
+    <row r="719" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G719" s="50"/>
+    </row>
+    <row r="720" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G720" s="50"/>
+    </row>
+    <row r="721" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G721" s="50"/>
+    </row>
+    <row r="722" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G722" s="50"/>
+    </row>
+    <row r="723" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G723" s="50"/>
+    </row>
+    <row r="724" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G724" s="50"/>
+    </row>
+    <row r="725" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G725" s="50"/>
+    </row>
+    <row r="726" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G726" s="50"/>
+    </row>
+    <row r="727" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G727" s="50"/>
+    </row>
+    <row r="728" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G728" s="50"/>
+    </row>
+    <row r="729" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G729" s="50"/>
+    </row>
+    <row r="730" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G730" s="50"/>
+    </row>
+    <row r="731" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G731" s="50"/>
+    </row>
+    <row r="732" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G732" s="50"/>
+    </row>
+    <row r="733" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G733" s="50"/>
+    </row>
+    <row r="734" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G734" s="50"/>
+    </row>
+    <row r="735" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G735" s="50"/>
+    </row>
+    <row r="736" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G736" s="50"/>
+    </row>
+    <row r="737" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G737" s="50"/>
+    </row>
+    <row r="738" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G738" s="50"/>
+    </row>
+    <row r="739" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G739" s="50"/>
+    </row>
+    <row r="740" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G740" s="50"/>
+    </row>
+    <row r="741" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G741" s="50"/>
+    </row>
+    <row r="742" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G742" s="50"/>
+    </row>
+    <row r="743" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G743" s="50"/>
+    </row>
+    <row r="744" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G744" s="50"/>
+    </row>
+    <row r="745" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G745" s="50"/>
+    </row>
+    <row r="746" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G746" s="50"/>
+    </row>
+    <row r="747" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G747" s="50"/>
+    </row>
+    <row r="748" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G748" s="50"/>
+    </row>
+    <row r="749" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G749" s="50"/>
+    </row>
+    <row r="750" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G750" s="50"/>
+    </row>
+    <row r="751" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G751" s="50"/>
+    </row>
+    <row r="752" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G752" s="50"/>
+    </row>
+    <row r="753" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G753" s="50"/>
+    </row>
+    <row r="754" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G754" s="50"/>
+    </row>
+    <row r="755" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G755" s="50"/>
+    </row>
+    <row r="756" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G756" s="50"/>
+    </row>
+    <row r="757" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G757" s="50"/>
+    </row>
+    <row r="758" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G758" s="50"/>
+    </row>
+    <row r="759" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G759" s="50"/>
+    </row>
+    <row r="760" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G760" s="50"/>
+    </row>
+    <row r="761" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G761" s="50"/>
+    </row>
+    <row r="762" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G762" s="50"/>
+    </row>
+    <row r="763" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G763" s="50"/>
+    </row>
+    <row r="764" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G764" s="50"/>
+    </row>
+    <row r="765" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G765" s="50"/>
+    </row>
+    <row r="766" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G766" s="50"/>
+    </row>
+    <row r="767" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G767" s="50"/>
+    </row>
+    <row r="768" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G768" s="50"/>
+    </row>
+    <row r="769" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G769" s="50"/>
+    </row>
+    <row r="770" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G770" s="50"/>
+    </row>
+    <row r="771" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G771" s="50"/>
+    </row>
+    <row r="772" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G772" s="50"/>
+    </row>
+    <row r="773" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G773" s="50"/>
+    </row>
+    <row r="774" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G774" s="50"/>
+    </row>
+    <row r="775" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G775" s="50"/>
+    </row>
+    <row r="776" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G776" s="50"/>
+    </row>
+    <row r="777" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G777" s="50"/>
+    </row>
+    <row r="778" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G778" s="50"/>
+    </row>
+    <row r="779" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G779" s="50"/>
+    </row>
+    <row r="780" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G780" s="50"/>
+    </row>
+    <row r="781" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G781" s="50"/>
+    </row>
+    <row r="782" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G782" s="50"/>
+    </row>
+    <row r="783" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G783" s="50"/>
+    </row>
+    <row r="784" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G784" s="50"/>
+    </row>
+    <row r="785" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G785" s="50"/>
+    </row>
+    <row r="786" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G786" s="50"/>
+    </row>
+    <row r="787" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G787" s="50"/>
+    </row>
+    <row r="788" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G788" s="50"/>
+    </row>
+    <row r="789" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G789" s="50"/>
+    </row>
+    <row r="790" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G790" s="50"/>
+    </row>
+    <row r="791" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G791" s="50"/>
+    </row>
+    <row r="792" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G792" s="50"/>
+    </row>
+    <row r="793" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G793" s="50"/>
+    </row>
+    <row r="794" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G794" s="50"/>
+    </row>
+    <row r="795" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G795" s="50"/>
+    </row>
+    <row r="796" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G796" s="50"/>
+    </row>
+    <row r="797" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G797" s="50"/>
+    </row>
+    <row r="798" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G798" s="50"/>
+    </row>
+    <row r="799" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G799" s="50"/>
+    </row>
+    <row r="800" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G800" s="50"/>
+    </row>
+    <row r="801" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G801" s="50"/>
+    </row>
+    <row r="802" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G802" s="50"/>
+    </row>
+    <row r="803" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G803" s="50"/>
+    </row>
+    <row r="804" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G804" s="50"/>
+    </row>
+    <row r="805" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G805" s="50"/>
+    </row>
+    <row r="806" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G806" s="50"/>
+    </row>
+    <row r="807" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G807" s="50"/>
+    </row>
+    <row r="808" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G808" s="50"/>
+    </row>
+    <row r="809" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G809" s="50"/>
+    </row>
+    <row r="810" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G810" s="50"/>
+    </row>
+    <row r="811" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G811" s="50"/>
+    </row>
+    <row r="812" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G812" s="50"/>
+    </row>
+    <row r="813" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G813" s="50"/>
+    </row>
+    <row r="814" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G814" s="50"/>
+    </row>
+    <row r="815" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G815" s="50"/>
+    </row>
+    <row r="816" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G816" s="50"/>
+    </row>
+    <row r="817" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G817" s="50"/>
+    </row>
+    <row r="818" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G818" s="50"/>
+    </row>
+    <row r="819" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G819" s="50"/>
+    </row>
+    <row r="820" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G820" s="50"/>
+    </row>
+    <row r="821" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G821" s="50"/>
+    </row>
+    <row r="822" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G822" s="50"/>
+    </row>
+    <row r="823" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G823" s="50"/>
+    </row>
+    <row r="824" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G824" s="50"/>
+    </row>
+    <row r="825" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G825" s="50"/>
+    </row>
+    <row r="826" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G826" s="50"/>
+    </row>
+    <row r="827" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G827" s="50"/>
+    </row>
+    <row r="828" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G828" s="50"/>
+    </row>
+    <row r="829" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G829" s="50"/>
+    </row>
+    <row r="830" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G830" s="50"/>
+    </row>
+    <row r="831" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G831" s="50"/>
+    </row>
+    <row r="832" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G832" s="50"/>
+    </row>
+    <row r="833" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G833" s="50"/>
+    </row>
+    <row r="834" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G834" s="50"/>
+    </row>
+    <row r="835" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G835" s="50"/>
+    </row>
+    <row r="836" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G836" s="50"/>
+    </row>
+    <row r="837" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G837" s="50"/>
+    </row>
+    <row r="838" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G838" s="50"/>
+    </row>
+    <row r="839" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G839" s="50"/>
+    </row>
+    <row r="840" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G840" s="50"/>
+    </row>
+    <row r="841" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G841" s="50"/>
+    </row>
+    <row r="842" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G842" s="50"/>
+    </row>
+    <row r="843" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G843" s="50"/>
+    </row>
+    <row r="844" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G844" s="50"/>
+    </row>
+    <row r="845" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G845" s="50"/>
+    </row>
+    <row r="846" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G846" s="50"/>
+    </row>
+    <row r="847" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G847" s="50"/>
+    </row>
+    <row r="848" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G848" s="50"/>
+    </row>
+    <row r="849" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G849" s="50"/>
+    </row>
+    <row r="850" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G850" s="50"/>
+    </row>
+    <row r="851" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G851" s="50"/>
+    </row>
+    <row r="852" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G852" s="50"/>
+    </row>
+    <row r="853" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G853" s="50"/>
+    </row>
+    <row r="854" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G854" s="50"/>
+    </row>
+    <row r="855" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G855" s="50"/>
+    </row>
+    <row r="856" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G856" s="50"/>
+    </row>
+    <row r="857" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G857" s="50"/>
+    </row>
+    <row r="858" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G858" s="50"/>
+    </row>
+    <row r="859" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G859" s="50"/>
+    </row>
+    <row r="860" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G860" s="50"/>
+    </row>
+    <row r="861" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G861" s="50"/>
+    </row>
+    <row r="862" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G862" s="50"/>
+    </row>
+    <row r="863" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G863" s="50"/>
+    </row>
+    <row r="864" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G864" s="50"/>
+    </row>
+    <row r="865" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G865" s="50"/>
+    </row>
+    <row r="866" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G866" s="50"/>
+    </row>
+    <row r="867" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G867" s="50"/>
+    </row>
+    <row r="868" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G868" s="50"/>
+    </row>
+    <row r="869" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G869" s="50"/>
+    </row>
+    <row r="870" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G870" s="50"/>
+    </row>
+    <row r="871" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G871" s="50"/>
+    </row>
+    <row r="872" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G872" s="50"/>
+    </row>
+    <row r="873" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G873" s="50"/>
+    </row>
+    <row r="874" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G874" s="50"/>
+    </row>
+    <row r="875" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G875" s="50"/>
+    </row>
+    <row r="876" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G876" s="50"/>
+    </row>
+    <row r="877" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G877" s="50"/>
+    </row>
+    <row r="878" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G878" s="50"/>
+    </row>
+    <row r="879" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G879" s="50"/>
+    </row>
+    <row r="880" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G880" s="50"/>
+    </row>
+    <row r="881" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G881" s="50"/>
+    </row>
+    <row r="882" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G882" s="50"/>
+    </row>
+    <row r="883" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G883" s="50"/>
+    </row>
+    <row r="884" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G884" s="50"/>
+    </row>
+    <row r="885" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G885" s="50"/>
+    </row>
+    <row r="886" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G886" s="50"/>
+    </row>
+    <row r="887" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G887" s="50"/>
+    </row>
+    <row r="888" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G888" s="50"/>
+    </row>
+    <row r="889" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G889" s="50"/>
+    </row>
+    <row r="890" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G890" s="50"/>
+    </row>
+    <row r="891" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G891" s="50"/>
+    </row>
+    <row r="892" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G892" s="50"/>
+    </row>
+    <row r="893" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G893" s="50"/>
+    </row>
+    <row r="894" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G894" s="50"/>
+    </row>
+    <row r="895" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G895" s="50"/>
+    </row>
+    <row r="896" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G896" s="50"/>
+    </row>
+    <row r="897" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G897" s="50"/>
+    </row>
+    <row r="898" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G898" s="50"/>
+    </row>
+    <row r="899" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G899" s="50"/>
+    </row>
+    <row r="900" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G900" s="50"/>
+    </row>
+    <row r="901" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G901" s="50"/>
+    </row>
+    <row r="902" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G902" s="50"/>
+    </row>
+    <row r="903" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G903" s="50"/>
+    </row>
+    <row r="904" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G904" s="50"/>
+    </row>
+    <row r="905" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G905" s="50"/>
+    </row>
+    <row r="906" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G906" s="50"/>
+    </row>
+    <row r="907" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G907" s="50"/>
+    </row>
+    <row r="908" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G908" s="50"/>
+    </row>
+    <row r="909" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G909" s="50"/>
+    </row>
+    <row r="910" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G910" s="50"/>
+    </row>
+    <row r="911" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G911" s="50"/>
+    </row>
+    <row r="912" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G912" s="50"/>
+    </row>
+    <row r="913" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G913" s="50"/>
+    </row>
+    <row r="914" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G914" s="50"/>
+    </row>
+    <row r="915" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G915" s="50"/>
+    </row>
+    <row r="916" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G916" s="50"/>
+    </row>
+    <row r="917" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G917" s="50"/>
+    </row>
+    <row r="918" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G918" s="50"/>
+    </row>
+    <row r="919" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G919" s="50"/>
+    </row>
+    <row r="920" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G920" s="50"/>
+    </row>
+    <row r="921" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G921" s="50"/>
+    </row>
+    <row r="922" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G922" s="50"/>
+    </row>
+    <row r="923" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G923" s="50"/>
+    </row>
+    <row r="924" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G924" s="50"/>
+    </row>
+    <row r="925" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G925" s="50"/>
+    </row>
+    <row r="926" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G926" s="50"/>
+    </row>
+    <row r="927" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G927" s="50"/>
+    </row>
+    <row r="928" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G928" s="50"/>
+    </row>
+    <row r="929" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G929" s="50"/>
+    </row>
+    <row r="930" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G930" s="50"/>
+    </row>
+    <row r="931" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G931" s="50"/>
+    </row>
+    <row r="932" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G932" s="50"/>
+    </row>
+    <row r="933" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G933" s="50"/>
+    </row>
+    <row r="934" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G934" s="50"/>
+    </row>
+    <row r="935" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G935" s="50"/>
+    </row>
+    <row r="936" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G936" s="50"/>
+    </row>
+    <row r="937" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G937" s="50"/>
+    </row>
+    <row r="938" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G938" s="50"/>
+    </row>
+    <row r="939" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G939" s="50"/>
+    </row>
+    <row r="940" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G940" s="50"/>
+    </row>
+    <row r="941" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G941" s="50"/>
+    </row>
+    <row r="942" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G942" s="50"/>
+    </row>
+    <row r="943" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G943" s="50"/>
+    </row>
+    <row r="944" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G944" s="50"/>
+    </row>
+    <row r="945" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G945" s="50"/>
+    </row>
+    <row r="946" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G946" s="50"/>
+    </row>
+    <row r="947" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G947" s="50"/>
+    </row>
+    <row r="948" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G948" s="50"/>
+    </row>
+    <row r="949" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G949" s="50"/>
+    </row>
+    <row r="950" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G950" s="50"/>
+    </row>
+    <row r="951" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G951" s="50"/>
+    </row>
+    <row r="952" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G952" s="50"/>
+    </row>
+    <row r="953" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G953" s="50"/>
+    </row>
+    <row r="954" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G954" s="50"/>
+    </row>
+    <row r="955" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G955" s="50"/>
+    </row>
+    <row r="956" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G956" s="50"/>
+    </row>
+    <row r="957" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G957" s="50"/>
+    </row>
+    <row r="958" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G958" s="50"/>
+    </row>
+    <row r="959" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G959" s="50"/>
+    </row>
+    <row r="960" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G960" s="50"/>
+    </row>
+    <row r="961" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G961" s="50"/>
+    </row>
+    <row r="962" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G962" s="50"/>
+    </row>
+    <row r="963" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G963" s="50"/>
+    </row>
+    <row r="964" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G964" s="50"/>
+    </row>
+    <row r="965" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G965" s="50"/>
+    </row>
+    <row r="966" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G966" s="50"/>
+    </row>
+    <row r="967" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G967" s="50"/>
+    </row>
+    <row r="968" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G968" s="50"/>
+    </row>
+    <row r="969" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G969" s="50"/>
+    </row>
+    <row r="970" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G970" s="50"/>
+    </row>
+    <row r="971" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G971" s="50"/>
+    </row>
+    <row r="972" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G972" s="50"/>
+    </row>
+    <row r="973" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G973" s="50"/>
+    </row>
+    <row r="974" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G974" s="50"/>
+    </row>
+    <row r="975" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G975" s="50"/>
+    </row>
+    <row r="976" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G976" s="50"/>
+    </row>
+    <row r="977" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G977" s="50"/>
+    </row>
+    <row r="978" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G978" s="50"/>
+    </row>
+    <row r="979" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G979" s="50"/>
+    </row>
+    <row r="980" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G980" s="50"/>
+    </row>
+    <row r="981" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G981" s="50"/>
+    </row>
+    <row r="982" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G982" s="50"/>
+    </row>
+    <row r="983" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G983" s="50"/>
+    </row>
+    <row r="984" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G984" s="50"/>
+    </row>
+    <row r="985" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G985" s="50"/>
+    </row>
+    <row r="986" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G986" s="50"/>
+    </row>
+    <row r="987" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G987" s="50"/>
+    </row>
+    <row r="988" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G988" s="50"/>
+    </row>
+    <row r="989" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G989" s="50"/>
+    </row>
+    <row r="990" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G990" s="50"/>
+    </row>
+    <row r="991" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G991" s="50"/>
+    </row>
+    <row r="992" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G992" s="50"/>
+    </row>
+    <row r="993" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G993" s="50"/>
+    </row>
+    <row r="994" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G994" s="50"/>
+    </row>
+    <row r="995" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G995" s="50"/>
+    </row>
+    <row r="996" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G996" s="50"/>
+    </row>
+    <row r="997" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G997" s="50"/>
+    </row>
+    <row r="998" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G998" s="50"/>
+    </row>
+    <row r="999" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G999" s="50"/>
+    </row>
+    <row r="1000" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G1000" s="50"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>

</xml_diff>

<commit_message>
- Moved data source prefix and id info to Design in cases where I had altered the sequence - Cleared data source prefix but maintained id to reference the gb file in the directory. This needs review as it may not be the best approach, or the files may need to be renamed (human readable name?). - Deleted ky484012.gb from directory
</commit_message>
<xml_diff>
--- a/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
+++ b/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/Fluorescent Reporter Proteins/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Fluorescent Reporter Proteins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED12EE5-8A8C-1E4D-B629-5E469F1EA25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7137088-1816-BD4D-9428-B0C338163333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7669" uniqueCount="7571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7666" uniqueCount="7572">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22791,18 +22791,9 @@
     <t>includes barcode after double stop, 4 BbsI cut sites</t>
   </si>
   <si>
-    <t>Type IIS compatible version from Murray Lab</t>
-  </si>
-  <si>
     <t>Mammalia</t>
   </si>
   <si>
-    <t>Sequence was missing bases, but matched to repressilator</t>
-  </si>
-  <si>
-    <t>stop codons added</t>
-  </si>
-  <si>
     <t>Chlamydomonas reinhardtii</t>
   </si>
   <si>
@@ -22816,6 +22807,18 @@
   </si>
   <si>
     <t>Literal Part</t>
+  </si>
+  <si>
+    <t>Source: AddGene-26495 / Sequence was missing bases, but matched to repressilator</t>
+  </si>
+  <si>
+    <t>Source: AddGene-120957 / Type IIS compatible version from Murray Lab</t>
+  </si>
+  <si>
+    <t>Source: GenBank-KY021423 / stop codons added</t>
+  </si>
+  <si>
+    <t>Source: AddGene-54827</t>
   </si>
 </sst>
 </file>
@@ -23207,12 +23210,12 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23669,8 +23672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23740,12 +23743,12 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="49"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -23926,7 +23929,7 @@
       <c r="F13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="41" t="s">
         <v>19</v>
       </c>
       <c r="H13" s="6" t="s">
@@ -24035,7 +24038,7 @@
         <v>47</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>7564</v>
+        <v>7568</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>7445</v>
@@ -24043,9 +24046,7 @@
       <c r="E16" s="18" t="s">
         <v>7549</v>
       </c>
-      <c r="F16" s="18" t="s">
-        <v>7485</v>
-      </c>
+      <c r="F16" s="41"/>
       <c r="G16" s="41">
         <v>26495</v>
       </c>
@@ -24254,16 +24255,14 @@
       <c r="B22" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="18" t="s">
-        <v>7562</v>
+      <c r="C22" s="41" t="s">
+        <v>7569</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="18" t="s">
         <v>7551</v>
       </c>
-      <c r="F22" s="18" t="s">
-        <v>7485</v>
-      </c>
+      <c r="F22" s="41"/>
       <c r="G22" s="41">
         <v>120957</v>
       </c>
@@ -24291,7 +24290,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="41" t="s">
-        <v>7565</v>
+        <v>7570</v>
       </c>
       <c r="D23" s="20" t="s">
         <v>7445</v>
@@ -24299,17 +24298,15 @@
       <c r="E23" s="18" t="s">
         <v>7552</v>
       </c>
-      <c r="F23" s="18" t="s">
-        <v>7469</v>
-      </c>
+      <c r="F23" s="41"/>
       <c r="G23" s="41" t="s">
-        <v>7568</v>
+        <v>7565</v>
       </c>
       <c r="H23" s="18" t="s">
         <v>7417</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>7563</v>
+        <v>7562</v>
       </c>
       <c r="J23" s="18" t="b">
         <v>1</v>
@@ -24364,20 +24361,20 @@
       <c r="B25" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="18"/>
+      <c r="C25" s="41" t="s">
+        <v>7571</v>
+      </c>
       <c r="D25" s="20"/>
       <c r="E25" s="18" t="s">
         <v>7550</v>
       </c>
-      <c r="F25" s="41" t="s">
-        <v>7485</v>
-      </c>
+      <c r="F25" s="41"/>
       <c r="G25" s="46">
         <v>54827</v>
       </c>
       <c r="H25" s="18"/>
       <c r="I25" s="18" t="s">
-        <v>7569</v>
+        <v>7566</v>
       </c>
       <c r="J25" s="18" t="b">
         <v>1</v>
@@ -24513,13 +24510,13 @@
         <v>7469</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>7567</v>
+        <v>7564</v>
       </c>
       <c r="H29" s="18" t="s">
         <v>10</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>7566</v>
+        <v>7563</v>
       </c>
       <c r="J29" s="18" t="b">
         <v>1</v>
@@ -69404,7 +69401,7 @@
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1">
       <c r="A30" s="45" t="s">
-        <v>7563</v>
+        <v>7562</v>
       </c>
       <c r="B30" s="18">
         <v>40674</v>
@@ -69413,7 +69410,7 @@
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1">
       <c r="A31" s="45" t="s">
-        <v>7566</v>
+        <v>7563</v>
       </c>
       <c r="B31" s="18">
         <v>3055</v>
@@ -69422,7 +69419,7 @@
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1">
       <c r="A32" s="45" t="s">
-        <v>7569</v>
+        <v>7566</v>
       </c>
       <c r="B32" s="18">
         <v>8355</v>
@@ -72097,7 +72094,7 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
@@ -72133,7 +72130,7 @@
         <v>7467</v>
       </c>
       <c r="G1" s="33" t="s">
-        <v>7570</v>
+        <v>7567</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
@@ -72155,7 +72152,7 @@
       <c r="F2" s="38" t="s">
         <v>7473</v>
       </c>
-      <c r="G2" s="50" t="b">
+      <c r="G2" s="47" t="b">
         <v>1</v>
       </c>
     </row>
@@ -72178,7 +72175,7 @@
       <c r="F3" s="38" t="s">
         <v>7478</v>
       </c>
-      <c r="G3" s="50" t="b">
+      <c r="G3" s="47" t="b">
         <v>0</v>
       </c>
     </row>
@@ -72201,7 +72198,7 @@
       <c r="F4" s="38" t="s">
         <v>7483</v>
       </c>
-      <c r="G4" s="50" t="b">
+      <c r="G4" s="47" t="b">
         <v>1</v>
       </c>
     </row>
@@ -72224,7 +72221,7 @@
       <c r="F5" s="38" t="s">
         <v>7489</v>
       </c>
-      <c r="G5" s="50" t="b">
+      <c r="G5" s="47" t="b">
         <v>0</v>
       </c>
     </row>
@@ -72247,7 +72244,7 @@
       <c r="F6" s="38" t="s">
         <v>7494</v>
       </c>
-      <c r="G6" s="50" t="b">
+      <c r="G6" s="47" t="b">
         <v>1</v>
       </c>
     </row>
@@ -72270,7 +72267,7 @@
       <c r="F7" s="38" t="s">
         <v>7499</v>
       </c>
-      <c r="G7" s="50" t="b">
+      <c r="G7" s="47" t="b">
         <v>0</v>
       </c>
     </row>
@@ -72280,7 +72277,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="35"/>
-      <c r="G8" s="50"/>
+      <c r="G8" s="47"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="3"/>
@@ -72288,7 +72285,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="G9" s="50"/>
+      <c r="G9" s="47"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="3"/>
@@ -72296,7 +72293,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="G10" s="50"/>
+      <c r="G10" s="47"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="3"/>
@@ -72304,7 +72301,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="G11" s="50"/>
+      <c r="G11" s="47"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
@@ -72312,7 +72309,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="G12" s="50"/>
+      <c r="G12" s="47"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="3"/>
@@ -72320,7 +72317,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="G13" s="50"/>
+      <c r="G13" s="47"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="3"/>
@@ -72328,2965 +72325,2965 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="G14" s="50"/>
+      <c r="G14" s="47"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
-      <c r="G15" s="50"/>
+      <c r="G15" s="47"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
-      <c r="G16" s="50"/>
+      <c r="G16" s="47"/>
     </row>
     <row r="17" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G17" s="50"/>
+      <c r="G17" s="47"/>
     </row>
     <row r="18" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G18" s="50"/>
+      <c r="G18" s="47"/>
     </row>
     <row r="19" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G19" s="50"/>
+      <c r="G19" s="47"/>
     </row>
     <row r="20" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G20" s="50"/>
+      <c r="G20" s="47"/>
     </row>
     <row r="21" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G21" s="50"/>
+      <c r="G21" s="47"/>
     </row>
     <row r="22" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G22" s="50"/>
+      <c r="G22" s="47"/>
     </row>
     <row r="23" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G23" s="50"/>
+      <c r="G23" s="47"/>
     </row>
     <row r="24" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G24" s="50"/>
+      <c r="G24" s="47"/>
     </row>
     <row r="25" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G25" s="50"/>
+      <c r="G25" s="47"/>
     </row>
     <row r="26" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G26" s="50"/>
+      <c r="G26" s="47"/>
     </row>
     <row r="27" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G27" s="50"/>
+      <c r="G27" s="47"/>
     </row>
     <row r="28" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G28" s="50"/>
+      <c r="G28" s="47"/>
     </row>
     <row r="29" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G29" s="50"/>
+      <c r="G29" s="47"/>
     </row>
     <row r="30" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G30" s="50"/>
+      <c r="G30" s="47"/>
     </row>
     <row r="31" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G31" s="50"/>
+      <c r="G31" s="47"/>
     </row>
     <row r="32" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G32" s="50"/>
+      <c r="G32" s="47"/>
     </row>
     <row r="33" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G33" s="50"/>
+      <c r="G33" s="47"/>
     </row>
     <row r="34" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G34" s="50"/>
+      <c r="G34" s="47"/>
     </row>
     <row r="35" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G35" s="50"/>
+      <c r="G35" s="47"/>
     </row>
     <row r="36" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G36" s="50"/>
+      <c r="G36" s="47"/>
     </row>
     <row r="37" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G37" s="50"/>
+      <c r="G37" s="47"/>
     </row>
     <row r="38" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G38" s="50"/>
+      <c r="G38" s="47"/>
     </row>
     <row r="39" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G39" s="50"/>
+      <c r="G39" s="47"/>
     </row>
     <row r="40" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G40" s="50"/>
+      <c r="G40" s="47"/>
     </row>
     <row r="41" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G41" s="50"/>
+      <c r="G41" s="47"/>
     </row>
     <row r="42" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G42" s="50"/>
+      <c r="G42" s="47"/>
     </row>
     <row r="43" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G43" s="50"/>
+      <c r="G43" s="47"/>
     </row>
     <row r="44" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G44" s="50"/>
+      <c r="G44" s="47"/>
     </row>
     <row r="45" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G45" s="50"/>
+      <c r="G45" s="47"/>
     </row>
     <row r="46" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G46" s="50"/>
+      <c r="G46" s="47"/>
     </row>
     <row r="47" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G47" s="50"/>
+      <c r="G47" s="47"/>
     </row>
     <row r="48" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G48" s="50"/>
+      <c r="G48" s="47"/>
     </row>
     <row r="49" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G49" s="50"/>
+      <c r="G49" s="47"/>
     </row>
     <row r="50" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G50" s="50"/>
+      <c r="G50" s="47"/>
     </row>
     <row r="51" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G51" s="50"/>
+      <c r="G51" s="47"/>
     </row>
     <row r="52" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G52" s="50"/>
+      <c r="G52" s="47"/>
     </row>
     <row r="53" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G53" s="50"/>
+      <c r="G53" s="47"/>
     </row>
     <row r="54" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G54" s="50"/>
+      <c r="G54" s="47"/>
     </row>
     <row r="55" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G55" s="50"/>
+      <c r="G55" s="47"/>
     </row>
     <row r="56" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G56" s="50"/>
+      <c r="G56" s="47"/>
     </row>
     <row r="57" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G57" s="50"/>
+      <c r="G57" s="47"/>
     </row>
     <row r="58" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G58" s="50"/>
+      <c r="G58" s="47"/>
     </row>
     <row r="59" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G59" s="50"/>
+      <c r="G59" s="47"/>
     </row>
     <row r="60" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G60" s="50"/>
+      <c r="G60" s="47"/>
     </row>
     <row r="61" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G61" s="50"/>
+      <c r="G61" s="47"/>
     </row>
     <row r="62" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G62" s="50"/>
+      <c r="G62" s="47"/>
     </row>
     <row r="63" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G63" s="50"/>
+      <c r="G63" s="47"/>
     </row>
     <row r="64" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G64" s="50"/>
+      <c r="G64" s="47"/>
     </row>
     <row r="65" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G65" s="50"/>
+      <c r="G65" s="47"/>
     </row>
     <row r="66" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G66" s="50"/>
+      <c r="G66" s="47"/>
     </row>
     <row r="67" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G67" s="50"/>
+      <c r="G67" s="47"/>
     </row>
     <row r="68" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G68" s="50"/>
+      <c r="G68" s="47"/>
     </row>
     <row r="69" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G69" s="50"/>
+      <c r="G69" s="47"/>
     </row>
     <row r="70" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G70" s="50"/>
+      <c r="G70" s="47"/>
     </row>
     <row r="71" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G71" s="50"/>
+      <c r="G71" s="47"/>
     </row>
     <row r="72" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G72" s="50"/>
+      <c r="G72" s="47"/>
     </row>
     <row r="73" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G73" s="50"/>
+      <c r="G73" s="47"/>
     </row>
     <row r="74" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G74" s="50"/>
+      <c r="G74" s="47"/>
     </row>
     <row r="75" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G75" s="50"/>
+      <c r="G75" s="47"/>
     </row>
     <row r="76" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G76" s="50"/>
+      <c r="G76" s="47"/>
     </row>
     <row r="77" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G77" s="50"/>
+      <c r="G77" s="47"/>
     </row>
     <row r="78" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G78" s="50"/>
+      <c r="G78" s="47"/>
     </row>
     <row r="79" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G79" s="50"/>
+      <c r="G79" s="47"/>
     </row>
     <row r="80" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G80" s="50"/>
+      <c r="G80" s="47"/>
     </row>
     <row r="81" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G81" s="50"/>
+      <c r="G81" s="47"/>
     </row>
     <row r="82" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G82" s="50"/>
+      <c r="G82" s="47"/>
     </row>
     <row r="83" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G83" s="50"/>
+      <c r="G83" s="47"/>
     </row>
     <row r="84" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G84" s="50"/>
+      <c r="G84" s="47"/>
     </row>
     <row r="85" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G85" s="50"/>
+      <c r="G85" s="47"/>
     </row>
     <row r="86" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G86" s="50"/>
+      <c r="G86" s="47"/>
     </row>
     <row r="87" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G87" s="50"/>
+      <c r="G87" s="47"/>
     </row>
     <row r="88" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G88" s="50"/>
+      <c r="G88" s="47"/>
     </row>
     <row r="89" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G89" s="50"/>
+      <c r="G89" s="47"/>
     </row>
     <row r="90" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G90" s="50"/>
+      <c r="G90" s="47"/>
     </row>
     <row r="91" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G91" s="50"/>
+      <c r="G91" s="47"/>
     </row>
     <row r="92" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G92" s="50"/>
+      <c r="G92" s="47"/>
     </row>
     <row r="93" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G93" s="50"/>
+      <c r="G93" s="47"/>
     </row>
     <row r="94" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G94" s="50"/>
+      <c r="G94" s="47"/>
     </row>
     <row r="95" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G95" s="50"/>
+      <c r="G95" s="47"/>
     </row>
     <row r="96" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G96" s="50"/>
+      <c r="G96" s="47"/>
     </row>
     <row r="97" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G97" s="50"/>
+      <c r="G97" s="47"/>
     </row>
     <row r="98" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G98" s="50"/>
+      <c r="G98" s="47"/>
     </row>
     <row r="99" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G99" s="50"/>
+      <c r="G99" s="47"/>
     </row>
     <row r="100" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G100" s="50"/>
+      <c r="G100" s="47"/>
     </row>
     <row r="101" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G101" s="50"/>
+      <c r="G101" s="47"/>
     </row>
     <row r="102" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G102" s="50"/>
+      <c r="G102" s="47"/>
     </row>
     <row r="103" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G103" s="50"/>
+      <c r="G103" s="47"/>
     </row>
     <row r="104" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G104" s="50"/>
+      <c r="G104" s="47"/>
     </row>
     <row r="105" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G105" s="50"/>
+      <c r="G105" s="47"/>
     </row>
     <row r="106" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G106" s="50"/>
+      <c r="G106" s="47"/>
     </row>
     <row r="107" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G107" s="50"/>
+      <c r="G107" s="47"/>
     </row>
     <row r="108" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G108" s="50"/>
+      <c r="G108" s="47"/>
     </row>
     <row r="109" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G109" s="50"/>
+      <c r="G109" s="47"/>
     </row>
     <row r="110" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G110" s="50"/>
+      <c r="G110" s="47"/>
     </row>
     <row r="111" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G111" s="50"/>
+      <c r="G111" s="47"/>
     </row>
     <row r="112" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G112" s="50"/>
+      <c r="G112" s="47"/>
     </row>
     <row r="113" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G113" s="50"/>
+      <c r="G113" s="47"/>
     </row>
     <row r="114" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G114" s="50"/>
+      <c r="G114" s="47"/>
     </row>
     <row r="115" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G115" s="50"/>
+      <c r="G115" s="47"/>
     </row>
     <row r="116" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G116" s="50"/>
+      <c r="G116" s="47"/>
     </row>
     <row r="117" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G117" s="50"/>
+      <c r="G117" s="47"/>
     </row>
     <row r="118" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G118" s="50"/>
+      <c r="G118" s="47"/>
     </row>
     <row r="119" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G119" s="50"/>
+      <c r="G119" s="47"/>
     </row>
     <row r="120" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G120" s="50"/>
+      <c r="G120" s="47"/>
     </row>
     <row r="121" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G121" s="50"/>
+      <c r="G121" s="47"/>
     </row>
     <row r="122" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G122" s="50"/>
+      <c r="G122" s="47"/>
     </row>
     <row r="123" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G123" s="50"/>
+      <c r="G123" s="47"/>
     </row>
     <row r="124" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G124" s="50"/>
+      <c r="G124" s="47"/>
     </row>
     <row r="125" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G125" s="50"/>
+      <c r="G125" s="47"/>
     </row>
     <row r="126" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G126" s="50"/>
+      <c r="G126" s="47"/>
     </row>
     <row r="127" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G127" s="50"/>
+      <c r="G127" s="47"/>
     </row>
     <row r="128" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G128" s="50"/>
+      <c r="G128" s="47"/>
     </row>
     <row r="129" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G129" s="50"/>
+      <c r="G129" s="47"/>
     </row>
     <row r="130" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G130" s="50"/>
+      <c r="G130" s="47"/>
     </row>
     <row r="131" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G131" s="50"/>
+      <c r="G131" s="47"/>
     </row>
     <row r="132" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G132" s="50"/>
+      <c r="G132" s="47"/>
     </row>
     <row r="133" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G133" s="50"/>
+      <c r="G133" s="47"/>
     </row>
     <row r="134" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G134" s="50"/>
+      <c r="G134" s="47"/>
     </row>
     <row r="135" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G135" s="50"/>
+      <c r="G135" s="47"/>
     </row>
     <row r="136" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G136" s="50"/>
+      <c r="G136" s="47"/>
     </row>
     <row r="137" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G137" s="50"/>
+      <c r="G137" s="47"/>
     </row>
     <row r="138" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G138" s="50"/>
+      <c r="G138" s="47"/>
     </row>
     <row r="139" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G139" s="50"/>
+      <c r="G139" s="47"/>
     </row>
     <row r="140" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G140" s="50"/>
+      <c r="G140" s="47"/>
     </row>
     <row r="141" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G141" s="50"/>
+      <c r="G141" s="47"/>
     </row>
     <row r="142" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G142" s="50"/>
+      <c r="G142" s="47"/>
     </row>
     <row r="143" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G143" s="50"/>
+      <c r="G143" s="47"/>
     </row>
     <row r="144" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G144" s="50"/>
+      <c r="G144" s="47"/>
     </row>
     <row r="145" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G145" s="50"/>
+      <c r="G145" s="47"/>
     </row>
     <row r="146" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G146" s="50"/>
+      <c r="G146" s="47"/>
     </row>
     <row r="147" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G147" s="50"/>
+      <c r="G147" s="47"/>
     </row>
     <row r="148" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G148" s="50"/>
+      <c r="G148" s="47"/>
     </row>
     <row r="149" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G149" s="50"/>
+      <c r="G149" s="47"/>
     </row>
     <row r="150" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G150" s="50"/>
+      <c r="G150" s="47"/>
     </row>
     <row r="151" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G151" s="50"/>
+      <c r="G151" s="47"/>
     </row>
     <row r="152" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G152" s="50"/>
+      <c r="G152" s="47"/>
     </row>
     <row r="153" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G153" s="50"/>
+      <c r="G153" s="47"/>
     </row>
     <row r="154" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G154" s="50"/>
+      <c r="G154" s="47"/>
     </row>
     <row r="155" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G155" s="50"/>
+      <c r="G155" s="47"/>
     </row>
     <row r="156" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G156" s="50"/>
+      <c r="G156" s="47"/>
     </row>
     <row r="157" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G157" s="50"/>
+      <c r="G157" s="47"/>
     </row>
     <row r="158" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G158" s="50"/>
+      <c r="G158" s="47"/>
     </row>
     <row r="159" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G159" s="50"/>
+      <c r="G159" s="47"/>
     </row>
     <row r="160" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G160" s="50"/>
+      <c r="G160" s="47"/>
     </row>
     <row r="161" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G161" s="50"/>
+      <c r="G161" s="47"/>
     </row>
     <row r="162" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G162" s="50"/>
+      <c r="G162" s="47"/>
     </row>
     <row r="163" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G163" s="50"/>
+      <c r="G163" s="47"/>
     </row>
     <row r="164" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G164" s="50"/>
+      <c r="G164" s="47"/>
     </row>
     <row r="165" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G165" s="50"/>
+      <c r="G165" s="47"/>
     </row>
     <row r="166" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G166" s="50"/>
+      <c r="G166" s="47"/>
     </row>
     <row r="167" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G167" s="50"/>
+      <c r="G167" s="47"/>
     </row>
     <row r="168" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G168" s="50"/>
+      <c r="G168" s="47"/>
     </row>
     <row r="169" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G169" s="50"/>
+      <c r="G169" s="47"/>
     </row>
     <row r="170" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G170" s="50"/>
+      <c r="G170" s="47"/>
     </row>
     <row r="171" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G171" s="50"/>
+      <c r="G171" s="47"/>
     </row>
     <row r="172" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G172" s="50"/>
+      <c r="G172" s="47"/>
     </row>
     <row r="173" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G173" s="50"/>
+      <c r="G173" s="47"/>
     </row>
     <row r="174" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G174" s="50"/>
+      <c r="G174" s="47"/>
     </row>
     <row r="175" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G175" s="50"/>
+      <c r="G175" s="47"/>
     </row>
     <row r="176" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G176" s="50"/>
+      <c r="G176" s="47"/>
     </row>
     <row r="177" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G177" s="50"/>
+      <c r="G177" s="47"/>
     </row>
     <row r="178" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G178" s="50"/>
+      <c r="G178" s="47"/>
     </row>
     <row r="179" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G179" s="50"/>
+      <c r="G179" s="47"/>
     </row>
     <row r="180" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G180" s="50"/>
+      <c r="G180" s="47"/>
     </row>
     <row r="181" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G181" s="50"/>
+      <c r="G181" s="47"/>
     </row>
     <row r="182" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G182" s="50"/>
+      <c r="G182" s="47"/>
     </row>
     <row r="183" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G183" s="50"/>
+      <c r="G183" s="47"/>
     </row>
     <row r="184" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G184" s="50"/>
+      <c r="G184" s="47"/>
     </row>
     <row r="185" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G185" s="50"/>
+      <c r="G185" s="47"/>
     </row>
     <row r="186" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G186" s="50"/>
+      <c r="G186" s="47"/>
     </row>
     <row r="187" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G187" s="50"/>
+      <c r="G187" s="47"/>
     </row>
     <row r="188" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G188" s="50"/>
+      <c r="G188" s="47"/>
     </row>
     <row r="189" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G189" s="50"/>
+      <c r="G189" s="47"/>
     </row>
     <row r="190" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G190" s="50"/>
+      <c r="G190" s="47"/>
     </row>
     <row r="191" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G191" s="50"/>
+      <c r="G191" s="47"/>
     </row>
     <row r="192" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G192" s="50"/>
+      <c r="G192" s="47"/>
     </row>
     <row r="193" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G193" s="50"/>
+      <c r="G193" s="47"/>
     </row>
     <row r="194" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G194" s="50"/>
+      <c r="G194" s="47"/>
     </row>
     <row r="195" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G195" s="50"/>
+      <c r="G195" s="47"/>
     </row>
     <row r="196" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G196" s="50"/>
+      <c r="G196" s="47"/>
     </row>
     <row r="197" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G197" s="50"/>
+      <c r="G197" s="47"/>
     </row>
     <row r="198" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G198" s="50"/>
+      <c r="G198" s="47"/>
     </row>
     <row r="199" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G199" s="50"/>
+      <c r="G199" s="47"/>
     </row>
     <row r="200" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G200" s="50"/>
+      <c r="G200" s="47"/>
     </row>
     <row r="201" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G201" s="50"/>
+      <c r="G201" s="47"/>
     </row>
     <row r="202" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G202" s="50"/>
+      <c r="G202" s="47"/>
     </row>
     <row r="203" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G203" s="50"/>
+      <c r="G203" s="47"/>
     </row>
     <row r="204" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G204" s="50"/>
+      <c r="G204" s="47"/>
     </row>
     <row r="205" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G205" s="50"/>
+      <c r="G205" s="47"/>
     </row>
     <row r="206" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G206" s="50"/>
+      <c r="G206" s="47"/>
     </row>
     <row r="207" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G207" s="50"/>
+      <c r="G207" s="47"/>
     </row>
     <row r="208" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G208" s="50"/>
+      <c r="G208" s="47"/>
     </row>
     <row r="209" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G209" s="50"/>
+      <c r="G209" s="47"/>
     </row>
     <row r="210" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G210" s="50"/>
+      <c r="G210" s="47"/>
     </row>
     <row r="211" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G211" s="50"/>
+      <c r="G211" s="47"/>
     </row>
     <row r="212" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G212" s="50"/>
+      <c r="G212" s="47"/>
     </row>
     <row r="213" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G213" s="50"/>
+      <c r="G213" s="47"/>
     </row>
     <row r="214" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G214" s="50"/>
+      <c r="G214" s="47"/>
     </row>
     <row r="215" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G215" s="50"/>
+      <c r="G215" s="47"/>
     </row>
     <row r="216" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G216" s="50"/>
+      <c r="G216" s="47"/>
     </row>
     <row r="217" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G217" s="50"/>
+      <c r="G217" s="47"/>
     </row>
     <row r="218" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G218" s="50"/>
+      <c r="G218" s="47"/>
     </row>
     <row r="219" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G219" s="50"/>
+      <c r="G219" s="47"/>
     </row>
     <row r="220" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G220" s="50"/>
+      <c r="G220" s="47"/>
     </row>
     <row r="221" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G221" s="50"/>
+      <c r="G221" s="47"/>
     </row>
     <row r="222" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G222" s="50"/>
+      <c r="G222" s="47"/>
     </row>
     <row r="223" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G223" s="50"/>
+      <c r="G223" s="47"/>
     </row>
     <row r="224" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G224" s="50"/>
+      <c r="G224" s="47"/>
     </row>
     <row r="225" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G225" s="50"/>
+      <c r="G225" s="47"/>
     </row>
     <row r="226" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G226" s="50"/>
+      <c r="G226" s="47"/>
     </row>
     <row r="227" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G227" s="50"/>
+      <c r="G227" s="47"/>
     </row>
     <row r="228" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G228" s="50"/>
+      <c r="G228" s="47"/>
     </row>
     <row r="229" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G229" s="50"/>
+      <c r="G229" s="47"/>
     </row>
     <row r="230" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G230" s="50"/>
+      <c r="G230" s="47"/>
     </row>
     <row r="231" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G231" s="50"/>
+      <c r="G231" s="47"/>
     </row>
     <row r="232" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G232" s="50"/>
+      <c r="G232" s="47"/>
     </row>
     <row r="233" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G233" s="50"/>
+      <c r="G233" s="47"/>
     </row>
     <row r="234" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G234" s="50"/>
+      <c r="G234" s="47"/>
     </row>
     <row r="235" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G235" s="50"/>
+      <c r="G235" s="47"/>
     </row>
     <row r="236" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G236" s="50"/>
+      <c r="G236" s="47"/>
     </row>
     <row r="237" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G237" s="50"/>
+      <c r="G237" s="47"/>
     </row>
     <row r="238" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G238" s="50"/>
+      <c r="G238" s="47"/>
     </row>
     <row r="239" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G239" s="50"/>
+      <c r="G239" s="47"/>
     </row>
     <row r="240" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G240" s="50"/>
+      <c r="G240" s="47"/>
     </row>
     <row r="241" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G241" s="50"/>
+      <c r="G241" s="47"/>
     </row>
     <row r="242" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G242" s="50"/>
+      <c r="G242" s="47"/>
     </row>
     <row r="243" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G243" s="50"/>
+      <c r="G243" s="47"/>
     </row>
     <row r="244" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G244" s="50"/>
+      <c r="G244" s="47"/>
     </row>
     <row r="245" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G245" s="50"/>
+      <c r="G245" s="47"/>
     </row>
     <row r="246" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G246" s="50"/>
+      <c r="G246" s="47"/>
     </row>
     <row r="247" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G247" s="50"/>
+      <c r="G247" s="47"/>
     </row>
     <row r="248" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G248" s="50"/>
+      <c r="G248" s="47"/>
     </row>
     <row r="249" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G249" s="50"/>
+      <c r="G249" s="47"/>
     </row>
     <row r="250" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G250" s="50"/>
+      <c r="G250" s="47"/>
     </row>
     <row r="251" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G251" s="50"/>
+      <c r="G251" s="47"/>
     </row>
     <row r="252" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G252" s="50"/>
+      <c r="G252" s="47"/>
     </row>
     <row r="253" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G253" s="50"/>
+      <c r="G253" s="47"/>
     </row>
     <row r="254" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G254" s="50"/>
+      <c r="G254" s="47"/>
     </row>
     <row r="255" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G255" s="50"/>
+      <c r="G255" s="47"/>
     </row>
     <row r="256" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G256" s="50"/>
+      <c r="G256" s="47"/>
     </row>
     <row r="257" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G257" s="50"/>
+      <c r="G257" s="47"/>
     </row>
     <row r="258" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G258" s="50"/>
+      <c r="G258" s="47"/>
     </row>
     <row r="259" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G259" s="50"/>
+      <c r="G259" s="47"/>
     </row>
     <row r="260" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G260" s="50"/>
+      <c r="G260" s="47"/>
     </row>
     <row r="261" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G261" s="50"/>
+      <c r="G261" s="47"/>
     </row>
     <row r="262" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G262" s="50"/>
+      <c r="G262" s="47"/>
     </row>
     <row r="263" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G263" s="50"/>
+      <c r="G263" s="47"/>
     </row>
     <row r="264" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G264" s="50"/>
+      <c r="G264" s="47"/>
     </row>
     <row r="265" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G265" s="50"/>
+      <c r="G265" s="47"/>
     </row>
     <row r="266" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G266" s="50"/>
+      <c r="G266" s="47"/>
     </row>
     <row r="267" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G267" s="50"/>
+      <c r="G267" s="47"/>
     </row>
     <row r="268" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G268" s="50"/>
+      <c r="G268" s="47"/>
     </row>
     <row r="269" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G269" s="50"/>
+      <c r="G269" s="47"/>
     </row>
     <row r="270" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G270" s="50"/>
+      <c r="G270" s="47"/>
     </row>
     <row r="271" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G271" s="50"/>
+      <c r="G271" s="47"/>
     </row>
     <row r="272" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G272" s="50"/>
+      <c r="G272" s="47"/>
     </row>
     <row r="273" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G273" s="50"/>
+      <c r="G273" s="47"/>
     </row>
     <row r="274" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G274" s="50"/>
+      <c r="G274" s="47"/>
     </row>
     <row r="275" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G275" s="50"/>
+      <c r="G275" s="47"/>
     </row>
     <row r="276" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G276" s="50"/>
+      <c r="G276" s="47"/>
     </row>
     <row r="277" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G277" s="50"/>
+      <c r="G277" s="47"/>
     </row>
     <row r="278" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G278" s="50"/>
+      <c r="G278" s="47"/>
     </row>
     <row r="279" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G279" s="50"/>
+      <c r="G279" s="47"/>
     </row>
     <row r="280" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G280" s="50"/>
+      <c r="G280" s="47"/>
     </row>
     <row r="281" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G281" s="50"/>
+      <c r="G281" s="47"/>
     </row>
     <row r="282" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G282" s="50"/>
+      <c r="G282" s="47"/>
     </row>
     <row r="283" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G283" s="50"/>
+      <c r="G283" s="47"/>
     </row>
     <row r="284" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G284" s="50"/>
+      <c r="G284" s="47"/>
     </row>
     <row r="285" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G285" s="50"/>
+      <c r="G285" s="47"/>
     </row>
     <row r="286" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G286" s="50"/>
+      <c r="G286" s="47"/>
     </row>
     <row r="287" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G287" s="50"/>
+      <c r="G287" s="47"/>
     </row>
     <row r="288" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G288" s="50"/>
+      <c r="G288" s="47"/>
     </row>
     <row r="289" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G289" s="50"/>
+      <c r="G289" s="47"/>
     </row>
     <row r="290" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G290" s="50"/>
+      <c r="G290" s="47"/>
     </row>
     <row r="291" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G291" s="50"/>
+      <c r="G291" s="47"/>
     </row>
     <row r="292" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G292" s="50"/>
+      <c r="G292" s="47"/>
     </row>
     <row r="293" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G293" s="50"/>
+      <c r="G293" s="47"/>
     </row>
     <row r="294" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G294" s="50"/>
+      <c r="G294" s="47"/>
     </row>
     <row r="295" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G295" s="50"/>
+      <c r="G295" s="47"/>
     </row>
     <row r="296" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G296" s="50"/>
+      <c r="G296" s="47"/>
     </row>
     <row r="297" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G297" s="50"/>
+      <c r="G297" s="47"/>
     </row>
     <row r="298" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G298" s="50"/>
+      <c r="G298" s="47"/>
     </row>
     <row r="299" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G299" s="50"/>
+      <c r="G299" s="47"/>
     </row>
     <row r="300" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G300" s="50"/>
+      <c r="G300" s="47"/>
     </row>
     <row r="301" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G301" s="50"/>
+      <c r="G301" s="47"/>
     </row>
     <row r="302" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G302" s="50"/>
+      <c r="G302" s="47"/>
     </row>
     <row r="303" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G303" s="50"/>
+      <c r="G303" s="47"/>
     </row>
     <row r="304" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G304" s="50"/>
+      <c r="G304" s="47"/>
     </row>
     <row r="305" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G305" s="50"/>
+      <c r="G305" s="47"/>
     </row>
     <row r="306" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G306" s="50"/>
+      <c r="G306" s="47"/>
     </row>
     <row r="307" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G307" s="50"/>
+      <c r="G307" s="47"/>
     </row>
     <row r="308" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G308" s="50"/>
+      <c r="G308" s="47"/>
     </row>
     <row r="309" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G309" s="50"/>
+      <c r="G309" s="47"/>
     </row>
     <row r="310" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G310" s="50"/>
+      <c r="G310" s="47"/>
     </row>
     <row r="311" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G311" s="50"/>
+      <c r="G311" s="47"/>
     </row>
     <row r="312" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G312" s="50"/>
+      <c r="G312" s="47"/>
     </row>
     <row r="313" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G313" s="50"/>
+      <c r="G313" s="47"/>
     </row>
     <row r="314" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G314" s="50"/>
+      <c r="G314" s="47"/>
     </row>
     <row r="315" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G315" s="50"/>
+      <c r="G315" s="47"/>
     </row>
     <row r="316" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G316" s="50"/>
+      <c r="G316" s="47"/>
     </row>
     <row r="317" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G317" s="50"/>
+      <c r="G317" s="47"/>
     </row>
     <row r="318" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G318" s="50"/>
+      <c r="G318" s="47"/>
     </row>
     <row r="319" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G319" s="50"/>
+      <c r="G319" s="47"/>
     </row>
     <row r="320" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G320" s="50"/>
+      <c r="G320" s="47"/>
     </row>
     <row r="321" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G321" s="50"/>
+      <c r="G321" s="47"/>
     </row>
     <row r="322" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G322" s="50"/>
+      <c r="G322" s="47"/>
     </row>
     <row r="323" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G323" s="50"/>
+      <c r="G323" s="47"/>
     </row>
     <row r="324" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G324" s="50"/>
+      <c r="G324" s="47"/>
     </row>
     <row r="325" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G325" s="50"/>
+      <c r="G325" s="47"/>
     </row>
     <row r="326" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G326" s="50"/>
+      <c r="G326" s="47"/>
     </row>
     <row r="327" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G327" s="50"/>
+      <c r="G327" s="47"/>
     </row>
     <row r="328" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G328" s="50"/>
+      <c r="G328" s="47"/>
     </row>
     <row r="329" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G329" s="50"/>
+      <c r="G329" s="47"/>
     </row>
     <row r="330" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G330" s="50"/>
+      <c r="G330" s="47"/>
     </row>
     <row r="331" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G331" s="50"/>
+      <c r="G331" s="47"/>
     </row>
     <row r="332" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G332" s="50"/>
+      <c r="G332" s="47"/>
     </row>
     <row r="333" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G333" s="50"/>
+      <c r="G333" s="47"/>
     </row>
     <row r="334" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G334" s="50"/>
+      <c r="G334" s="47"/>
     </row>
     <row r="335" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G335" s="50"/>
+      <c r="G335" s="47"/>
     </row>
     <row r="336" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G336" s="50"/>
+      <c r="G336" s="47"/>
     </row>
     <row r="337" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G337" s="50"/>
+      <c r="G337" s="47"/>
     </row>
     <row r="338" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G338" s="50"/>
+      <c r="G338" s="47"/>
     </row>
     <row r="339" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G339" s="50"/>
+      <c r="G339" s="47"/>
     </row>
     <row r="340" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G340" s="50"/>
+      <c r="G340" s="47"/>
     </row>
     <row r="341" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G341" s="50"/>
+      <c r="G341" s="47"/>
     </row>
     <row r="342" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G342" s="50"/>
+      <c r="G342" s="47"/>
     </row>
     <row r="343" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G343" s="50"/>
+      <c r="G343" s="47"/>
     </row>
     <row r="344" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G344" s="50"/>
+      <c r="G344" s="47"/>
     </row>
     <row r="345" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G345" s="50"/>
+      <c r="G345" s="47"/>
     </row>
     <row r="346" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G346" s="50"/>
+      <c r="G346" s="47"/>
     </row>
     <row r="347" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G347" s="50"/>
+      <c r="G347" s="47"/>
     </row>
     <row r="348" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G348" s="50"/>
+      <c r="G348" s="47"/>
     </row>
     <row r="349" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G349" s="50"/>
+      <c r="G349" s="47"/>
     </row>
     <row r="350" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G350" s="50"/>
+      <c r="G350" s="47"/>
     </row>
     <row r="351" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G351" s="50"/>
+      <c r="G351" s="47"/>
     </row>
     <row r="352" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G352" s="50"/>
+      <c r="G352" s="47"/>
     </row>
     <row r="353" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G353" s="50"/>
+      <c r="G353" s="47"/>
     </row>
     <row r="354" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G354" s="50"/>
+      <c r="G354" s="47"/>
     </row>
     <row r="355" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G355" s="50"/>
+      <c r="G355" s="47"/>
     </row>
     <row r="356" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G356" s="50"/>
+      <c r="G356" s="47"/>
     </row>
     <row r="357" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G357" s="50"/>
+      <c r="G357" s="47"/>
     </row>
     <row r="358" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G358" s="50"/>
+      <c r="G358" s="47"/>
     </row>
     <row r="359" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G359" s="50"/>
+      <c r="G359" s="47"/>
     </row>
     <row r="360" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G360" s="50"/>
+      <c r="G360" s="47"/>
     </row>
     <row r="361" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G361" s="50"/>
+      <c r="G361" s="47"/>
     </row>
     <row r="362" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G362" s="50"/>
+      <c r="G362" s="47"/>
     </row>
     <row r="363" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G363" s="50"/>
+      <c r="G363" s="47"/>
     </row>
     <row r="364" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G364" s="50"/>
+      <c r="G364" s="47"/>
     </row>
     <row r="365" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G365" s="50"/>
+      <c r="G365" s="47"/>
     </row>
     <row r="366" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G366" s="50"/>
+      <c r="G366" s="47"/>
     </row>
     <row r="367" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G367" s="50"/>
+      <c r="G367" s="47"/>
     </row>
     <row r="368" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G368" s="50"/>
+      <c r="G368" s="47"/>
     </row>
     <row r="369" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G369" s="50"/>
+      <c r="G369" s="47"/>
     </row>
     <row r="370" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G370" s="50"/>
+      <c r="G370" s="47"/>
     </row>
     <row r="371" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G371" s="50"/>
+      <c r="G371" s="47"/>
     </row>
     <row r="372" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G372" s="50"/>
+      <c r="G372" s="47"/>
     </row>
     <row r="373" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G373" s="50"/>
+      <c r="G373" s="47"/>
     </row>
     <row r="374" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G374" s="50"/>
+      <c r="G374" s="47"/>
     </row>
     <row r="375" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G375" s="50"/>
+      <c r="G375" s="47"/>
     </row>
     <row r="376" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G376" s="50"/>
+      <c r="G376" s="47"/>
     </row>
     <row r="377" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G377" s="50"/>
+      <c r="G377" s="47"/>
     </row>
     <row r="378" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G378" s="50"/>
+      <c r="G378" s="47"/>
     </row>
     <row r="379" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G379" s="50"/>
+      <c r="G379" s="47"/>
     </row>
     <row r="380" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G380" s="50"/>
+      <c r="G380" s="47"/>
     </row>
     <row r="381" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G381" s="50"/>
+      <c r="G381" s="47"/>
     </row>
     <row r="382" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G382" s="50"/>
+      <c r="G382" s="47"/>
     </row>
     <row r="383" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G383" s="50"/>
+      <c r="G383" s="47"/>
     </row>
     <row r="384" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G384" s="50"/>
+      <c r="G384" s="47"/>
     </row>
     <row r="385" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G385" s="50"/>
+      <c r="G385" s="47"/>
     </row>
     <row r="386" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G386" s="50"/>
+      <c r="G386" s="47"/>
     </row>
     <row r="387" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G387" s="50"/>
+      <c r="G387" s="47"/>
     </row>
     <row r="388" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G388" s="50"/>
+      <c r="G388" s="47"/>
     </row>
     <row r="389" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G389" s="50"/>
+      <c r="G389" s="47"/>
     </row>
     <row r="390" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G390" s="50"/>
+      <c r="G390" s="47"/>
     </row>
     <row r="391" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G391" s="50"/>
+      <c r="G391" s="47"/>
     </row>
     <row r="392" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G392" s="50"/>
+      <c r="G392" s="47"/>
     </row>
     <row r="393" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G393" s="50"/>
+      <c r="G393" s="47"/>
     </row>
     <row r="394" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G394" s="50"/>
+      <c r="G394" s="47"/>
     </row>
     <row r="395" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G395" s="50"/>
+      <c r="G395" s="47"/>
     </row>
     <row r="396" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G396" s="50"/>
+      <c r="G396" s="47"/>
     </row>
     <row r="397" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G397" s="50"/>
+      <c r="G397" s="47"/>
     </row>
     <row r="398" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G398" s="50"/>
+      <c r="G398" s="47"/>
     </row>
     <row r="399" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G399" s="50"/>
+      <c r="G399" s="47"/>
     </row>
     <row r="400" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G400" s="50"/>
+      <c r="G400" s="47"/>
     </row>
     <row r="401" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G401" s="50"/>
+      <c r="G401" s="47"/>
     </row>
     <row r="402" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G402" s="50"/>
+      <c r="G402" s="47"/>
     </row>
     <row r="403" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G403" s="50"/>
+      <c r="G403" s="47"/>
     </row>
     <row r="404" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G404" s="50"/>
+      <c r="G404" s="47"/>
     </row>
     <row r="405" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G405" s="50"/>
+      <c r="G405" s="47"/>
     </row>
     <row r="406" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G406" s="50"/>
+      <c r="G406" s="47"/>
     </row>
     <row r="407" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G407" s="50"/>
+      <c r="G407" s="47"/>
     </row>
     <row r="408" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G408" s="50"/>
+      <c r="G408" s="47"/>
     </row>
     <row r="409" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G409" s="50"/>
+      <c r="G409" s="47"/>
     </row>
     <row r="410" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G410" s="50"/>
+      <c r="G410" s="47"/>
     </row>
     <row r="411" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G411" s="50"/>
+      <c r="G411" s="47"/>
     </row>
     <row r="412" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G412" s="50"/>
+      <c r="G412" s="47"/>
     </row>
     <row r="413" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G413" s="50"/>
+      <c r="G413" s="47"/>
     </row>
     <row r="414" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G414" s="50"/>
+      <c r="G414" s="47"/>
     </row>
     <row r="415" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G415" s="50"/>
+      <c r="G415" s="47"/>
     </row>
     <row r="416" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G416" s="50"/>
+      <c r="G416" s="47"/>
     </row>
     <row r="417" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G417" s="50"/>
+      <c r="G417" s="47"/>
     </row>
     <row r="418" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G418" s="50"/>
+      <c r="G418" s="47"/>
     </row>
     <row r="419" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G419" s="50"/>
+      <c r="G419" s="47"/>
     </row>
     <row r="420" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G420" s="50"/>
+      <c r="G420" s="47"/>
     </row>
     <row r="421" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G421" s="50"/>
+      <c r="G421" s="47"/>
     </row>
     <row r="422" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G422" s="50"/>
+      <c r="G422" s="47"/>
     </row>
     <row r="423" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G423" s="50"/>
+      <c r="G423" s="47"/>
     </row>
     <row r="424" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G424" s="50"/>
+      <c r="G424" s="47"/>
     </row>
     <row r="425" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G425" s="50"/>
+      <c r="G425" s="47"/>
     </row>
     <row r="426" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G426" s="50"/>
+      <c r="G426" s="47"/>
     </row>
     <row r="427" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G427" s="50"/>
+      <c r="G427" s="47"/>
     </row>
     <row r="428" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G428" s="50"/>
+      <c r="G428" s="47"/>
     </row>
     <row r="429" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G429" s="50"/>
+      <c r="G429" s="47"/>
     </row>
     <row r="430" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G430" s="50"/>
+      <c r="G430" s="47"/>
     </row>
     <row r="431" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G431" s="50"/>
+      <c r="G431" s="47"/>
     </row>
     <row r="432" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G432" s="50"/>
+      <c r="G432" s="47"/>
     </row>
     <row r="433" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G433" s="50"/>
+      <c r="G433" s="47"/>
     </row>
     <row r="434" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G434" s="50"/>
+      <c r="G434" s="47"/>
     </row>
     <row r="435" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G435" s="50"/>
+      <c r="G435" s="47"/>
     </row>
     <row r="436" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G436" s="50"/>
+      <c r="G436" s="47"/>
     </row>
     <row r="437" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G437" s="50"/>
+      <c r="G437" s="47"/>
     </row>
     <row r="438" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G438" s="50"/>
+      <c r="G438" s="47"/>
     </row>
     <row r="439" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G439" s="50"/>
+      <c r="G439" s="47"/>
     </row>
     <row r="440" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G440" s="50"/>
+      <c r="G440" s="47"/>
     </row>
     <row r="441" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G441" s="50"/>
+      <c r="G441" s="47"/>
     </row>
     <row r="442" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G442" s="50"/>
+      <c r="G442" s="47"/>
     </row>
     <row r="443" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G443" s="50"/>
+      <c r="G443" s="47"/>
     </row>
     <row r="444" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G444" s="50"/>
+      <c r="G444" s="47"/>
     </row>
     <row r="445" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G445" s="50"/>
+      <c r="G445" s="47"/>
     </row>
     <row r="446" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G446" s="50"/>
+      <c r="G446" s="47"/>
     </row>
     <row r="447" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G447" s="50"/>
+      <c r="G447" s="47"/>
     </row>
     <row r="448" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G448" s="50"/>
+      <c r="G448" s="47"/>
     </row>
     <row r="449" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G449" s="50"/>
+      <c r="G449" s="47"/>
     </row>
     <row r="450" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G450" s="50"/>
+      <c r="G450" s="47"/>
     </row>
     <row r="451" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G451" s="50"/>
+      <c r="G451" s="47"/>
     </row>
     <row r="452" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G452" s="50"/>
+      <c r="G452" s="47"/>
     </row>
     <row r="453" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G453" s="50"/>
+      <c r="G453" s="47"/>
     </row>
     <row r="454" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G454" s="50"/>
+      <c r="G454" s="47"/>
     </row>
     <row r="455" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G455" s="50"/>
+      <c r="G455" s="47"/>
     </row>
     <row r="456" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G456" s="50"/>
+      <c r="G456" s="47"/>
     </row>
     <row r="457" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G457" s="50"/>
+      <c r="G457" s="47"/>
     </row>
     <row r="458" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G458" s="50"/>
+      <c r="G458" s="47"/>
     </row>
     <row r="459" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G459" s="50"/>
+      <c r="G459" s="47"/>
     </row>
     <row r="460" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G460" s="50"/>
+      <c r="G460" s="47"/>
     </row>
     <row r="461" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G461" s="50"/>
+      <c r="G461" s="47"/>
     </row>
     <row r="462" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G462" s="50"/>
+      <c r="G462" s="47"/>
     </row>
     <row r="463" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G463" s="50"/>
+      <c r="G463" s="47"/>
     </row>
     <row r="464" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G464" s="50"/>
+      <c r="G464" s="47"/>
     </row>
     <row r="465" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G465" s="50"/>
+      <c r="G465" s="47"/>
     </row>
     <row r="466" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G466" s="50"/>
+      <c r="G466" s="47"/>
     </row>
     <row r="467" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G467" s="50"/>
+      <c r="G467" s="47"/>
     </row>
     <row r="468" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G468" s="50"/>
+      <c r="G468" s="47"/>
     </row>
     <row r="469" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G469" s="50"/>
+      <c r="G469" s="47"/>
     </row>
     <row r="470" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G470" s="50"/>
+      <c r="G470" s="47"/>
     </row>
     <row r="471" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G471" s="50"/>
+      <c r="G471" s="47"/>
     </row>
     <row r="472" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G472" s="50"/>
+      <c r="G472" s="47"/>
     </row>
     <row r="473" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G473" s="50"/>
+      <c r="G473" s="47"/>
     </row>
     <row r="474" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G474" s="50"/>
+      <c r="G474" s="47"/>
     </row>
     <row r="475" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G475" s="50"/>
+      <c r="G475" s="47"/>
     </row>
     <row r="476" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G476" s="50"/>
+      <c r="G476" s="47"/>
     </row>
     <row r="477" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G477" s="50"/>
+      <c r="G477" s="47"/>
     </row>
     <row r="478" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G478" s="50"/>
+      <c r="G478" s="47"/>
     </row>
     <row r="479" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G479" s="50"/>
+      <c r="G479" s="47"/>
     </row>
     <row r="480" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G480" s="50"/>
+      <c r="G480" s="47"/>
     </row>
     <row r="481" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G481" s="50"/>
+      <c r="G481" s="47"/>
     </row>
     <row r="482" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G482" s="50"/>
+      <c r="G482" s="47"/>
     </row>
     <row r="483" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G483" s="50"/>
+      <c r="G483" s="47"/>
     </row>
     <row r="484" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G484" s="50"/>
+      <c r="G484" s="47"/>
     </row>
     <row r="485" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G485" s="50"/>
+      <c r="G485" s="47"/>
     </row>
     <row r="486" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G486" s="50"/>
+      <c r="G486" s="47"/>
     </row>
     <row r="487" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G487" s="50"/>
+      <c r="G487" s="47"/>
     </row>
     <row r="488" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G488" s="50"/>
+      <c r="G488" s="47"/>
     </row>
     <row r="489" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G489" s="50"/>
+      <c r="G489" s="47"/>
     </row>
     <row r="490" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G490" s="50"/>
+      <c r="G490" s="47"/>
     </row>
     <row r="491" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G491" s="50"/>
+      <c r="G491" s="47"/>
     </row>
     <row r="492" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G492" s="50"/>
+      <c r="G492" s="47"/>
     </row>
     <row r="493" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G493" s="50"/>
+      <c r="G493" s="47"/>
     </row>
     <row r="494" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G494" s="50"/>
+      <c r="G494" s="47"/>
     </row>
     <row r="495" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G495" s="50"/>
+      <c r="G495" s="47"/>
     </row>
     <row r="496" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G496" s="50"/>
+      <c r="G496" s="47"/>
     </row>
     <row r="497" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G497" s="50"/>
+      <c r="G497" s="47"/>
     </row>
     <row r="498" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G498" s="50"/>
+      <c r="G498" s="47"/>
     </row>
     <row r="499" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G499" s="50"/>
+      <c r="G499" s="47"/>
     </row>
     <row r="500" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G500" s="50"/>
+      <c r="G500" s="47"/>
     </row>
     <row r="501" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G501" s="50"/>
+      <c r="G501" s="47"/>
     </row>
     <row r="502" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G502" s="50"/>
+      <c r="G502" s="47"/>
     </row>
     <row r="503" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G503" s="50"/>
+      <c r="G503" s="47"/>
     </row>
     <row r="504" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G504" s="50"/>
+      <c r="G504" s="47"/>
     </row>
     <row r="505" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G505" s="50"/>
+      <c r="G505" s="47"/>
     </row>
     <row r="506" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G506" s="50"/>
+      <c r="G506" s="47"/>
     </row>
     <row r="507" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G507" s="50"/>
+      <c r="G507" s="47"/>
     </row>
     <row r="508" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G508" s="50"/>
+      <c r="G508" s="47"/>
     </row>
     <row r="509" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G509" s="50"/>
+      <c r="G509" s="47"/>
     </row>
     <row r="510" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G510" s="50"/>
+      <c r="G510" s="47"/>
     </row>
     <row r="511" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G511" s="50"/>
+      <c r="G511" s="47"/>
     </row>
     <row r="512" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G512" s="50"/>
+      <c r="G512" s="47"/>
     </row>
     <row r="513" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G513" s="50"/>
+      <c r="G513" s="47"/>
     </row>
     <row r="514" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G514" s="50"/>
+      <c r="G514" s="47"/>
     </row>
     <row r="515" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G515" s="50"/>
+      <c r="G515" s="47"/>
     </row>
     <row r="516" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G516" s="50"/>
+      <c r="G516" s="47"/>
     </row>
     <row r="517" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G517" s="50"/>
+      <c r="G517" s="47"/>
     </row>
     <row r="518" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G518" s="50"/>
+      <c r="G518" s="47"/>
     </row>
     <row r="519" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G519" s="50"/>
+      <c r="G519" s="47"/>
     </row>
     <row r="520" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G520" s="50"/>
+      <c r="G520" s="47"/>
     </row>
     <row r="521" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G521" s="50"/>
+      <c r="G521" s="47"/>
     </row>
     <row r="522" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G522" s="50"/>
+      <c r="G522" s="47"/>
     </row>
     <row r="523" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G523" s="50"/>
+      <c r="G523" s="47"/>
     </row>
     <row r="524" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G524" s="50"/>
+      <c r="G524" s="47"/>
     </row>
     <row r="525" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G525" s="50"/>
+      <c r="G525" s="47"/>
     </row>
     <row r="526" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G526" s="50"/>
+      <c r="G526" s="47"/>
     </row>
     <row r="527" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G527" s="50"/>
+      <c r="G527" s="47"/>
     </row>
     <row r="528" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G528" s="50"/>
+      <c r="G528" s="47"/>
     </row>
     <row r="529" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G529" s="50"/>
+      <c r="G529" s="47"/>
     </row>
     <row r="530" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G530" s="50"/>
+      <c r="G530" s="47"/>
     </row>
     <row r="531" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G531" s="50"/>
+      <c r="G531" s="47"/>
     </row>
     <row r="532" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G532" s="50"/>
+      <c r="G532" s="47"/>
     </row>
     <row r="533" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G533" s="50"/>
+      <c r="G533" s="47"/>
     </row>
     <row r="534" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G534" s="50"/>
+      <c r="G534" s="47"/>
     </row>
     <row r="535" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G535" s="50"/>
+      <c r="G535" s="47"/>
     </row>
     <row r="536" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G536" s="50"/>
+      <c r="G536" s="47"/>
     </row>
     <row r="537" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G537" s="50"/>
+      <c r="G537" s="47"/>
     </row>
     <row r="538" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G538" s="50"/>
+      <c r="G538" s="47"/>
     </row>
     <row r="539" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G539" s="50"/>
+      <c r="G539" s="47"/>
     </row>
     <row r="540" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G540" s="50"/>
+      <c r="G540" s="47"/>
     </row>
     <row r="541" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G541" s="50"/>
+      <c r="G541" s="47"/>
     </row>
     <row r="542" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G542" s="50"/>
+      <c r="G542" s="47"/>
     </row>
     <row r="543" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G543" s="50"/>
+      <c r="G543" s="47"/>
     </row>
     <row r="544" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G544" s="50"/>
+      <c r="G544" s="47"/>
     </row>
     <row r="545" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G545" s="50"/>
+      <c r="G545" s="47"/>
     </row>
     <row r="546" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G546" s="50"/>
+      <c r="G546" s="47"/>
     </row>
     <row r="547" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G547" s="50"/>
+      <c r="G547" s="47"/>
     </row>
     <row r="548" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G548" s="50"/>
+      <c r="G548" s="47"/>
     </row>
     <row r="549" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G549" s="50"/>
+      <c r="G549" s="47"/>
     </row>
     <row r="550" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G550" s="50"/>
+      <c r="G550" s="47"/>
     </row>
     <row r="551" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G551" s="50"/>
+      <c r="G551" s="47"/>
     </row>
     <row r="552" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G552" s="50"/>
+      <c r="G552" s="47"/>
     </row>
     <row r="553" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G553" s="50"/>
+      <c r="G553" s="47"/>
     </row>
     <row r="554" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G554" s="50"/>
+      <c r="G554" s="47"/>
     </row>
     <row r="555" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G555" s="50"/>
+      <c r="G555" s="47"/>
     </row>
     <row r="556" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G556" s="50"/>
+      <c r="G556" s="47"/>
     </row>
     <row r="557" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G557" s="50"/>
+      <c r="G557" s="47"/>
     </row>
     <row r="558" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G558" s="50"/>
+      <c r="G558" s="47"/>
     </row>
     <row r="559" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G559" s="50"/>
+      <c r="G559" s="47"/>
     </row>
     <row r="560" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G560" s="50"/>
+      <c r="G560" s="47"/>
     </row>
     <row r="561" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G561" s="50"/>
+      <c r="G561" s="47"/>
     </row>
     <row r="562" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G562" s="50"/>
+      <c r="G562" s="47"/>
     </row>
     <row r="563" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G563" s="50"/>
+      <c r="G563" s="47"/>
     </row>
     <row r="564" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G564" s="50"/>
+      <c r="G564" s="47"/>
     </row>
     <row r="565" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G565" s="50"/>
+      <c r="G565" s="47"/>
     </row>
     <row r="566" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G566" s="50"/>
+      <c r="G566" s="47"/>
     </row>
     <row r="567" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G567" s="50"/>
+      <c r="G567" s="47"/>
     </row>
     <row r="568" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G568" s="50"/>
+      <c r="G568" s="47"/>
     </row>
     <row r="569" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G569" s="50"/>
+      <c r="G569" s="47"/>
     </row>
     <row r="570" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G570" s="50"/>
+      <c r="G570" s="47"/>
     </row>
     <row r="571" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G571" s="50"/>
+      <c r="G571" s="47"/>
     </row>
     <row r="572" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G572" s="50"/>
+      <c r="G572" s="47"/>
     </row>
     <row r="573" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G573" s="50"/>
+      <c r="G573" s="47"/>
     </row>
     <row r="574" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G574" s="50"/>
+      <c r="G574" s="47"/>
     </row>
     <row r="575" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G575" s="50"/>
+      <c r="G575" s="47"/>
     </row>
     <row r="576" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G576" s="50"/>
+      <c r="G576" s="47"/>
     </row>
     <row r="577" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G577" s="50"/>
+      <c r="G577" s="47"/>
     </row>
     <row r="578" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G578" s="50"/>
+      <c r="G578" s="47"/>
     </row>
     <row r="579" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G579" s="50"/>
+      <c r="G579" s="47"/>
     </row>
     <row r="580" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G580" s="50"/>
+      <c r="G580" s="47"/>
     </row>
     <row r="581" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G581" s="50"/>
+      <c r="G581" s="47"/>
     </row>
     <row r="582" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G582" s="50"/>
+      <c r="G582" s="47"/>
     </row>
     <row r="583" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G583" s="50"/>
+      <c r="G583" s="47"/>
     </row>
     <row r="584" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G584" s="50"/>
+      <c r="G584" s="47"/>
     </row>
     <row r="585" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G585" s="50"/>
+      <c r="G585" s="47"/>
     </row>
     <row r="586" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G586" s="50"/>
+      <c r="G586" s="47"/>
     </row>
     <row r="587" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G587" s="50"/>
+      <c r="G587" s="47"/>
     </row>
     <row r="588" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G588" s="50"/>
+      <c r="G588" s="47"/>
     </row>
     <row r="589" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G589" s="50"/>
+      <c r="G589" s="47"/>
     </row>
     <row r="590" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G590" s="50"/>
+      <c r="G590" s="47"/>
     </row>
     <row r="591" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G591" s="50"/>
+      <c r="G591" s="47"/>
     </row>
     <row r="592" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G592" s="50"/>
+      <c r="G592" s="47"/>
     </row>
     <row r="593" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G593" s="50"/>
+      <c r="G593" s="47"/>
     </row>
     <row r="594" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G594" s="50"/>
+      <c r="G594" s="47"/>
     </row>
     <row r="595" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G595" s="50"/>
+      <c r="G595" s="47"/>
     </row>
     <row r="596" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G596" s="50"/>
+      <c r="G596" s="47"/>
     </row>
     <row r="597" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G597" s="50"/>
+      <c r="G597" s="47"/>
     </row>
     <row r="598" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G598" s="50"/>
+      <c r="G598" s="47"/>
     </row>
     <row r="599" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G599" s="50"/>
+      <c r="G599" s="47"/>
     </row>
     <row r="600" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G600" s="50"/>
+      <c r="G600" s="47"/>
     </row>
     <row r="601" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G601" s="50"/>
+      <c r="G601" s="47"/>
     </row>
     <row r="602" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G602" s="50"/>
+      <c r="G602" s="47"/>
     </row>
     <row r="603" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G603" s="50"/>
+      <c r="G603" s="47"/>
     </row>
     <row r="604" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G604" s="50"/>
+      <c r="G604" s="47"/>
     </row>
     <row r="605" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G605" s="50"/>
+      <c r="G605" s="47"/>
     </row>
     <row r="606" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G606" s="50"/>
+      <c r="G606" s="47"/>
     </row>
     <row r="607" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G607" s="50"/>
+      <c r="G607" s="47"/>
     </row>
     <row r="608" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G608" s="50"/>
+      <c r="G608" s="47"/>
     </row>
     <row r="609" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G609" s="50"/>
+      <c r="G609" s="47"/>
     </row>
     <row r="610" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G610" s="50"/>
+      <c r="G610" s="47"/>
     </row>
     <row r="611" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G611" s="50"/>
+      <c r="G611" s="47"/>
     </row>
     <row r="612" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G612" s="50"/>
+      <c r="G612" s="47"/>
     </row>
     <row r="613" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G613" s="50"/>
+      <c r="G613" s="47"/>
     </row>
     <row r="614" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G614" s="50"/>
+      <c r="G614" s="47"/>
     </row>
     <row r="615" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G615" s="50"/>
+      <c r="G615" s="47"/>
     </row>
     <row r="616" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G616" s="50"/>
+      <c r="G616" s="47"/>
     </row>
     <row r="617" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G617" s="50"/>
+      <c r="G617" s="47"/>
     </row>
     <row r="618" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G618" s="50"/>
+      <c r="G618" s="47"/>
     </row>
     <row r="619" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G619" s="50"/>
+      <c r="G619" s="47"/>
     </row>
     <row r="620" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G620" s="50"/>
+      <c r="G620" s="47"/>
     </row>
     <row r="621" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G621" s="50"/>
+      <c r="G621" s="47"/>
     </row>
     <row r="622" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G622" s="50"/>
+      <c r="G622" s="47"/>
     </row>
     <row r="623" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G623" s="50"/>
+      <c r="G623" s="47"/>
     </row>
     <row r="624" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G624" s="50"/>
+      <c r="G624" s="47"/>
     </row>
     <row r="625" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G625" s="50"/>
+      <c r="G625" s="47"/>
     </row>
     <row r="626" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G626" s="50"/>
+      <c r="G626" s="47"/>
     </row>
     <row r="627" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G627" s="50"/>
+      <c r="G627" s="47"/>
     </row>
     <row r="628" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G628" s="50"/>
+      <c r="G628" s="47"/>
     </row>
     <row r="629" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G629" s="50"/>
+      <c r="G629" s="47"/>
     </row>
     <row r="630" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G630" s="50"/>
+      <c r="G630" s="47"/>
     </row>
     <row r="631" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G631" s="50"/>
+      <c r="G631" s="47"/>
     </row>
     <row r="632" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G632" s="50"/>
+      <c r="G632" s="47"/>
     </row>
     <row r="633" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G633" s="50"/>
+      <c r="G633" s="47"/>
     </row>
     <row r="634" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G634" s="50"/>
+      <c r="G634" s="47"/>
     </row>
     <row r="635" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G635" s="50"/>
+      <c r="G635" s="47"/>
     </row>
     <row r="636" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G636" s="50"/>
+      <c r="G636" s="47"/>
     </row>
     <row r="637" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G637" s="50"/>
+      <c r="G637" s="47"/>
     </row>
     <row r="638" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G638" s="50"/>
+      <c r="G638" s="47"/>
     </row>
     <row r="639" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G639" s="50"/>
+      <c r="G639" s="47"/>
     </row>
     <row r="640" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G640" s="50"/>
+      <c r="G640" s="47"/>
     </row>
     <row r="641" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G641" s="50"/>
+      <c r="G641" s="47"/>
     </row>
     <row r="642" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G642" s="50"/>
+      <c r="G642" s="47"/>
     </row>
     <row r="643" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G643" s="50"/>
+      <c r="G643" s="47"/>
     </row>
     <row r="644" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G644" s="50"/>
+      <c r="G644" s="47"/>
     </row>
     <row r="645" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G645" s="50"/>
+      <c r="G645" s="47"/>
     </row>
     <row r="646" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G646" s="50"/>
+      <c r="G646" s="47"/>
     </row>
     <row r="647" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G647" s="50"/>
+      <c r="G647" s="47"/>
     </row>
     <row r="648" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G648" s="50"/>
+      <c r="G648" s="47"/>
     </row>
     <row r="649" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G649" s="50"/>
+      <c r="G649" s="47"/>
     </row>
     <row r="650" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G650" s="50"/>
+      <c r="G650" s="47"/>
     </row>
     <row r="651" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G651" s="50"/>
+      <c r="G651" s="47"/>
     </row>
     <row r="652" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G652" s="50"/>
+      <c r="G652" s="47"/>
     </row>
     <row r="653" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G653" s="50"/>
+      <c r="G653" s="47"/>
     </row>
     <row r="654" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G654" s="50"/>
+      <c r="G654" s="47"/>
     </row>
     <row r="655" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G655" s="50"/>
+      <c r="G655" s="47"/>
     </row>
     <row r="656" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G656" s="50"/>
+      <c r="G656" s="47"/>
     </row>
     <row r="657" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G657" s="50"/>
+      <c r="G657" s="47"/>
     </row>
     <row r="658" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G658" s="50"/>
+      <c r="G658" s="47"/>
     </row>
     <row r="659" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G659" s="50"/>
+      <c r="G659" s="47"/>
     </row>
     <row r="660" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G660" s="50"/>
+      <c r="G660" s="47"/>
     </row>
     <row r="661" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G661" s="50"/>
+      <c r="G661" s="47"/>
     </row>
     <row r="662" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G662" s="50"/>
+      <c r="G662" s="47"/>
     </row>
     <row r="663" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G663" s="50"/>
+      <c r="G663" s="47"/>
     </row>
     <row r="664" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G664" s="50"/>
+      <c r="G664" s="47"/>
     </row>
     <row r="665" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G665" s="50"/>
+      <c r="G665" s="47"/>
     </row>
     <row r="666" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G666" s="50"/>
+      <c r="G666" s="47"/>
     </row>
     <row r="667" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G667" s="50"/>
+      <c r="G667" s="47"/>
     </row>
     <row r="668" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G668" s="50"/>
+      <c r="G668" s="47"/>
     </row>
     <row r="669" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G669" s="50"/>
+      <c r="G669" s="47"/>
     </row>
     <row r="670" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G670" s="50"/>
+      <c r="G670" s="47"/>
     </row>
     <row r="671" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G671" s="50"/>
+      <c r="G671" s="47"/>
     </row>
     <row r="672" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G672" s="50"/>
+      <c r="G672" s="47"/>
     </row>
     <row r="673" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G673" s="50"/>
+      <c r="G673" s="47"/>
     </row>
     <row r="674" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G674" s="50"/>
+      <c r="G674" s="47"/>
     </row>
     <row r="675" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G675" s="50"/>
+      <c r="G675" s="47"/>
     </row>
     <row r="676" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G676" s="50"/>
+      <c r="G676" s="47"/>
     </row>
     <row r="677" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G677" s="50"/>
+      <c r="G677" s="47"/>
     </row>
     <row r="678" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G678" s="50"/>
+      <c r="G678" s="47"/>
     </row>
     <row r="679" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G679" s="50"/>
+      <c r="G679" s="47"/>
     </row>
     <row r="680" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G680" s="50"/>
+      <c r="G680" s="47"/>
     </row>
     <row r="681" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G681" s="50"/>
+      <c r="G681" s="47"/>
     </row>
     <row r="682" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G682" s="50"/>
+      <c r="G682" s="47"/>
     </row>
     <row r="683" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G683" s="50"/>
+      <c r="G683" s="47"/>
     </row>
     <row r="684" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G684" s="50"/>
+      <c r="G684" s="47"/>
     </row>
     <row r="685" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G685" s="50"/>
+      <c r="G685" s="47"/>
     </row>
     <row r="686" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G686" s="50"/>
+      <c r="G686" s="47"/>
     </row>
     <row r="687" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G687" s="50"/>
+      <c r="G687" s="47"/>
     </row>
     <row r="688" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G688" s="50"/>
+      <c r="G688" s="47"/>
     </row>
     <row r="689" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G689" s="50"/>
+      <c r="G689" s="47"/>
     </row>
     <row r="690" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G690" s="50"/>
+      <c r="G690" s="47"/>
     </row>
     <row r="691" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G691" s="50"/>
+      <c r="G691" s="47"/>
     </row>
     <row r="692" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G692" s="50"/>
+      <c r="G692" s="47"/>
     </row>
     <row r="693" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G693" s="50"/>
+      <c r="G693" s="47"/>
     </row>
     <row r="694" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G694" s="50"/>
+      <c r="G694" s="47"/>
     </row>
     <row r="695" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G695" s="50"/>
+      <c r="G695" s="47"/>
     </row>
     <row r="696" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G696" s="50"/>
+      <c r="G696" s="47"/>
     </row>
     <row r="697" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G697" s="50"/>
+      <c r="G697" s="47"/>
     </row>
     <row r="698" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G698" s="50"/>
+      <c r="G698" s="47"/>
     </row>
     <row r="699" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G699" s="50"/>
+      <c r="G699" s="47"/>
     </row>
     <row r="700" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G700" s="50"/>
+      <c r="G700" s="47"/>
     </row>
     <row r="701" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G701" s="50"/>
+      <c r="G701" s="47"/>
     </row>
     <row r="702" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G702" s="50"/>
+      <c r="G702" s="47"/>
     </row>
     <row r="703" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G703" s="50"/>
+      <c r="G703" s="47"/>
     </row>
     <row r="704" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G704" s="50"/>
+      <c r="G704" s="47"/>
     </row>
     <row r="705" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G705" s="50"/>
+      <c r="G705" s="47"/>
     </row>
     <row r="706" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G706" s="50"/>
+      <c r="G706" s="47"/>
     </row>
     <row r="707" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G707" s="50"/>
+      <c r="G707" s="47"/>
     </row>
     <row r="708" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G708" s="50"/>
+      <c r="G708" s="47"/>
     </row>
     <row r="709" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G709" s="50"/>
+      <c r="G709" s="47"/>
     </row>
     <row r="710" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G710" s="50"/>
+      <c r="G710" s="47"/>
     </row>
     <row r="711" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G711" s="50"/>
+      <c r="G711" s="47"/>
     </row>
     <row r="712" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G712" s="50"/>
+      <c r="G712" s="47"/>
     </row>
     <row r="713" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G713" s="50"/>
+      <c r="G713" s="47"/>
     </row>
     <row r="714" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G714" s="50"/>
+      <c r="G714" s="47"/>
     </row>
     <row r="715" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G715" s="50"/>
+      <c r="G715" s="47"/>
     </row>
     <row r="716" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G716" s="50"/>
+      <c r="G716" s="47"/>
     </row>
     <row r="717" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G717" s="50"/>
+      <c r="G717" s="47"/>
     </row>
     <row r="718" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G718" s="50"/>
+      <c r="G718" s="47"/>
     </row>
     <row r="719" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G719" s="50"/>
+      <c r="G719" s="47"/>
     </row>
     <row r="720" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G720" s="50"/>
+      <c r="G720" s="47"/>
     </row>
     <row r="721" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G721" s="50"/>
+      <c r="G721" s="47"/>
     </row>
     <row r="722" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G722" s="50"/>
+      <c r="G722" s="47"/>
     </row>
     <row r="723" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G723" s="50"/>
+      <c r="G723" s="47"/>
     </row>
     <row r="724" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G724" s="50"/>
+      <c r="G724" s="47"/>
     </row>
     <row r="725" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G725" s="50"/>
+      <c r="G725" s="47"/>
     </row>
     <row r="726" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G726" s="50"/>
+      <c r="G726" s="47"/>
     </row>
     <row r="727" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G727" s="50"/>
+      <c r="G727" s="47"/>
     </row>
     <row r="728" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G728" s="50"/>
+      <c r="G728" s="47"/>
     </row>
     <row r="729" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G729" s="50"/>
+      <c r="G729" s="47"/>
     </row>
     <row r="730" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G730" s="50"/>
+      <c r="G730" s="47"/>
     </row>
     <row r="731" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G731" s="50"/>
+      <c r="G731" s="47"/>
     </row>
     <row r="732" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G732" s="50"/>
+      <c r="G732" s="47"/>
     </row>
     <row r="733" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G733" s="50"/>
+      <c r="G733" s="47"/>
     </row>
     <row r="734" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G734" s="50"/>
+      <c r="G734" s="47"/>
     </row>
     <row r="735" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G735" s="50"/>
+      <c r="G735" s="47"/>
     </row>
     <row r="736" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G736" s="50"/>
+      <c r="G736" s="47"/>
     </row>
     <row r="737" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G737" s="50"/>
+      <c r="G737" s="47"/>
     </row>
     <row r="738" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G738" s="50"/>
+      <c r="G738" s="47"/>
     </row>
     <row r="739" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G739" s="50"/>
+      <c r="G739" s="47"/>
     </row>
     <row r="740" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G740" s="50"/>
+      <c r="G740" s="47"/>
     </row>
     <row r="741" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G741" s="50"/>
+      <c r="G741" s="47"/>
     </row>
     <row r="742" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G742" s="50"/>
+      <c r="G742" s="47"/>
     </row>
     <row r="743" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G743" s="50"/>
+      <c r="G743" s="47"/>
     </row>
     <row r="744" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G744" s="50"/>
+      <c r="G744" s="47"/>
     </row>
     <row r="745" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G745" s="50"/>
+      <c r="G745" s="47"/>
     </row>
     <row r="746" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G746" s="50"/>
+      <c r="G746" s="47"/>
     </row>
     <row r="747" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G747" s="50"/>
+      <c r="G747" s="47"/>
     </row>
     <row r="748" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G748" s="50"/>
+      <c r="G748" s="47"/>
     </row>
     <row r="749" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G749" s="50"/>
+      <c r="G749" s="47"/>
     </row>
     <row r="750" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G750" s="50"/>
+      <c r="G750" s="47"/>
     </row>
     <row r="751" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G751" s="50"/>
+      <c r="G751" s="47"/>
     </row>
     <row r="752" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G752" s="50"/>
+      <c r="G752" s="47"/>
     </row>
     <row r="753" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G753" s="50"/>
+      <c r="G753" s="47"/>
     </row>
     <row r="754" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G754" s="50"/>
+      <c r="G754" s="47"/>
     </row>
     <row r="755" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G755" s="50"/>
+      <c r="G755" s="47"/>
     </row>
     <row r="756" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G756" s="50"/>
+      <c r="G756" s="47"/>
     </row>
     <row r="757" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G757" s="50"/>
+      <c r="G757" s="47"/>
     </row>
     <row r="758" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G758" s="50"/>
+      <c r="G758" s="47"/>
     </row>
     <row r="759" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G759" s="50"/>
+      <c r="G759" s="47"/>
     </row>
     <row r="760" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G760" s="50"/>
+      <c r="G760" s="47"/>
     </row>
     <row r="761" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G761" s="50"/>
+      <c r="G761" s="47"/>
     </row>
     <row r="762" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G762" s="50"/>
+      <c r="G762" s="47"/>
     </row>
     <row r="763" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G763" s="50"/>
+      <c r="G763" s="47"/>
     </row>
     <row r="764" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G764" s="50"/>
+      <c r="G764" s="47"/>
     </row>
     <row r="765" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G765" s="50"/>
+      <c r="G765" s="47"/>
     </row>
     <row r="766" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G766" s="50"/>
+      <c r="G766" s="47"/>
     </row>
     <row r="767" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G767" s="50"/>
+      <c r="G767" s="47"/>
     </row>
     <row r="768" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G768" s="50"/>
+      <c r="G768" s="47"/>
     </row>
     <row r="769" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G769" s="50"/>
+      <c r="G769" s="47"/>
     </row>
     <row r="770" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G770" s="50"/>
+      <c r="G770" s="47"/>
     </row>
     <row r="771" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G771" s="50"/>
+      <c r="G771" s="47"/>
     </row>
     <row r="772" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G772" s="50"/>
+      <c r="G772" s="47"/>
     </row>
     <row r="773" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G773" s="50"/>
+      <c r="G773" s="47"/>
     </row>
     <row r="774" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G774" s="50"/>
+      <c r="G774" s="47"/>
     </row>
     <row r="775" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G775" s="50"/>
+      <c r="G775" s="47"/>
     </row>
     <row r="776" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G776" s="50"/>
+      <c r="G776" s="47"/>
     </row>
     <row r="777" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G777" s="50"/>
+      <c r="G777" s="47"/>
     </row>
     <row r="778" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G778" s="50"/>
+      <c r="G778" s="47"/>
     </row>
     <row r="779" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G779" s="50"/>
+      <c r="G779" s="47"/>
     </row>
     <row r="780" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G780" s="50"/>
+      <c r="G780" s="47"/>
     </row>
     <row r="781" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G781" s="50"/>
+      <c r="G781" s="47"/>
     </row>
     <row r="782" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G782" s="50"/>
+      <c r="G782" s="47"/>
     </row>
     <row r="783" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G783" s="50"/>
+      <c r="G783" s="47"/>
     </row>
     <row r="784" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G784" s="50"/>
+      <c r="G784" s="47"/>
     </row>
     <row r="785" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G785" s="50"/>
+      <c r="G785" s="47"/>
     </row>
     <row r="786" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G786" s="50"/>
+      <c r="G786" s="47"/>
     </row>
     <row r="787" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G787" s="50"/>
+      <c r="G787" s="47"/>
     </row>
     <row r="788" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G788" s="50"/>
+      <c r="G788" s="47"/>
     </row>
     <row r="789" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G789" s="50"/>
+      <c r="G789" s="47"/>
     </row>
     <row r="790" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G790" s="50"/>
+      <c r="G790" s="47"/>
     </row>
     <row r="791" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G791" s="50"/>
+      <c r="G791" s="47"/>
     </row>
     <row r="792" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G792" s="50"/>
+      <c r="G792" s="47"/>
     </row>
     <row r="793" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G793" s="50"/>
+      <c r="G793" s="47"/>
     </row>
     <row r="794" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G794" s="50"/>
+      <c r="G794" s="47"/>
     </row>
     <row r="795" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G795" s="50"/>
+      <c r="G795" s="47"/>
     </row>
     <row r="796" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G796" s="50"/>
+      <c r="G796" s="47"/>
     </row>
     <row r="797" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G797" s="50"/>
+      <c r="G797" s="47"/>
     </row>
     <row r="798" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G798" s="50"/>
+      <c r="G798" s="47"/>
     </row>
     <row r="799" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G799" s="50"/>
+      <c r="G799" s="47"/>
     </row>
     <row r="800" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G800" s="50"/>
+      <c r="G800" s="47"/>
     </row>
     <row r="801" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G801" s="50"/>
+      <c r="G801" s="47"/>
     </row>
     <row r="802" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G802" s="50"/>
+      <c r="G802" s="47"/>
     </row>
     <row r="803" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G803" s="50"/>
+      <c r="G803" s="47"/>
     </row>
     <row r="804" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G804" s="50"/>
+      <c r="G804" s="47"/>
     </row>
     <row r="805" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G805" s="50"/>
+      <c r="G805" s="47"/>
     </row>
     <row r="806" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G806" s="50"/>
+      <c r="G806" s="47"/>
     </row>
     <row r="807" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G807" s="50"/>
+      <c r="G807" s="47"/>
     </row>
     <row r="808" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G808" s="50"/>
+      <c r="G808" s="47"/>
     </row>
     <row r="809" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G809" s="50"/>
+      <c r="G809" s="47"/>
     </row>
     <row r="810" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G810" s="50"/>
+      <c r="G810" s="47"/>
     </row>
     <row r="811" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G811" s="50"/>
+      <c r="G811" s="47"/>
     </row>
     <row r="812" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G812" s="50"/>
+      <c r="G812" s="47"/>
     </row>
     <row r="813" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G813" s="50"/>
+      <c r="G813" s="47"/>
     </row>
     <row r="814" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G814" s="50"/>
+      <c r="G814" s="47"/>
     </row>
     <row r="815" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G815" s="50"/>
+      <c r="G815" s="47"/>
     </row>
     <row r="816" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G816" s="50"/>
+      <c r="G816" s="47"/>
     </row>
     <row r="817" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G817" s="50"/>
+      <c r="G817" s="47"/>
     </row>
     <row r="818" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G818" s="50"/>
+      <c r="G818" s="47"/>
     </row>
     <row r="819" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G819" s="50"/>
+      <c r="G819" s="47"/>
     </row>
     <row r="820" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G820" s="50"/>
+      <c r="G820" s="47"/>
     </row>
     <row r="821" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G821" s="50"/>
+      <c r="G821" s="47"/>
     </row>
     <row r="822" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G822" s="50"/>
+      <c r="G822" s="47"/>
     </row>
     <row r="823" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G823" s="50"/>
+      <c r="G823" s="47"/>
     </row>
     <row r="824" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G824" s="50"/>
+      <c r="G824" s="47"/>
     </row>
     <row r="825" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G825" s="50"/>
+      <c r="G825" s="47"/>
     </row>
     <row r="826" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G826" s="50"/>
+      <c r="G826" s="47"/>
     </row>
     <row r="827" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G827" s="50"/>
+      <c r="G827" s="47"/>
     </row>
     <row r="828" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G828" s="50"/>
+      <c r="G828" s="47"/>
     </row>
     <row r="829" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G829" s="50"/>
+      <c r="G829" s="47"/>
     </row>
     <row r="830" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G830" s="50"/>
+      <c r="G830" s="47"/>
     </row>
     <row r="831" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G831" s="50"/>
+      <c r="G831" s="47"/>
     </row>
     <row r="832" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G832" s="50"/>
+      <c r="G832" s="47"/>
     </row>
     <row r="833" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G833" s="50"/>
+      <c r="G833" s="47"/>
     </row>
     <row r="834" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G834" s="50"/>
+      <c r="G834" s="47"/>
     </row>
     <row r="835" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G835" s="50"/>
+      <c r="G835" s="47"/>
     </row>
     <row r="836" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G836" s="50"/>
+      <c r="G836" s="47"/>
     </row>
     <row r="837" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G837" s="50"/>
+      <c r="G837" s="47"/>
     </row>
     <row r="838" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G838" s="50"/>
+      <c r="G838" s="47"/>
     </row>
     <row r="839" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G839" s="50"/>
+      <c r="G839" s="47"/>
     </row>
     <row r="840" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G840" s="50"/>
+      <c r="G840" s="47"/>
     </row>
     <row r="841" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G841" s="50"/>
+      <c r="G841" s="47"/>
     </row>
     <row r="842" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G842" s="50"/>
+      <c r="G842" s="47"/>
     </row>
     <row r="843" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G843" s="50"/>
+      <c r="G843" s="47"/>
     </row>
     <row r="844" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G844" s="50"/>
+      <c r="G844" s="47"/>
     </row>
     <row r="845" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G845" s="50"/>
+      <c r="G845" s="47"/>
     </row>
     <row r="846" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G846" s="50"/>
+      <c r="G846" s="47"/>
     </row>
     <row r="847" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G847" s="50"/>
+      <c r="G847" s="47"/>
     </row>
     <row r="848" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G848" s="50"/>
+      <c r="G848" s="47"/>
     </row>
     <row r="849" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G849" s="50"/>
+      <c r="G849" s="47"/>
     </row>
     <row r="850" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G850" s="50"/>
+      <c r="G850" s="47"/>
     </row>
     <row r="851" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G851" s="50"/>
+      <c r="G851" s="47"/>
     </row>
     <row r="852" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G852" s="50"/>
+      <c r="G852" s="47"/>
     </row>
     <row r="853" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G853" s="50"/>
+      <c r="G853" s="47"/>
     </row>
     <row r="854" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G854" s="50"/>
+      <c r="G854" s="47"/>
     </row>
     <row r="855" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G855" s="50"/>
+      <c r="G855" s="47"/>
     </row>
     <row r="856" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G856" s="50"/>
+      <c r="G856" s="47"/>
     </row>
     <row r="857" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G857" s="50"/>
+      <c r="G857" s="47"/>
     </row>
     <row r="858" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G858" s="50"/>
+      <c r="G858" s="47"/>
     </row>
     <row r="859" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G859" s="50"/>
+      <c r="G859" s="47"/>
     </row>
     <row r="860" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G860" s="50"/>
+      <c r="G860" s="47"/>
     </row>
     <row r="861" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G861" s="50"/>
+      <c r="G861" s="47"/>
     </row>
     <row r="862" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G862" s="50"/>
+      <c r="G862" s="47"/>
     </row>
     <row r="863" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G863" s="50"/>
+      <c r="G863" s="47"/>
     </row>
     <row r="864" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G864" s="50"/>
+      <c r="G864" s="47"/>
     </row>
     <row r="865" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G865" s="50"/>
+      <c r="G865" s="47"/>
     </row>
     <row r="866" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G866" s="50"/>
+      <c r="G866" s="47"/>
     </row>
     <row r="867" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G867" s="50"/>
+      <c r="G867" s="47"/>
     </row>
     <row r="868" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G868" s="50"/>
+      <c r="G868" s="47"/>
     </row>
     <row r="869" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G869" s="50"/>
+      <c r="G869" s="47"/>
     </row>
     <row r="870" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G870" s="50"/>
+      <c r="G870" s="47"/>
     </row>
     <row r="871" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G871" s="50"/>
+      <c r="G871" s="47"/>
     </row>
     <row r="872" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G872" s="50"/>
+      <c r="G872" s="47"/>
     </row>
     <row r="873" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G873" s="50"/>
+      <c r="G873" s="47"/>
     </row>
     <row r="874" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G874" s="50"/>
+      <c r="G874" s="47"/>
     </row>
     <row r="875" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G875" s="50"/>
+      <c r="G875" s="47"/>
     </row>
     <row r="876" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G876" s="50"/>
+      <c r="G876" s="47"/>
     </row>
     <row r="877" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G877" s="50"/>
+      <c r="G877" s="47"/>
     </row>
     <row r="878" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G878" s="50"/>
+      <c r="G878" s="47"/>
     </row>
     <row r="879" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G879" s="50"/>
+      <c r="G879" s="47"/>
     </row>
     <row r="880" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G880" s="50"/>
+      <c r="G880" s="47"/>
     </row>
     <row r="881" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G881" s="50"/>
+      <c r="G881" s="47"/>
     </row>
     <row r="882" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G882" s="50"/>
+      <c r="G882" s="47"/>
     </row>
     <row r="883" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G883" s="50"/>
+      <c r="G883" s="47"/>
     </row>
     <row r="884" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G884" s="50"/>
+      <c r="G884" s="47"/>
     </row>
     <row r="885" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G885" s="50"/>
+      <c r="G885" s="47"/>
     </row>
     <row r="886" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G886" s="50"/>
+      <c r="G886" s="47"/>
     </row>
     <row r="887" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G887" s="50"/>
+      <c r="G887" s="47"/>
     </row>
     <row r="888" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G888" s="50"/>
+      <c r="G888" s="47"/>
     </row>
     <row r="889" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G889" s="50"/>
+      <c r="G889" s="47"/>
     </row>
     <row r="890" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G890" s="50"/>
+      <c r="G890" s="47"/>
     </row>
     <row r="891" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G891" s="50"/>
+      <c r="G891" s="47"/>
     </row>
     <row r="892" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G892" s="50"/>
+      <c r="G892" s="47"/>
     </row>
     <row r="893" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G893" s="50"/>
+      <c r="G893" s="47"/>
     </row>
     <row r="894" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G894" s="50"/>
+      <c r="G894" s="47"/>
     </row>
     <row r="895" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G895" s="50"/>
+      <c r="G895" s="47"/>
     </row>
     <row r="896" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G896" s="50"/>
+      <c r="G896" s="47"/>
     </row>
     <row r="897" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G897" s="50"/>
+      <c r="G897" s="47"/>
     </row>
     <row r="898" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G898" s="50"/>
+      <c r="G898" s="47"/>
     </row>
     <row r="899" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G899" s="50"/>
+      <c r="G899" s="47"/>
     </row>
     <row r="900" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G900" s="50"/>
+      <c r="G900" s="47"/>
     </row>
     <row r="901" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G901" s="50"/>
+      <c r="G901" s="47"/>
     </row>
     <row r="902" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G902" s="50"/>
+      <c r="G902" s="47"/>
     </row>
     <row r="903" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G903" s="50"/>
+      <c r="G903" s="47"/>
     </row>
     <row r="904" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G904" s="50"/>
+      <c r="G904" s="47"/>
     </row>
     <row r="905" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G905" s="50"/>
+      <c r="G905" s="47"/>
     </row>
     <row r="906" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G906" s="50"/>
+      <c r="G906" s="47"/>
     </row>
     <row r="907" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G907" s="50"/>
+      <c r="G907" s="47"/>
     </row>
     <row r="908" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G908" s="50"/>
+      <c r="G908" s="47"/>
     </row>
     <row r="909" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G909" s="50"/>
+      <c r="G909" s="47"/>
     </row>
     <row r="910" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G910" s="50"/>
+      <c r="G910" s="47"/>
     </row>
     <row r="911" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G911" s="50"/>
+      <c r="G911" s="47"/>
     </row>
     <row r="912" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G912" s="50"/>
+      <c r="G912" s="47"/>
     </row>
     <row r="913" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G913" s="50"/>
+      <c r="G913" s="47"/>
     </row>
     <row r="914" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G914" s="50"/>
+      <c r="G914" s="47"/>
     </row>
     <row r="915" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G915" s="50"/>
+      <c r="G915" s="47"/>
     </row>
     <row r="916" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G916" s="50"/>
+      <c r="G916" s="47"/>
     </row>
     <row r="917" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G917" s="50"/>
+      <c r="G917" s="47"/>
     </row>
     <row r="918" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G918" s="50"/>
+      <c r="G918" s="47"/>
     </row>
     <row r="919" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G919" s="50"/>
+      <c r="G919" s="47"/>
     </row>
     <row r="920" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G920" s="50"/>
+      <c r="G920" s="47"/>
     </row>
     <row r="921" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G921" s="50"/>
+      <c r="G921" s="47"/>
     </row>
     <row r="922" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G922" s="50"/>
+      <c r="G922" s="47"/>
     </row>
     <row r="923" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G923" s="50"/>
+      <c r="G923" s="47"/>
     </row>
     <row r="924" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G924" s="50"/>
+      <c r="G924" s="47"/>
     </row>
     <row r="925" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G925" s="50"/>
+      <c r="G925" s="47"/>
     </row>
     <row r="926" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G926" s="50"/>
+      <c r="G926" s="47"/>
     </row>
     <row r="927" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G927" s="50"/>
+      <c r="G927" s="47"/>
     </row>
     <row r="928" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G928" s="50"/>
+      <c r="G928" s="47"/>
     </row>
     <row r="929" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G929" s="50"/>
+      <c r="G929" s="47"/>
     </row>
     <row r="930" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G930" s="50"/>
+      <c r="G930" s="47"/>
     </row>
     <row r="931" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G931" s="50"/>
+      <c r="G931" s="47"/>
     </row>
     <row r="932" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G932" s="50"/>
+      <c r="G932" s="47"/>
     </row>
     <row r="933" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G933" s="50"/>
+      <c r="G933" s="47"/>
     </row>
     <row r="934" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G934" s="50"/>
+      <c r="G934" s="47"/>
     </row>
     <row r="935" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G935" s="50"/>
+      <c r="G935" s="47"/>
     </row>
     <row r="936" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G936" s="50"/>
+      <c r="G936" s="47"/>
     </row>
     <row r="937" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G937" s="50"/>
+      <c r="G937" s="47"/>
     </row>
     <row r="938" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G938" s="50"/>
+      <c r="G938" s="47"/>
     </row>
     <row r="939" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G939" s="50"/>
+      <c r="G939" s="47"/>
     </row>
     <row r="940" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G940" s="50"/>
+      <c r="G940" s="47"/>
     </row>
     <row r="941" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G941" s="50"/>
+      <c r="G941" s="47"/>
     </row>
     <row r="942" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G942" s="50"/>
+      <c r="G942" s="47"/>
     </row>
     <row r="943" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G943" s="50"/>
+      <c r="G943" s="47"/>
     </row>
     <row r="944" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G944" s="50"/>
+      <c r="G944" s="47"/>
     </row>
     <row r="945" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G945" s="50"/>
+      <c r="G945" s="47"/>
     </row>
     <row r="946" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G946" s="50"/>
+      <c r="G946" s="47"/>
     </row>
     <row r="947" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G947" s="50"/>
+      <c r="G947" s="47"/>
     </row>
     <row r="948" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G948" s="50"/>
+      <c r="G948" s="47"/>
     </row>
     <row r="949" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G949" s="50"/>
+      <c r="G949" s="47"/>
     </row>
     <row r="950" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G950" s="50"/>
+      <c r="G950" s="47"/>
     </row>
     <row r="951" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G951" s="50"/>
+      <c r="G951" s="47"/>
     </row>
     <row r="952" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G952" s="50"/>
+      <c r="G952" s="47"/>
     </row>
     <row r="953" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G953" s="50"/>
+      <c r="G953" s="47"/>
     </row>
     <row r="954" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G954" s="50"/>
+      <c r="G954" s="47"/>
     </row>
     <row r="955" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G955" s="50"/>
+      <c r="G955" s="47"/>
     </row>
     <row r="956" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G956" s="50"/>
+      <c r="G956" s="47"/>
     </row>
     <row r="957" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G957" s="50"/>
+      <c r="G957" s="47"/>
     </row>
     <row r="958" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G958" s="50"/>
+      <c r="G958" s="47"/>
     </row>
     <row r="959" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G959" s="50"/>
+      <c r="G959" s="47"/>
     </row>
     <row r="960" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G960" s="50"/>
+      <c r="G960" s="47"/>
     </row>
     <row r="961" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G961" s="50"/>
+      <c r="G961" s="47"/>
     </row>
     <row r="962" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G962" s="50"/>
+      <c r="G962" s="47"/>
     </row>
     <row r="963" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G963" s="50"/>
+      <c r="G963" s="47"/>
     </row>
     <row r="964" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G964" s="50"/>
+      <c r="G964" s="47"/>
     </row>
     <row r="965" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G965" s="50"/>
+      <c r="G965" s="47"/>
     </row>
     <row r="966" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G966" s="50"/>
+      <c r="G966" s="47"/>
     </row>
     <row r="967" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G967" s="50"/>
+      <c r="G967" s="47"/>
     </row>
     <row r="968" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G968" s="50"/>
+      <c r="G968" s="47"/>
     </row>
     <row r="969" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G969" s="50"/>
+      <c r="G969" s="47"/>
     </row>
     <row r="970" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G970" s="50"/>
+      <c r="G970" s="47"/>
     </row>
     <row r="971" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G971" s="50"/>
+      <c r="G971" s="47"/>
     </row>
     <row r="972" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G972" s="50"/>
+      <c r="G972" s="47"/>
     </row>
     <row r="973" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G973" s="50"/>
+      <c r="G973" s="47"/>
     </row>
     <row r="974" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G974" s="50"/>
+      <c r="G974" s="47"/>
     </row>
     <row r="975" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G975" s="50"/>
+      <c r="G975" s="47"/>
     </row>
     <row r="976" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G976" s="50"/>
+      <c r="G976" s="47"/>
     </row>
     <row r="977" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G977" s="50"/>
+      <c r="G977" s="47"/>
     </row>
     <row r="978" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G978" s="50"/>
+      <c r="G978" s="47"/>
     </row>
     <row r="979" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G979" s="50"/>
+      <c r="G979" s="47"/>
     </row>
     <row r="980" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G980" s="50"/>
+      <c r="G980" s="47"/>
     </row>
     <row r="981" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G981" s="50"/>
+      <c r="G981" s="47"/>
     </row>
     <row r="982" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G982" s="50"/>
+      <c r="G982" s="47"/>
     </row>
     <row r="983" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G983" s="50"/>
+      <c r="G983" s="47"/>
     </row>
     <row r="984" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G984" s="50"/>
+      <c r="G984" s="47"/>
     </row>
     <row r="985" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G985" s="50"/>
+      <c r="G985" s="47"/>
     </row>
     <row r="986" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G986" s="50"/>
+      <c r="G986" s="47"/>
     </row>
     <row r="987" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G987" s="50"/>
+      <c r="G987" s="47"/>
     </row>
     <row r="988" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G988" s="50"/>
+      <c r="G988" s="47"/>
     </row>
     <row r="989" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G989" s="50"/>
+      <c r="G989" s="47"/>
     </row>
     <row r="990" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G990" s="50"/>
+      <c r="G990" s="47"/>
     </row>
     <row r="991" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G991" s="50"/>
+      <c r="G991" s="47"/>
     </row>
     <row r="992" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G992" s="50"/>
+      <c r="G992" s="47"/>
     </row>
     <row r="993" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G993" s="50"/>
+      <c r="G993" s="47"/>
     </row>
     <row r="994" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G994" s="50"/>
+      <c r="G994" s="47"/>
     </row>
     <row r="995" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G995" s="50"/>
+      <c r="G995" s="47"/>
     </row>
     <row r="996" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G996" s="50"/>
+      <c r="G996" s="47"/>
     </row>
     <row r="997" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G997" s="50"/>
+      <c r="G997" s="47"/>
     </row>
     <row r="998" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G998" s="50"/>
+      <c r="G998" s="47"/>
     </row>
     <row r="999" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G999" s="50"/>
+      <c r="G999" s="47"/>
     </row>
     <row r="1000" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G1000" s="50"/>
+      <c r="G1000" s="47"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
test for adding flanking sequences to packages - added D1005 and D1006 as Registry parts to the fluorescent proteins package - flanked the CDS parts in the libraries and composites tab with them
</commit_message>
<xml_diff>
--- a/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
+++ b/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/Fluorescent Reporter Proteins/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Fluorescent Reporter Proteins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFAD970-0B5A-5E4C-A631-2A159C7C5277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CE8019-498A-D74F-AC45-48D79B87F67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35500" yWindow="-840" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7674" uniqueCount="7578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7692" uniqueCount="7583">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22763,6 +22763,21 @@
   </si>
   <si>
     <t>E0040, E1010, E0030, E0020, J97000, J97001, J97002, J97003, K592100, J06504, K864100, mKate2, GFPmut3, mScarlet, KY484012</t>
+  </si>
+  <si>
+    <t>D1005</t>
+  </si>
+  <si>
+    <t>D1006</t>
+  </si>
+  <si>
+    <t>L0 CDS 5' Flanking Region</t>
+  </si>
+  <si>
+    <t>L0 CDS 3' Flanking Region</t>
+  </si>
+  <si>
+    <t>Includes BsaI and fusion site</t>
   </si>
 </sst>
 </file>
@@ -23582,8 +23597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23863,7 +23878,7 @@
         <v>9</v>
       </c>
       <c r="J15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" t="b">
         <v>0</v>
@@ -23899,8 +23914,8 @@
       <c r="I16" t="s">
         <v>9</v>
       </c>
-      <c r="J16" t="b">
-        <v>1</v>
+      <c r="J16" s="33" t="b">
+        <v>0</v>
       </c>
       <c r="K16" t="b">
         <v>0</v>
@@ -23932,8 +23947,8 @@
       <c r="I17" t="s">
         <v>9</v>
       </c>
-      <c r="J17" t="b">
-        <v>1</v>
+      <c r="J17" s="33" t="b">
+        <v>0</v>
       </c>
       <c r="K17" t="b">
         <v>0</v>
@@ -23965,8 +23980,8 @@
       <c r="I18" t="s">
         <v>9</v>
       </c>
-      <c r="J18" t="b">
-        <v>1</v>
+      <c r="J18" s="33" t="b">
+        <v>0</v>
       </c>
       <c r="K18" t="b">
         <v>0</v>
@@ -23998,8 +24013,8 @@
       <c r="I19" t="s">
         <v>9</v>
       </c>
-      <c r="J19" t="b">
-        <v>1</v>
+      <c r="J19" s="33" t="b">
+        <v>0</v>
       </c>
       <c r="K19" t="b">
         <v>0</v>
@@ -24031,8 +24046,8 @@
       <c r="I20" t="s">
         <v>9</v>
       </c>
-      <c r="J20" t="b">
-        <v>1</v>
+      <c r="J20" s="33" t="b">
+        <v>0</v>
       </c>
       <c r="K20" t="b">
         <v>0</v>
@@ -24063,8 +24078,8 @@
       <c r="I21" t="s">
         <v>9</v>
       </c>
-      <c r="J21" t="b">
-        <v>1</v>
+      <c r="J21" s="33" t="b">
+        <v>0</v>
       </c>
       <c r="K21" t="b">
         <v>0</v>
@@ -24094,8 +24109,8 @@
       <c r="I22" t="s">
         <v>9</v>
       </c>
-      <c r="J22" t="b">
-        <v>1</v>
+      <c r="J22" s="33" t="b">
+        <v>0</v>
       </c>
       <c r="K22" t="b">
         <v>0</v>
@@ -24130,8 +24145,8 @@
       <c r="I23" t="s">
         <v>80</v>
       </c>
-      <c r="J23" t="b">
-        <v>1</v>
+      <c r="J23" s="33" t="b">
+        <v>0</v>
       </c>
       <c r="K23" t="b">
         <v>0</v>
@@ -24160,8 +24175,8 @@
       <c r="I24" t="s">
         <v>9</v>
       </c>
-      <c r="J24" t="b">
-        <v>1</v>
+      <c r="J24" s="33" t="b">
+        <v>0</v>
       </c>
       <c r="K24" t="b">
         <v>0</v>
@@ -24191,8 +24206,8 @@
       <c r="I25" t="s">
         <v>87</v>
       </c>
-      <c r="J25" t="b">
-        <v>1</v>
+      <c r="J25" s="33" t="b">
+        <v>0</v>
       </c>
       <c r="K25" t="b">
         <v>0</v>
@@ -24223,8 +24238,8 @@
       <c r="I26" t="s">
         <v>9</v>
       </c>
-      <c r="J26" t="b">
-        <v>1</v>
+      <c r="J26" s="33" t="b">
+        <v>0</v>
       </c>
       <c r="K26" t="b">
         <v>0</v>
@@ -24256,8 +24271,8 @@
       <c r="I27" t="s">
         <v>9</v>
       </c>
-      <c r="J27" t="b">
-        <v>1</v>
+      <c r="J27" s="33" t="b">
+        <v>0</v>
       </c>
       <c r="K27" t="b">
         <v>0</v>
@@ -24286,8 +24301,8 @@
       <c r="I28" t="s">
         <v>9</v>
       </c>
-      <c r="J28" t="b">
-        <v>1</v>
+      <c r="J28" s="33" t="b">
+        <v>0</v>
       </c>
       <c r="K28" t="b">
         <v>0</v>
@@ -24319,8 +24334,8 @@
       <c r="I29" t="s">
         <v>101</v>
       </c>
-      <c r="J29" t="b">
-        <v>1</v>
+      <c r="J29" s="33" t="b">
+        <v>0</v>
       </c>
       <c r="K29" t="b">
         <v>0</v>
@@ -24352,8 +24367,8 @@
       <c r="I30" t="s">
         <v>9</v>
       </c>
-      <c r="J30" t="b">
-        <v>1</v>
+      <c r="J30" s="33" t="b">
+        <v>0</v>
       </c>
       <c r="K30" t="b">
         <v>0</v>
@@ -24392,6 +24407,30 @@
       <c r="M31" s="16"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A32" s="33" t="s">
+        <v>7578</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>7582</v>
+      </c>
+      <c r="E32" s="33" t="s">
+        <v>7580</v>
+      </c>
+      <c r="F32" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" s="33" t="s">
+        <v>7578</v>
+      </c>
+      <c r="H32" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="I32" s="33" t="s">
+        <v>9</v>
+      </c>
       <c r="J32" t="b">
         <v>0</v>
       </c>
@@ -24403,6 +24442,30 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A33" s="33" t="s">
+        <v>7579</v>
+      </c>
+      <c r="B33" s="33" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>7582</v>
+      </c>
+      <c r="E33" s="33" t="s">
+        <v>7581</v>
+      </c>
+      <c r="F33" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="G33" s="33" t="s">
+        <v>7579</v>
+      </c>
+      <c r="H33" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="I33" s="33" t="s">
+        <v>9</v>
+      </c>
       <c r="J33" t="b">
         <v>0</v>
       </c>
@@ -25437,8 +25500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -25759,10 +25822,15 @@
       <c r="E14" t="s">
         <v>105</v>
       </c>
-      <c r="G14" s="37" t="s">
+      <c r="G14" s="33" t="s">
+        <v>7578</v>
+      </c>
+      <c r="H14" s="37" t="s">
         <v>7577</v>
       </c>
-      <c r="I14" s="25"/>
+      <c r="I14" s="25" t="s">
+        <v>7579</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="16" customHeight="1">
       <c r="D15" t="b">
@@ -25814,7 +25882,9 @@
   </sheetPr>
   <dimension ref="A1:Z2535"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A630" workbookViewId="0">
+      <selection activeCell="B482" sqref="B482"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
fixed: missed updating pSB1C3 to pSB1C5 to reflect removal of BioBrick prefix and suffix
</commit_message>
<xml_diff>
--- a/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
+++ b/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Fluorescent Reporter Proteins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CE8019-498A-D74F-AC45-48D79B87F67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A2FD14-1F83-184B-B6A5-A5DE6C642F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35500" yWindow="-840" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35500" yWindow="-840" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7692" uniqueCount="7583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7692" uniqueCount="7584">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22778,6 +22778,9 @@
   </si>
   <si>
     <t>Includes BsaI and fusion site</t>
+  </si>
+  <si>
+    <t>pSB1C5</t>
   </si>
 </sst>
 </file>
@@ -23597,8 +23600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24380,7 +24383,7 @@
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
       <c r="A31" t="s">
-        <v>105</v>
+        <v>7583</v>
       </c>
       <c r="B31" t="s">
         <v>106</v>
@@ -25500,8 +25503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -25820,7 +25823,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>105</v>
+        <v>7583</v>
       </c>
       <c r="G14" s="33" t="s">
         <v>7578</v>

</xml_diff>

<commit_message>
Check of GB files showed that the file showed that pSB1C3 was the backbone. Data source ID for pSB1C5, was set to pSB1C3...whoops! Fixed.
</commit_message>
<xml_diff>
--- a/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
+++ b/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Fluorescent Reporter Proteins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09162B9C-53A3-CF4E-A9F4-B99A18C79AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939F55EE-8A25-0E47-9E94-B2572B4D6916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37420" yWindow="-160" windowWidth="35940" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23298,15 +23298,15 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23764,7 +23764,7 @@
   <dimension ref="A1:M983"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23838,14 +23838,14 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="53" t="s">
         <v>7590</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="53"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="55"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -24673,7 +24673,7 @@
         <v>42</v>
       </c>
       <c r="G31" s="21" t="s">
-        <v>7501</v>
+        <v>7547</v>
       </c>
       <c r="H31" s="18"/>
       <c r="I31" s="18" t="s">
@@ -26368,7 +26368,7 @@
       <c r="X13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="51" t="s">
         <v>7593</v>
       </c>
       <c r="B14" s="22"/>
@@ -26379,13 +26379,13 @@
         <v>7547</v>
       </c>
       <c r="F14" s="18"/>
-      <c r="G14" s="54" t="s">
+      <c r="G14" s="51" t="s">
         <v>7548</v>
       </c>
       <c r="H14" s="43" t="s">
         <v>7594</v>
       </c>
-      <c r="I14" s="55" t="s">
+      <c r="I14" s="52" t="s">
         <v>7549</v>
       </c>
       <c r="J14" s="18"/>

</xml_diff>

<commit_message>
- converted pSB1C5 from iGEM Registry into Benchling for a .gb export - removed pSB1C5 from iGEM_raw_imports.fasta - removed Data Source for pSB1C5 in package.xlsx, hoping this correctly references the pSB1C5.gb file in the package directory (but may cause issues if there are issues with overwriting pSB1C5 from other files in the package).
</commit_message>
<xml_diff>
--- a/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
+++ b/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Fluorescent Reporter Proteins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939F55EE-8A25-0E47-9E94-B2572B4D6916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC19C5A-3738-3348-96C7-6D73DECFF391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37420" yWindow="-160" windowWidth="35940" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7703" uniqueCount="7595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7702" uniqueCount="7595">
   <si>
     <t>Collection Name</t>
   </si>
@@ -23763,8 +23763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24669,9 +24669,7 @@
       <c r="C31" s="18"/>
       <c r="D31" s="21"/>
       <c r="E31" s="18"/>
-      <c r="F31" s="18" t="s">
-        <v>42</v>
-      </c>
+      <c r="F31" s="18"/>
       <c r="G31" s="21" t="s">
         <v>7547</v>
       </c>
@@ -72256,7 +72254,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D11"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
- changed package xlsx to reflect local sequence files for data sources for in-directory gb files
</commit_message>
<xml_diff>
--- a/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
+++ b/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Fluorescent Reporter Proteins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC19C5A-3738-3348-96C7-6D73DECFF391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CC9483-BC1C-B740-83A4-9A0704A54BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37420" yWindow="-160" windowWidth="35940" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7702" uniqueCount="7595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7707" uniqueCount="7595">
   <si>
     <t>Collection Name</t>
   </si>
@@ -23764,7 +23764,7 @@
   <dimension ref="A1:M983"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24141,7 +24141,9 @@
       <c r="E16" s="18" t="s">
         <v>7558</v>
       </c>
-      <c r="F16" s="18"/>
+      <c r="F16" s="18" t="s">
+        <v>7521</v>
+      </c>
       <c r="G16" s="23">
         <v>26495</v>
       </c>
@@ -24357,7 +24359,9 @@
       <c r="E22" s="18" t="s">
         <v>7564</v>
       </c>
-      <c r="F22" s="18"/>
+      <c r="F22" s="18" t="s">
+        <v>7521</v>
+      </c>
       <c r="G22" s="18">
         <v>120957</v>
       </c>
@@ -24391,7 +24395,9 @@
       <c r="E23" s="18" t="s">
         <v>7565</v>
       </c>
-      <c r="F23" s="18"/>
+      <c r="F23" s="18" t="s">
+        <v>7521</v>
+      </c>
       <c r="G23" s="18" t="s">
         <v>7580</v>
       </c>
@@ -24461,7 +24467,9 @@
       <c r="E25" s="18" t="s">
         <v>7567</v>
       </c>
-      <c r="F25" s="18"/>
+      <c r="F25" s="18" t="s">
+        <v>7521</v>
+      </c>
       <c r="G25" s="21">
         <v>54827</v>
       </c>
@@ -24669,7 +24677,9 @@
       <c r="C31" s="18"/>
       <c r="D31" s="21"/>
       <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
+      <c r="F31" s="18" t="s">
+        <v>7521</v>
+      </c>
       <c r="G31" s="21" t="s">
         <v>7547</v>
       </c>

</xml_diff>

<commit_message>
- changed pSB1C5 role from plasmid to plasmid_vector
</commit_message>
<xml_diff>
--- a/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
+++ b/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Fluorescent Reporter Proteins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CC9483-BC1C-B740-83A4-9A0704A54BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30E294F-BD0D-FE49-BBC8-4B1D39119207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37420" yWindow="-160" windowWidth="35940" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23763,8 +23763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24672,7 +24672,7 @@
         <v>7547</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="21"/>

</xml_diff>

<commit_message>
mrfp1 Type IIS version wasn't being built, and R0011 had a missing seq error
</commit_message>
<xml_diff>
--- a/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
+++ b/Fluorescent Reporter Proteins/Fluorescent Reporter Proteins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Fluorescent Reporter Proteins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30E294F-BD0D-FE49-BBC8-4B1D39119207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1058A50-D6FF-804D-B822-91540E53D2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37420" yWindow="-160" windowWidth="35940" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36720" yWindow="2200" windowWidth="35940" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -22887,7 +22887,7 @@
     <t>Fluorescent Proteins in vector</t>
   </si>
   <si>
-    <t>E0040, E1010, E0030, E0020, J97000, J97001, J97002, J97003, K592100, J06504, K864100, mKate2, GFPmut3, mScarlet, KY484012</t>
+    <t>E0040, E1010, E0030, E0020, J97000, J97001, J97002, J97003, K592100, J06504, K864100, mKate2, GFPmut3, mScarlet, KY484012, mRFP1</t>
   </si>
 </sst>
 </file>
@@ -23763,8 +23763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24311,7 +24311,7 @@
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
       <c r="A21" s="18" t="s">
-        <v>7538</v>
+        <v>7579</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>47</v>
@@ -25882,8 +25882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>